<commit_message>
Add unique collections to spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B156E-AC98-3942-9F07-026AB61F2F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7807A6B-E1E4-7B43-9F04-67803A09C3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23720" yWindow="800" windowWidth="22840" windowHeight="13320" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23720" yWindow="800" windowWidth="22840" windowHeight="13320" activeTab="3" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="170">
-  <si>
-    <t>collection</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="172">
   <si>
     <t>uses_iiif</t>
   </si>
@@ -550,6 +547,15 @@
   </si>
   <si>
     <t>Augustus (27 v.-14 n. Chr.); Emerita; 25 v.Chr. - 23 v.Chr.; Quinar; RIC I² 1b</t>
+  </si>
+  <si>
+    <t>collection_name</t>
+  </si>
+  <si>
+    <t>first_example_coin</t>
+  </si>
+  <si>
+    <t>first_example_coin_uri</t>
   </si>
 </sst>
 </file>
@@ -636,10 +642,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:C56" totalsRowShown="0">
+  <autoFilter ref="A1:C56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name"/>
+    <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
+    <tableColumn id="3" xr3:uid="{20BC787A-CE5D-C845-ACD7-9B05986C804E}" name="first_example_coin_uri"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:E66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection"/>
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name"/>
     <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif"/>
     <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links"/>
     <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name"/>
@@ -982,13 +1000,644 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0256B6-CC9F-DA43-B2FC-ADA39BBB9055}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="91.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C56" r:id="rId1" xr:uid="{8BA57D8B-DD13-5443-A303-A3E91DB58EC6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -996,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,58 +1660,58 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1071,15 +1720,15 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1088,32 +1737,32 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1122,32 +1771,32 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -1156,15 +1805,15 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1173,32 +1822,32 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1207,168 +1856,168 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
         <v>48</v>
       </c>
-      <c r="B19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>52</v>
-      </c>
-      <c r="E20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -1377,66 +2026,66 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" t="b">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>59</v>
-      </c>
-      <c r="E23" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>64</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -1445,32 +2094,32 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
         <v>67</v>
       </c>
-      <c r="B27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>68</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -1479,15 +2128,15 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" t="s">
         <v>71</v>
-      </c>
-      <c r="E28" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -1496,32 +2145,32 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" t="s">
         <v>74</v>
-      </c>
-      <c r="E29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>77</v>
-      </c>
-      <c r="E30" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1530,49 +2179,49 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
         <v>79</v>
-      </c>
-      <c r="E31" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>82</v>
-      </c>
-      <c r="E32" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
         <v>84</v>
       </c>
-      <c r="B33" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>85</v>
-      </c>
-      <c r="E33" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -1581,15 +2230,15 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="s">
         <v>87</v>
-      </c>
-      <c r="E34" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -1598,100 +2247,100 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
         <v>89</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
         <v>91</v>
       </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>92</v>
-      </c>
-      <c r="E36" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
         <v>94</v>
       </c>
-      <c r="B37" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>95</v>
-      </c>
-      <c r="E37" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>98</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>101</v>
-      </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
         <v>102</v>
       </c>
-      <c r="B40" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>103</v>
-      </c>
-      <c r="E40" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -1700,49 +2349,49 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="s">
         <v>106</v>
-      </c>
-      <c r="E41" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
         <v>108</v>
       </c>
-      <c r="B42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>109</v>
-      </c>
-      <c r="E42" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
         <v>111</v>
       </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>112</v>
-      </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
@@ -1751,66 +2400,66 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
         <v>114</v>
       </c>
-      <c r="B45" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>115</v>
-      </c>
-      <c r="E45" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
         <v>117</v>
       </c>
-      <c r="B46" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>118</v>
-      </c>
-      <c r="E46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
         <v>120</v>
       </c>
-      <c r="B47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>121</v>
-      </c>
-      <c r="E47" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -1819,49 +2468,49 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" t="s">
         <v>124</v>
-      </c>
-      <c r="E48" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
         <v>126</v>
       </c>
-      <c r="B49" t="b">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>127</v>
-      </c>
-      <c r="E49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
         <v>129</v>
       </c>
-      <c r="B50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>130</v>
-      </c>
-      <c r="E50" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" t="b">
         <v>0</v>
@@ -1870,15 +2519,15 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -1887,15 +2536,15 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
         <v>134</v>
-      </c>
-      <c r="E52" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -1904,66 +2553,66 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
         <v>138</v>
       </c>
-      <c r="B54" t="b">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>139</v>
-      </c>
-      <c r="E54" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="b">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>142</v>
-      </c>
-      <c r="E55" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" t="s">
         <v>144</v>
-      </c>
-      <c r="B56" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B57" t="b">
         <v>0</v>
@@ -1972,83 +2621,83 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
         <v>147</v>
       </c>
-      <c r="B58" t="b">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>148</v>
-      </c>
       <c r="E58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
         <v>149</v>
       </c>
-      <c r="B59" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>150</v>
-      </c>
-      <c r="E59" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
         <v>152</v>
       </c>
-      <c r="B60" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>153</v>
-      </c>
-      <c r="E60" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
         <v>155</v>
       </c>
-      <c r="B61" t="b">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>156</v>
-      </c>
-      <c r="E61" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -2057,15 +2706,15 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" t="s">
         <v>159</v>
-      </c>
-      <c r="E62" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -2074,32 +2723,32 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" t="s">
         <v>162</v>
-      </c>
-      <c r="E63" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
         <v>164</v>
       </c>
-      <c r="B64" t="b">
-        <v>0</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -2108,15 +2757,15 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" t="s">
         <v>167</v>
-      </c>
-      <c r="E65" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -2125,10 +2774,10 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add examples fields to spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7807A6B-E1E4-7B43-9F04-67803A09C3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CCF2D-94DB-5F4E-8BF3-133985285E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23720" yWindow="800" windowWidth="22840" windowHeight="13320" activeTab="3" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23720" yWindow="760" windowWidth="22840" windowHeight="13320" activeTab="2" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="191">
+  <si>
+    <t>collection</t>
+  </si>
   <si>
     <t>uses_iiif</t>
   </si>
@@ -556,6 +559,60 @@
   </si>
   <si>
     <t>first_example_coin_uri</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t>findspot</t>
+  </si>
+  <si>
+    <t>Albrighton</t>
+  </si>
+  <si>
+    <t>hoard</t>
+  </si>
+  <si>
+    <t>Llíria Hoard</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>IMP-4734</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>first_example_appearance</t>
+  </si>
+  <si>
+    <t>first_example_uri</t>
+  </si>
+  <si>
+    <t>first_example_value</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>NUMERIC</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>max_length</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -609,7 +666,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -642,19 +702,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:C56" totalsRowShown="0">
-  <autoFilter ref="A1:C56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name"/>
-    <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
-    <tableColumn id="3" xr3:uid="{20BC787A-CE5D-C845-ACD7-9B05986C804E}" name="first_example_coin_uri"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}" name="Table3" displayName="Table3" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1AEF8EC5-25F4-B84B-A364-B64CEFC825DE}" name="field_name"/>
+    <tableColumn id="5" xr3:uid="{F44B81FB-8489-CE43-BDA4-9774E1114C75}" name="data_type"/>
+    <tableColumn id="2" xr3:uid="{6B57CCD3-20A3-EF44-B27A-3D5C9C628B9F}" name="first_example_appearance"/>
+    <tableColumn id="3" xr3:uid="{FE16FEB6-F7BC-3D44-B0AD-08BC0DA6CC10}" name="first_example_value"/>
+    <tableColumn id="4" xr3:uid="{83604E6F-7F23-124E-AF69-D270CC8BAA42}" name="first_example_uri"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:D57" totalsRowCount="1">
+  <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="0">
+      <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
+    <tableColumn id="3" xr3:uid="{20BC787A-CE5D-C845-ACD7-9B05986C804E}" name="first_example_coin_uri" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:E66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name"/>
@@ -988,651 +1065,1036 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE1820D-22EF-E748-B98F-E9ADAA6A4092}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1.66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0256B6-CC9F-DA43-B2FC-ADA39BBB9055}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="91.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
         <v>5</v>
+      </c>
+      <c r="B2">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
         <v>15</v>
+      </c>
+      <c r="B4">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
         <v>18</v>
       </c>
+      <c r="B5">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>32</v>
+      </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
         <v>26</v>
+      </c>
+      <c r="B7">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
         <v>29</v>
+      </c>
+      <c r="B8">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
         <v>32</v>
+      </c>
+      <c r="B9">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
         <v>35</v>
+      </c>
+      <c r="B10">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
         <v>40</v>
+      </c>
+      <c r="B12">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
         <v>43</v>
+      </c>
+      <c r="B13">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s">
         <v>46</v>
       </c>
+      <c r="B14">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>79</v>
+      </c>
       <c r="C14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
         <v>48</v>
+      </c>
+      <c r="B15">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
         <v>51</v>
+      </c>
+      <c r="B16">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s">
         <v>54</v>
+      </c>
+      <c r="B17">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
         <v>58</v>
+      </c>
+      <c r="B19">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
         <v>61</v>
       </c>
+      <c r="B20">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>18</v>
+      </c>
       <c r="C20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
         <v>63</v>
+      </c>
+      <c r="B21">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="B22">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
         <v>67</v>
+      </c>
+      <c r="B23">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" t="s">
         <v>70</v>
+      </c>
+      <c r="B24">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
         <v>73</v>
+      </c>
+      <c r="B25">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" t="s">
         <v>81</v>
+      </c>
+      <c r="B27">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="B28">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" t="s">
         <v>91</v>
+      </c>
+      <c r="B29">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" t="s">
         <v>94</v>
+      </c>
+      <c r="B30">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" t="s">
         <v>97</v>
+      </c>
+      <c r="B31">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" t="s">
         <v>100</v>
       </c>
+      <c r="B32">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>19</v>
+      </c>
       <c r="C32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" t="s">
         <v>102</v>
+      </c>
+      <c r="B33">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" t="s">
         <v>105</v>
+      </c>
+      <c r="B34">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" t="s">
         <v>108</v>
+      </c>
+      <c r="B35">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
         <v>110</v>
       </c>
-      <c r="B36" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" t="s">
-        <v>48</v>
+        <v>113</v>
+      </c>
+      <c r="B37">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" t="s">
         <v>114</v>
+      </c>
+      <c r="B38">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" t="s">
         <v>117</v>
+      </c>
+      <c r="B39">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" t="s">
         <v>120</v>
+      </c>
+      <c r="B40">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" t="s">
         <v>123</v>
+      </c>
+      <c r="B41">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" t="s">
         <v>126</v>
+      </c>
+      <c r="B42">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+      <c r="B43">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" t="s">
         <v>133</v>
+      </c>
+      <c r="B44">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" t="s">
         <v>136</v>
       </c>
+      <c r="B45">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>32</v>
+      </c>
       <c r="C45" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" t="s">
         <v>138</v>
+      </c>
+      <c r="B46">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" t="s">
         <v>141</v>
+      </c>
+      <c r="B47">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" t="s">
-        <v>35</v>
+        <v>144</v>
+      </c>
+      <c r="B48">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="D48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" t="s">
-        <v>48</v>
+        <v>146</v>
+      </c>
+      <c r="B49">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" t="s">
         <v>147</v>
       </c>
+      <c r="B50">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>47</v>
+      </c>
       <c r="C50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="D50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>148</v>
-      </c>
-      <c r="B51" t="s">
         <v>149</v>
+      </c>
+      <c r="B51">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" t="s">
         <v>152</v>
+      </c>
+      <c r="B52">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>154</v>
-      </c>
-      <c r="B53" t="s">
         <v>155</v>
+      </c>
+      <c r="B53">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>36</v>
       </c>
       <c r="C53" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>157</v>
-      </c>
-      <c r="B54" t="s">
         <v>158</v>
+      </c>
+      <c r="B54">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>160</v>
-      </c>
-      <c r="B55" t="s">
         <v>161</v>
+      </c>
+      <c r="B55">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>163</v>
-      </c>
-      <c r="B56" t="s">
-        <v>168</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>106</v>
+        <v>164</v>
+      </c>
+      <c r="B56">
+        <f>LEN(CollectionsTable[[#This Row],[collection_name]])</f>
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>169</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57">
+        <f>SUBTOTAL(104,CollectionsTable[max_length])</f>
+        <v>140</v>
+      </c>
+      <c r="D57">
+        <f>SUBTOTAL(103,CollectionsTable[first_example_coin_uri])</f>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C56" r:id="rId1" xr:uid="{8BA57D8B-DD13-5443-A303-A3E91DB58EC6}"/>
+    <hyperlink ref="D56" r:id="rId1" xr:uid="{8BA57D8B-DD13-5443-A303-A3E91DB58EC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1660,24 +2122,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1686,15 +2148,15 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -1703,15 +2165,15 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1720,15 +2182,15 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1737,15 +2199,15 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -1754,15 +2216,15 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1771,15 +2233,15 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -1788,15 +2250,15 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -1805,15 +2267,15 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1822,15 +2284,15 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -1839,15 +2301,15 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1856,15 +2318,15 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -1873,15 +2335,15 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -1890,32 +2352,32 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -1924,15 +2386,15 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
@@ -1941,15 +2403,15 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -1958,15 +2420,15 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -1975,15 +2437,15 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -1992,15 +2454,15 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -2009,15 +2471,15 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -2026,15 +2488,15 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -2043,15 +2505,15 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2060,15 +2522,15 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -2077,15 +2539,15 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -2094,15 +2556,15 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2111,15 +2573,15 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2128,15 +2590,15 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -2145,15 +2607,15 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2162,15 +2624,15 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -2179,15 +2641,15 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -2196,15 +2658,15 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2213,15 +2675,15 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -2230,15 +2692,15 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2247,15 +2709,15 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
@@ -2264,15 +2726,15 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
@@ -2281,15 +2743,15 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B38" t="b">
         <v>0</v>
@@ -2298,15 +2760,15 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B39" t="b">
         <v>0</v>
@@ -2315,15 +2777,15 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B40" t="b">
         <v>0</v>
@@ -2332,15 +2794,15 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E40" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -2349,15 +2811,15 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" t="b">
         <v>0</v>
@@ -2366,32 +2828,32 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" t="s">
         <v>110</v>
-      </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E43" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
@@ -2400,15 +2862,15 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B45" t="b">
         <v>0</v>
@@ -2417,15 +2879,15 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B46" t="b">
         <v>0</v>
@@ -2434,15 +2896,15 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B47" t="b">
         <v>0</v>
@@ -2451,15 +2913,15 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -2468,15 +2930,15 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B49" t="b">
         <v>0</v>
@@ -2485,15 +2947,15 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
@@ -2502,15 +2964,15 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B51" t="b">
         <v>0</v>
@@ -2519,15 +2981,15 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -2536,15 +2998,15 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -2553,15 +3015,15 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E53" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -2570,15 +3032,15 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B55" t="b">
         <v>0</v>
@@ -2587,15 +3049,15 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B56" t="b">
         <v>0</v>
@@ -2604,15 +3066,15 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B57" t="b">
         <v>0</v>
@@ -2621,15 +3083,15 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B58" t="b">
         <v>0</v>
@@ -2638,15 +3100,15 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E58" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
@@ -2655,15 +3117,15 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E59" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B60" t="b">
         <v>0</v>
@@ -2672,15 +3134,15 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
@@ -2689,15 +3151,15 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E61" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -2706,15 +3168,15 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E62" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -2723,15 +3185,15 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E63" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
@@ -2740,15 +3202,15 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -2757,15 +3219,15 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E65" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -2774,10 +3236,10 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review and define analysis section fields
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CCF2D-94DB-5F4E-8BF3-133985285E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDD1058-169B-8E40-B2CF-162FED0168D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23720" yWindow="760" windowWidth="22840" windowHeight="13320" activeTab="2" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23700" yWindow="1920" windowWidth="22840" windowHeight="13320" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Collections" sheetId="4" r:id="rId4"/>
     <sheet name="CollectionsAndIIIF" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="197">
   <si>
     <t>collection</t>
   </si>
@@ -613,6 +613,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>average_axis</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.1A</t>
+  </si>
+  <si>
+    <t>average_diameter</t>
+  </si>
+  <si>
+    <t>average_weight</t>
+  </si>
+  <si>
+    <t>example_field_value</t>
+  </si>
+  <si>
+    <t>example_field_uri</t>
   </si>
 </sst>
 </file>
@@ -657,19 +675,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -688,6 +702,9 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -702,25 +719,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}" name="Table3" displayName="Table3" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1AEF8EC5-25F4-B84B-A364-B64CEFC825DE}" name="field_name"/>
-    <tableColumn id="5" xr3:uid="{F44B81FB-8489-CE43-BDA4-9774E1114C75}" name="data_type"/>
-    <tableColumn id="2" xr3:uid="{6B57CCD3-20A3-EF44-B27A-3D5C9C628B9F}" name="first_example_appearance"/>
-    <tableColumn id="3" xr3:uid="{FE16FEB6-F7BC-3D44-B0AD-08BC0DA6CC10}" name="first_example_value"/>
-    <tableColumn id="4" xr3:uid="{83604E6F-7F23-124E-AF69-D270CC8BAA42}" name="first_example_uri"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B83FD7C4-BC5E-964C-B461-DC52D3B69E7A}" name="Table4" displayName="Table4" ref="A1:D5" totalsRowCount="1">
+  <autoFilter ref="A1:D4" xr:uid="{B83FD7C4-BC5E-964C-B461-DC52D3B69E7A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6FCD53BA-46E5-D742-88DF-173639671333}" name="field_name" totalsRowLabel="Total"/>
+    <tableColumn id="4" xr3:uid="{83C51FA8-C31D-934E-B6E2-27DD1E38B08E}" name="data_type"/>
+    <tableColumn id="2" xr3:uid="{8EB8692E-7B6F-A44D-845C-2A7700B65138}" name="example_field_value"/>
+    <tableColumn id="3" xr3:uid="{F9107982-C933-EB4E-AD79-59D542CAA952}" name="example_field_uri" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}" name="Table3" displayName="Table3" ref="A1:E9" totalsRowCount="1">
+  <autoFilter ref="A1:E8" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1AEF8EC5-25F4-B84B-A364-B64CEFC825DE}" name="field_name" totalsRowLabel="Total"/>
+    <tableColumn id="5" xr3:uid="{F44B81FB-8489-CE43-BDA4-9774E1114C75}" name="data_type"/>
+    <tableColumn id="2" xr3:uid="{6B57CCD3-20A3-EF44-B27A-3D5C9C628B9F}" name="first_example_appearance"/>
+    <tableColumn id="3" xr3:uid="{FE16FEB6-F7BC-3D44-B0AD-08BC0DA6CC10}" name="first_example_value"/>
+    <tableColumn id="4" xr3:uid="{83604E6F-7F23-124E-AF69-D270CC8BAA42}" name="first_example_uri" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:D57" totalsRowCount="1">
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="1">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -730,8 +760,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="1">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:E66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name"/>
@@ -1041,13 +1071,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDD5D45-1DCC-E44B-8D59-8507F8236A7D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3">
+        <v>13.66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4">
+        <v>1.61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5">
+        <f>SUBTOTAL(103,Table4[example_field_uri])</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1065,9 +1172,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE1820D-22EF-E748-B98F-E9ADAA6A4092}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1215,6 +1322,15 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9">
+        <f>SUBTOTAL(103,Table3[first_example_uri])</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1228,7 +1344,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2121,19 +2237,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Determine which collections use IIIF windows
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDD1058-169B-8E40-B2CF-162FED0168D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBCBF9C-240D-E44E-8542-98736217BFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23700" yWindow="1920" windowWidth="22840" windowHeight="13320" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23700" yWindow="1900" windowWidth="22840" windowHeight="13320" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ExamplesFields" sheetId="3" r:id="rId3"/>
     <sheet name="Collections" sheetId="4" r:id="rId4"/>
     <sheet name="CollectionsAndIIIF" sheetId="5" r:id="rId5"/>
+    <sheet name="CollectionsAndIIIFSummary" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="200">
   <si>
     <t>collection</t>
   </si>
@@ -631,13 +632,22 @@
   </si>
   <si>
     <t>example_field_uri</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>collection_count</t>
+  </si>
+  <si>
+    <t>Collections That Use Both: 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -649,6 +659,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -675,15 +693,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -750,7 +775,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="3">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -761,14 +786,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:E66" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:G67" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="A1:G66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif"/>
     <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="0">
+      <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1073,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDD5D45-1DCC-E44B-8D59-8507F8236A7D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2221,10 +2252,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2232,11 +2263,12 @@
     <col min="1" max="1" width="69.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="48.1640625" customWidth="1"/>
-    <col min="5" max="5" width="56.5" customWidth="1"/>
+    <col min="4" max="5" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="48.1640625" customWidth="1"/>
+    <col min="7" max="7" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -2247,13 +2279,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2263,14 +2301,22 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2280,14 +2326,22 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E3" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2297,14 +2351,22 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2314,14 +2376,22 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E5" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2331,14 +2401,22 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2348,14 +2426,22 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2365,14 +2451,22 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E8" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2382,14 +2476,22 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E9" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2399,14 +2501,22 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E10" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2416,14 +2526,22 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2433,14 +2551,22 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2450,14 +2576,22 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E13" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2467,14 +2601,22 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E14" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F14" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2484,14 +2626,22 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2501,14 +2651,22 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2518,14 +2676,22 @@
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2535,14 +2701,22 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2552,14 +2726,22 @@
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E19" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F19" t="s">
         <v>49</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2569,14 +2751,22 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F20" t="s">
         <v>52</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2586,14 +2776,22 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E21" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F21" t="s">
         <v>55</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -2603,14 +2801,22 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E22" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F22" t="s">
         <v>49</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2620,14 +2826,22 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E23" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F23" t="s">
         <v>59</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2637,14 +2851,22 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E24" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F24" t="s">
         <v>62</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2654,14 +2876,22 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E25" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F25" t="s">
         <v>64</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2671,14 +2901,22 @@
       <c r="C26">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E26" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F26" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2688,14 +2926,22 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E27" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F27" t="s">
         <v>68</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2705,14 +2951,22 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E28" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F28" t="s">
         <v>71</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -2722,14 +2976,22 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E29" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F29" t="s">
         <v>74</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2739,14 +3001,22 @@
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="E30" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F30" t="s">
         <v>77</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2756,14 +3026,22 @@
       <c r="C31">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="E31" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F31" t="s">
         <v>79</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -2773,14 +3051,22 @@
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E32" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F32" t="s">
         <v>82</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2790,14 +3076,22 @@
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E33" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F33" t="s">
         <v>85</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -2807,14 +3101,22 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E34" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F34" t="s">
         <v>87</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2824,14 +3126,22 @@
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -2841,14 +3151,22 @@
       <c r="C36">
         <v>2</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E36" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F36" t="s">
         <v>92</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -2858,14 +3176,22 @@
       <c r="C37">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E37" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F37" t="s">
         <v>95</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2875,14 +3201,22 @@
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E38" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F38" t="s">
         <v>98</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2892,14 +3226,22 @@
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E39" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F39" t="s">
         <v>101</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -2909,14 +3251,22 @@
       <c r="C40">
         <v>2</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E40" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F40" t="s">
         <v>103</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -2926,14 +3276,22 @@
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E41" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F41" t="s">
         <v>106</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2943,14 +3301,22 @@
       <c r="C42">
         <v>2</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E42" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F42" t="s">
         <v>109</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -2960,14 +3326,22 @@
       <c r="C43">
         <v>2</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E43" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F43" t="s">
         <v>112</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -2977,14 +3351,22 @@
       <c r="C44">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E44" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F44" t="s">
         <v>49</v>
       </c>
-      <c r="E44" t="s">
+      <c r="G44" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -2994,14 +3376,22 @@
       <c r="C45">
         <v>2</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E45" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F45" t="s">
         <v>115</v>
       </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -3011,14 +3401,22 @@
       <c r="C46">
         <v>2</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E46" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F46" t="s">
         <v>118</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3028,14 +3426,22 @@
       <c r="C47">
         <v>2</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E47" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F47" t="s">
         <v>121</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -3045,14 +3451,22 @@
       <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E48" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F48" t="s">
         <v>124</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3062,14 +3476,22 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E49" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F49" t="s">
         <v>127</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -3079,14 +3501,22 @@
       <c r="C50">
         <v>0</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="E50" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F50" t="s">
         <v>130</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -3096,14 +3526,22 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="E51" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F51" t="s">
         <v>132</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -3113,14 +3551,22 @@
       <c r="C52">
         <v>2</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E52" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F52" t="s">
         <v>134</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -3130,14 +3576,22 @@
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E53" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F53" t="s">
         <v>137</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3147,14 +3601,22 @@
       <c r="C54">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E54" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F54" t="s">
         <v>139</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3164,14 +3626,22 @@
       <c r="C55">
         <v>2</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E55" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F55" t="s">
         <v>142</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -3181,14 +3651,22 @@
       <c r="C56">
         <v>2</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E56" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F56" t="s">
         <v>36</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>146</v>
       </c>
@@ -3198,14 +3676,22 @@
       <c r="C57">
         <v>2</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E57" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F57" t="s">
         <v>49</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3215,14 +3701,22 @@
       <c r="C58">
         <v>2</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E58" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F58" t="s">
         <v>148</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -3232,14 +3726,22 @@
       <c r="C59">
         <v>2</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E59" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F59" t="s">
         <v>150</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -3249,14 +3751,22 @@
       <c r="C60">
         <v>2</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E60" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F60" t="s">
         <v>153</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -3266,14 +3776,22 @@
       <c r="C61">
         <v>2</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E61" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F61" t="s">
         <v>156</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>158</v>
       </c>
@@ -3283,14 +3801,22 @@
       <c r="C62">
         <v>2</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E62" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F62" t="s">
         <v>159</v>
       </c>
-      <c r="E62" t="s">
+      <c r="G62" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>161</v>
       </c>
@@ -3300,14 +3826,22 @@
       <c r="C63">
         <v>2</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="E63" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F63" t="s">
         <v>162</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -3317,14 +3851,22 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E64" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>hide</v>
+      </c>
+      <c r="F64" t="s">
         <v>165</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>164</v>
       </c>
@@ -3334,14 +3876,22 @@
       <c r="C65">
         <v>1</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E65" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F65" t="s">
         <v>167</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>164</v>
       </c>
@@ -3351,20 +3901,328 @@
       <c r="C66">
         <v>2</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66">
+        <f>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</f>
+        <v>3</v>
+      </c>
+      <c r="E66" t="str">
+        <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
+        <v>do not hide</v>
+      </c>
+      <c r="F66" t="s">
         <v>169</v>
       </c>
-      <c r="E66" t="s">
+      <c r="G66" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>190</v>
+      </c>
+      <c r="G67">
+        <f>SUBTOTAL(103,CollectionsAndIIIFTable[example_page_link])</f>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E64" r:id="rId1" xr:uid="{DA67D385-1BD1-1B49-AC38-DC1F0097C7EC}"/>
+    <hyperlink ref="G64" r:id="rId1" xr:uid="{DA67D385-1BD1-1B49-AC38-DC1F0097C7EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE74E1F-321C-FE4E-8C79-1D622E514933}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="81.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="str">
+        <f>_xlfn.CONCAT("Collections That Do Not Use IIIF: ",COUNTA(A2:A47))</f>
+        <v>Collections That Do Not Use IIIF: 43</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>_xlfn.CONCAT("Collections That Use IIIF: ",COUNTA(C2:C47))</f>
+        <v>Collections That Use IIIF: 13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Start reviewing IIIF-to-link conversion for collections
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBCBF9C-240D-E44E-8542-98736217BFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457C5C57-4FE4-0840-8D83-B050E2BB0B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23700" yWindow="1900" windowWidth="22840" windowHeight="13320" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="214">
   <si>
     <t>collection</t>
   </si>
@@ -641,6 +641,48 @@
   </si>
   <si>
     <t>Collections That Use Both: 1</t>
+  </si>
+  <si>
+    <t>link_to_image</t>
+  </si>
+  <si>
+    <t>https://numismatics.org/collectionimages/19501999/1978/1978.106.67.obv.noscale.jpg</t>
+  </si>
+  <si>
+    <t>link_from_scraping</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>https://numismatics.org/collectionimages/19001949/1944/1944.100.39301.obv.width175.jpg</t>
+  </si>
+  <si>
+    <t>https://numismatics.org/collectionimages/19001949/1944/1944.100.39301.obv.noscale.jpg</t>
+  </si>
+  <si>
+    <t>Extract "src" element from child "img" tag in "a" tag, then change "width175" to "noscale". "title" element of "a" tag contains "Obverse" or "Reverse" to tell which side it is.</t>
+  </si>
+  <si>
+    <t>https://numismatics.org/collectionimages/19501999/1978/1978.106.67.obv.width175.jpg</t>
+  </si>
+  <si>
+    <t>https://gallica.bnf.fr/ark:/12148/btv1b10443621k/f1.highres</t>
+  </si>
+  <si>
+    <t>https://gallica.bnf.fr/ark:/12148/btv1b10443621k</t>
+  </si>
+  <si>
+    <t>Extract "id" element from "a" tag, then add "f1.highres" to the end to get obverse and "f2.highres" to get reverse. "title" element of "a" tag contains obverse/reverse text, which can be searched.</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_10/11_11/f9f4285c_b306_4a84_88f0_a3c100bc730f/mid_00636137_001.jpg</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_10/11_11/f9f4285c_b306_4a84_88f0_a3c100bc730f/small_00636137_001.jpg</t>
+  </si>
+  <si>
+    <t>Extract "src" element from child "img" tag in "a" tag, then change "small" to "mid". Unable to tell if single side or both sides in image.</t>
   </si>
 </sst>
 </file>
@@ -693,10 +735,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,9 +838,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:G67" totalsRowCount="1" headerRowDxfId="2">
-  <autoFilter ref="A1:G66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif"/>
     <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links"/>
@@ -800,6 +858,9 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name"/>
     <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2252,23 +2313,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="69.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="5" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="48.1640625" customWidth="1"/>
-    <col min="7" max="7" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -2290,8 +2357,17 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2316,7 +2392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2341,14 +2417,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
       <c r="D4">
@@ -2359,21 +2435,30 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5">
@@ -2384,14 +2469,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2416,14 +2510,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7">
@@ -2434,14 +2528,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2466,7 +2569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2491,14 +2594,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
         <v>1</v>
       </c>
       <c r="D10">
@@ -2509,14 +2612,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2541,14 +2653,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
         <v>2</v>
       </c>
       <c r="D12">
@@ -2559,14 +2671,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2591,7 +2706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2616,7 +2731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2641,7 +2756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2691,7 +2806,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2716,7 +2831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2741,7 +2856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2766,7 +2881,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2791,7 +2906,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -2816,7 +2931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2841,7 +2956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2866,7 +2981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2891,7 +3006,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2916,7 +3031,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2941,7 +3056,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2966,14 +3081,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
         <v>1</v>
       </c>
       <c r="D29">
@@ -2984,14 +3099,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3016,14 +3134,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
         <v>2</v>
       </c>
       <c r="D31">
@@ -3034,14 +3152,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -3066,7 +3187,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -3091,7 +3212,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -3116,7 +3237,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -3141,7 +3262,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -3166,7 +3287,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3191,7 +3312,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -3216,7 +3337,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -3241,7 +3362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3266,14 +3387,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B41" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5">
         <v>2</v>
       </c>
       <c r="D41">
@@ -3284,14 +3405,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3316,7 +3440,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -3341,7 +3465,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3366,7 +3490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -3391,7 +3515,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -3416,7 +3540,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3441,14 +3565,14 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B48" t="b">
-        <v>1</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="5">
         <v>2</v>
       </c>
       <c r="D48">
@@ -3459,14 +3583,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3491,7 +3618,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -3516,7 +3643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -3541,14 +3668,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B52" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52">
+      <c r="B52" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
         <v>2</v>
       </c>
       <c r="D52">
@@ -3559,21 +3686,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B53" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53">
+      <c r="B53" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5">
         <v>2</v>
       </c>
       <c r="D53">
@@ -3584,14 +3714,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3616,7 +3749,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3641,7 +3774,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -3666,7 +3799,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>146</v>
       </c>
@@ -3691,7 +3824,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3716,7 +3849,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -3741,7 +3874,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -3766,7 +3899,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -3791,14 +3924,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B62" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62">
+      <c r="B62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C62" s="5">
         <v>2</v>
       </c>
       <c r="D62">
@@ -3809,21 +3942,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B63" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63">
+      <c r="B63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C63" s="5">
         <v>2</v>
       </c>
       <c r="D63">
@@ -3834,14 +3970,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -3866,14 +4005,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B65" t="b">
-        <v>1</v>
-      </c>
-      <c r="C65">
+      <c r="B65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C65" s="5">
         <v>1</v>
       </c>
       <c r="D65">
@@ -3884,21 +4023,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B66" t="b">
-        <v>1</v>
-      </c>
-      <c r="C66">
+      <c r="B66" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C66" s="5">
         <v>2</v>
       </c>
       <c r="D66">
@@ -3909,20 +4051,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>190</v>
       </c>
       <c r="G67">
         <f>SUBTOTAL(103,CollectionsAndIIIFTable[example_page_link])</f>
-        <v>65</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue collection-IIIF conversion review
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457C5C57-4FE4-0840-8D83-B050E2BB0B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA88C5E8-49E7-DC4A-A96F-F1A16659B59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="238">
   <si>
     <t>collection</t>
   </si>
@@ -683,6 +683,78 @@
   </si>
   <si>
     <t>Extract "src" element from child "img" tag in "a" tag, then change "small" to "mid". Unable to tell if single side or both sides in image.</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-1966_kenom_389059/files/images/record_DE-1966_kenom_389059_vs.jpg/full/!400,400/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-1966_kenom_389059/record_DE-1966_kenom_389059_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https:</t>
+  </si>
+  <si>
+    <t>www.kenom.de</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>record_DE-1966_kenom_389059</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>record_DE-1966_kenom_389059_vs.jpg</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>!400,400</t>
+  </si>
+  <si>
+    <t>default.jpg</t>
+  </si>
+  <si>
+    <t>iiif</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>120,</t>
+  </si>
+  <si>
+    <t>image link</t>
+  </si>
+  <si>
+    <t>iiif link</t>
+  </si>
+  <si>
+    <t>1. convert "iiif/image" to "api/v1/records"</t>
+  </si>
+  <si>
+    <t>2. Find "record_DE…" substring</t>
+  </si>
+  <si>
+    <t>3. Change "record_DE…" substring to "record_DE…/files/images/"</t>
+  </si>
+  <si>
+    <t>4. Replace "120," to "!600,600"</t>
+  </si>
+  <si>
+    <t>Try breaking into list and working by index?</t>
   </si>
 </sst>
 </file>
@@ -714,20 +786,37 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -739,7 +828,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -748,6 +836,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2313,13 +2404,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2332,10 +2423,11 @@
     <col min="6" max="6" width="30.6640625" customWidth="1"/>
     <col min="7" max="7" width="23.1640625" customWidth="1"/>
     <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -2357,17 +2449,17 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2392,7 +2484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2417,14 +2509,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4">
@@ -2435,30 +2527,30 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
         <v>2</v>
       </c>
       <c r="D5">
@@ -2469,23 +2561,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2510,14 +2602,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
         <v>2</v>
       </c>
       <c r="D7">
@@ -2528,23 +2620,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2569,7 +2661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2594,14 +2686,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10">
@@ -2612,23 +2704,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2653,14 +2745,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12">
@@ -2671,17 +2763,63 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="L12" t="s">
+        <v>231</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="N12" t="s">
+        <v>217</v>
+      </c>
+      <c r="O12" t="s">
+        <v>218</v>
+      </c>
+      <c r="P12" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>220</v>
+      </c>
+      <c r="R12" t="s">
+        <v>221</v>
+      </c>
+      <c r="S12" t="s">
+        <v>222</v>
+      </c>
+      <c r="T12" t="s">
+        <v>223</v>
+      </c>
+      <c r="U12" t="s">
+        <v>224</v>
+      </c>
+      <c r="V12" t="s">
+        <v>225</v>
+      </c>
+      <c r="W12" t="s">
+        <v>226</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2706,7 +2844,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2731,7 +2869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2756,7 +2894,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2781,7 +2919,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2806,7 +2944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2831,7 +2969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2856,7 +2994,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2881,7 +3019,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2906,7 +3044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -2931,7 +3069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2956,7 +3094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2981,7 +3119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -3006,7 +3144,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3031,7 +3169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3056,7 +3194,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3081,14 +3219,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
         <v>1</v>
       </c>
       <c r="D29">
@@ -3099,17 +3237,50 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="L29" t="s">
+        <v>232</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="N29" t="s">
+        <v>217</v>
+      </c>
+      <c r="O29" t="s">
+        <v>228</v>
+      </c>
+      <c r="P29" t="s">
+        <v>229</v>
+      </c>
+      <c r="R29" t="s">
+        <v>221</v>
+      </c>
+      <c r="U29" t="s">
+        <v>224</v>
+      </c>
+      <c r="V29" t="s">
+        <v>225</v>
+      </c>
+      <c r="W29" t="s">
+        <v>230</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3134,14 +3305,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5">
+      <c r="B31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
         <v>2</v>
       </c>
       <c r="D31">
@@ -3152,17 +3323,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -3187,7 +3358,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -3212,7 +3383,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -3237,7 +3408,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -3262,7 +3433,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -3287,7 +3458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3312,7 +3483,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -3337,7 +3508,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -3362,7 +3533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3387,14 +3558,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="B41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
         <v>2</v>
       </c>
       <c r="D41">
@@ -3405,17 +3576,20 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="3"/>
+      <c r="P41" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3440,7 +3614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -3465,7 +3639,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3490,7 +3664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -3515,7 +3689,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -3540,7 +3714,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3565,14 +3739,14 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="B48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4">
         <v>2</v>
       </c>
       <c r="D48">
@@ -3583,17 +3757,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3618,7 +3792,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -3643,7 +3817,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -3668,14 +3842,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B52" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52" s="5">
+      <c r="B52" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4">
         <v>2</v>
       </c>
       <c r="D52">
@@ -3686,24 +3860,31 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G52" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="3"/>
+      <c r="L52" t="s">
+        <v>233</v>
+      </c>
+      <c r="P52" t="str">
+        <f>SUBSTITUTE(P41, "iiif/image","api/v1/records",1)</f>
+        <v>https://www.kenom.de/api/v1/records/record_DE-1966_kenom_389059/record_DE-1966_kenom_389059_vs.jpg/full/120,/0/default.jpg</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B53" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53" s="5">
+      <c r="B53" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4">
         <v>2</v>
       </c>
       <c r="D53">
@@ -3714,17 +3895,20 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="G53" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="3"/>
+      <c r="L53" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3749,7 +3933,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3774,7 +3958,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -3799,7 +3983,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>146</v>
       </c>
@@ -3824,7 +4008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3849,7 +4033,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -3874,7 +4058,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -3899,7 +4083,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -3924,14 +4108,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" s="5">
+      <c r="B62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C62" s="4">
         <v>2</v>
       </c>
       <c r="D62">
@@ -3942,24 +4126,27 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G62" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="3"/>
+      <c r="L62" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63" s="5">
+      <c r="B63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4">
         <v>2</v>
       </c>
       <c r="D63">
@@ -3970,17 +4157,20 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G63" s="5" t="s">
+      <c r="G63" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="3"/>
+      <c r="L63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -4005,14 +4195,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B65" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C65" s="5">
+      <c r="B65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4">
         <v>1</v>
       </c>
       <c r="D65">
@@ -4023,24 +4213,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G65" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="4"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B66" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C66" s="5">
+      <c r="B66" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4">
         <v>2</v>
       </c>
       <c r="D66">
@@ -4051,17 +4241,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="4"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="3"/>
+      <c r="L66" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="P66" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Finish reviewing IIIF and collection link conversion
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA88C5E8-49E7-DC4A-A96F-F1A16659B59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919F323-087D-B54D-932D-3A308052CBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="243">
   <si>
     <t>collection</t>
   </si>
@@ -691,77 +691,100 @@
     <t>https://www.kenom.de/iiif/image/record_DE-1966_kenom_389059/record_DE-1966_kenom_389059_vs.jpg/full/120,/0/default.jpg</t>
   </si>
   <si>
-    <t>https:</t>
-  </si>
-  <si>
-    <t>www.kenom.de</t>
-  </si>
-  <si>
-    <t>api</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>records</t>
-  </si>
-  <si>
-    <t>record_DE-1966_kenom_389059</t>
-  </si>
-  <si>
-    <t>files</t>
-  </si>
-  <si>
-    <t>images</t>
-  </si>
-  <si>
-    <t>record_DE-1966_kenom_389059_vs.jpg</t>
-  </si>
-  <si>
-    <t>full</t>
-  </si>
-  <si>
-    <t>!400,400</t>
-  </si>
-  <si>
-    <t>default.jpg</t>
-  </si>
-  <si>
-    <t>iiif</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>120,</t>
-  </si>
-  <si>
-    <t>image link</t>
-  </si>
-  <si>
-    <t>iiif link</t>
-  </si>
-  <si>
-    <t>1. convert "iiif/image" to "api/v1/records"</t>
-  </si>
-  <si>
-    <t>2. Find "record_DE…" substring</t>
-  </si>
-  <si>
-    <t>3. Change "record_DE…" substring to "record_DE…/files/images/"</t>
-  </si>
-  <si>
-    <t>4. Replace "120," to "!600,600"</t>
-  </si>
-  <si>
-    <t>Try breaking into list and working by index?</t>
+    <t>1. Remove ""https://"" from string
+2. Replace ""iiif/image"" with ""api/v1/records""
+3. mod_list = [item + ""/files/images"" if ""record_"" in item and "".jpg"" not in item else item for item in mod_link.split(""/"")]
+4. mod_list = [""!600,600"" if "","" in item else item for item in mod_list]
+5. Join list of strings into one string with ""/""
+6. Concatenate ""https://"" to the front of the string</t>
+  </si>
+  <si>
+    <t>https://ids.lib.harvard.edu/ids/view/43344604?width=3000&amp;height=3000</t>
+  </si>
+  <si>
+    <t>https://nrs.harvard.edu/urn-3:HUAM:COIN07283_dynmc?width=240</t>
+  </si>
+  <si>
+    <t>Does not appear to be scrapable.</t>
+  </si>
+  <si>
+    <t>https://media.getty.edu/iiif/image/6c6daab7-9d8e-41a6-8907-c83b05d61184/full/600,600/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://media.getty.edu/iiif/image/6c6daab7-9d8e-41a6-8907-c83b05d61184/full/,120/0/native.jpg</t>
+  </si>
+  <si>
+    <t>Replace "/,120/0/native.jpg" with "/600,600/0/default.jpg"</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-MUS-062622_kenom_161787/files/images/record_DE-MUS-062622_kenom_161787_vs.jpg/full/!400,400/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-MUS-062622_kenom_161787/record_DE-MUS-062622_kenom_161787_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>Same as Coin Cabinet of the Mainz City Archives</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-MUS-109513_kenom_213442/files/images/record_DE-MUS-109513_kenom_213442_vs.jpg/full/!400,400/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-MUS-109513_kenom_213442/record_DE-MUS-109513_kenom_213442_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-MUS-099114_kenom_183317/files/images/record_DE-MUS-099114_kenom_183317_vs.jpg/full/!400,400/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-MUS-099114_kenom_183317/record_DE-MUS-099114_kenom_183317_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-MUS-805310_kenom_308174/files/images/record_DE-MUS-805310_kenom_308174_vs.jpg/full/!600,600/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-MUS-805310_kenom_308174/record_DE-MUS-805310_kenom_308174_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://iiif.lib.virginia.edu/iiif/tsm:1699771/full/full/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://iiif.lib.virginia.edu/iiif/tsm:1699771/full/,120/0/default.jpg</t>
+  </si>
+  <si>
+    <t>Replace "/,120/" to "/full/". Difference between heads and tails is ID after "tsm:"</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/api/v1/records/record_DE-MUS-878719_kenom_122660/files/images/record_DE-MUS-878719_kenom_122660_vs.jpg/full/!400,400/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.kenom.de/iiif/image/record_DE-MUS-878719_kenom_122660/record_DE-MUS-878719_kenom_122660_vs.jpg/full/120,/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://gams.uni-graz.at/archive/get/o:numis.2531/IMAGE_1</t>
+  </si>
+  <si>
+    <t>http://gams.uni-graz.at/iiif/o:numis.2531/IMAGE_1/full/!120,120/0/default.jpg</t>
+  </si>
+  <si>
+    <t>https://gams.uni-graz.at/archive/get/o:numis.981/IMAGE_1</t>
+  </si>
+  <si>
+    <t>http://gams.uni-graz.at/iiif/o:numis.981/IMAGE_1/full/!120,120/0/default.jpg</t>
+  </si>
+  <si>
+    <t>1. replace "iiif" with "archive/get"
+2. replace with "/full/!120,120/0/default.jpg" with ""
+3. replace "http" with "https"
+(Difference between heads/tails is IMAGE_1/IMAGE_2, which comes from the link)</t>
+  </si>
+  <si>
+    <t>Similar to below. This one link example has two "a" tags. The first tag is populated, the second one is empty.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -785,6 +808,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -795,8 +824,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFD78"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -824,7 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -837,7 +866,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -875,6 +916,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFD78"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2404,13 +2450,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
-  <dimension ref="A1:Y67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L66" sqref="L66"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2425,9 +2471,10 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="48.6640625" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -2459,7 +2506,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2484,7 +2531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2509,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2543,7 +2590,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2577,7 +2624,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2602,7 +2649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2636,7 +2683,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2661,7 +2708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2686,7 +2733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2720,7 +2767,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2745,7 +2792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -2775,51 +2822,11 @@
       <c r="I12" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="L12" t="s">
-        <v>231</v>
-      </c>
-      <c r="M12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="N12" t="s">
-        <v>217</v>
-      </c>
-      <c r="O12" t="s">
-        <v>218</v>
-      </c>
-      <c r="P12" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>220</v>
-      </c>
-      <c r="R12" t="s">
-        <v>221</v>
-      </c>
-      <c r="S12" t="s">
-        <v>222</v>
-      </c>
-      <c r="T12" t="s">
-        <v>223</v>
-      </c>
-      <c r="U12" t="s">
-        <v>224</v>
-      </c>
-      <c r="V12" t="s">
-        <v>225</v>
-      </c>
-      <c r="W12" t="s">
-        <v>226</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2869,7 +2876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2894,7 +2901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2919,7 +2926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2944,7 +2951,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2969,7 +2976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2994,7 +3001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -3019,7 +3026,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -3044,7 +3051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3069,7 +3076,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -3094,7 +3101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -3119,7 +3126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -3144,7 +3151,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3169,7 +3176,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3194,7 +3201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3219,14 +3226,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="B29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29">
@@ -3237,50 +3244,23 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="3"/>
-      <c r="L29" t="s">
-        <v>232</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="H29" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="O29" t="s">
-        <v>228</v>
-      </c>
-      <c r="P29" t="s">
-        <v>229</v>
-      </c>
-      <c r="R29" t="s">
-        <v>221</v>
-      </c>
-      <c r="U29" t="s">
-        <v>224</v>
-      </c>
-      <c r="V29" t="s">
-        <v>225</v>
-      </c>
-      <c r="W29" t="s">
-        <v>230</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3305,7 +3285,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
@@ -3329,11 +3309,17 @@
       <c r="G31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -3558,7 +3544,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>105</v>
       </c>
@@ -3582,12 +3568,16 @@
       <c r="G41" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
-      <c r="P41" s="6" t="s">
-        <v>215</v>
-      </c>
+      <c r="H41" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="P41" s="10"/>
     </row>
     <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -3739,7 +3729,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>123</v>
       </c>
@@ -3763,11 +3753,17 @@
       <c r="G48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3792,7 +3788,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -3817,7 +3813,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -3842,7 +3838,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -3866,18 +3862,17 @@
       <c r="G52" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="3"/>
-      <c r="L52" t="s">
-        <v>233</v>
-      </c>
-      <c r="P52" t="str">
-        <f>SUBSTITUTE(P41, "iiif/image","api/v1/records",1)</f>
-        <v>https://www.kenom.de/api/v1/records/record_DE-1966_kenom_389059/record_DE-1966_kenom_389059_vs.jpg/full/120,/0/default.jpg</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H52" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>136</v>
       </c>
@@ -3901,14 +3896,18 @@
       <c r="G53" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="3"/>
-      <c r="L53" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3933,7 +3932,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>146</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -4033,7 +4032,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -4108,7 +4107,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>158</v>
       </c>
@@ -4132,14 +4131,17 @@
       <c r="G62" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="3"/>
-      <c r="L62" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H62" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>161</v>
       </c>
@@ -4163,14 +4165,17 @@
       <c r="G63" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="3"/>
-      <c r="L63" t="s">
+      <c r="H63" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="I63" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J63" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -4195,7 +4200,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -4219,11 +4224,17 @@
       <c r="G65" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H65" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>164</v>
       </c>
@@ -4247,17 +4258,17 @@
       <c r="G66" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="3"/>
-      <c r="L66" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="P66" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H66" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>190</v>
       </c>
@@ -4267,12 +4278,33 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G64" r:id="rId1" xr:uid="{DA67D385-1BD1-1B49-AC38-DC1F0097C7EC}"/>
+    <hyperlink ref="H29" r:id="rId2" xr:uid="{EA3E0A11-DA6C-374B-89D2-4B9D62190E21}"/>
+    <hyperlink ref="I29" r:id="rId3" xr:uid="{FDEFF056-2EDE-5240-96DF-ED858624CCCF}"/>
+    <hyperlink ref="H31" r:id="rId4" xr:uid="{D95E151D-7F3D-614A-9361-5B1CE18E9057}"/>
+    <hyperlink ref="I31" r:id="rId5" xr:uid="{CCDE5903-6778-AF4F-8FEA-A34355F5CBF7}"/>
+    <hyperlink ref="H41" r:id="rId6" xr:uid="{F0E47668-3724-A746-A30B-30458C176769}"/>
+    <hyperlink ref="I41" r:id="rId7" xr:uid="{CE9F3152-3064-0F4E-8CE5-E21C8F7ED7F4}"/>
+    <hyperlink ref="H48" r:id="rId8" xr:uid="{EA8DD536-5C4F-5E4B-9840-1ABD6B1BA08E}"/>
+    <hyperlink ref="I48" r:id="rId9" xr:uid="{9C082327-A73C-514B-A74F-8B92ADB7D5B0}"/>
+    <hyperlink ref="H52" r:id="rId10" xr:uid="{003554C1-224E-424B-8DF8-CEC71767ECCE}"/>
+    <hyperlink ref="I52" r:id="rId11" xr:uid="{66D05ADF-07D0-7E4A-BCF4-309FF4649111}"/>
+    <hyperlink ref="H53" r:id="rId12" xr:uid="{F2927119-8074-4F46-B453-A87FCCC5FBD2}"/>
+    <hyperlink ref="I53" r:id="rId13" xr:uid="{A4606C0A-8884-7D48-8542-036C271D85F0}"/>
+    <hyperlink ref="H62" r:id="rId14" xr:uid="{A2A800BC-3B18-B44E-B5C3-453D2248D028}"/>
+    <hyperlink ref="I62" r:id="rId15" xr:uid="{19D25D6B-6515-E14A-973C-545CAF76E107}"/>
+    <hyperlink ref="H63" r:id="rId16" xr:uid="{73EC1D96-C559-6E49-9186-6D2B433ED210}"/>
+    <hyperlink ref="I63" r:id="rId17" xr:uid="{2ED7BBCE-750B-2446-A5FC-8B06696E163D}"/>
+    <hyperlink ref="H65" r:id="rId18" xr:uid="{A15065EE-A649-C048-83C0-6AC7F91E83AC}"/>
+    <hyperlink ref="I65" r:id="rId19" xr:uid="{968B633B-85F4-E145-A01E-D89C2E6A132A}"/>
+    <hyperlink ref="H66" r:id="rId20" xr:uid="{718848CF-7DD6-594B-9F8D-3E76791CADFE}"/>
+    <hyperlink ref="I66" r:id="rId21" xr:uid="{223800AA-A6C1-2D42-8154-61CFBA8142F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Review non-IIIF images links
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31488914-931B-C64C-BDC5-B0324172802F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4D254-9651-D541-8597-565E1F42A403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-26880" yWindow="2580" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="245">
   <si>
     <t>collection</t>
   </si>
@@ -778,6 +778,12 @@
   </si>
   <si>
     <t>Similar to below. This one link example has two "a" tags. The first tag is populated, the second one is empty.</t>
+  </si>
+  <si>
+    <t>"href" element from "a" tag.</t>
+  </si>
+  <si>
+    <t>Redirects to home page of museum where there is no image to scrape. This link may help resolve the issue: https://stackoverflow.com/questions/110498/is-there-an-easy-way-to-request-a-url-in-python-and-not-follow-redirects</t>
   </si>
 </sst>
 </file>
@@ -878,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -886,7 +892,31 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -964,7 +994,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="11">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -975,29 +1005,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="2">
-  <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="10">
+  <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="9">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="8">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2453,35 +2477,35 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="40" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9" style="4" customWidth="1"/>
+    <col min="3" max="3" width="4.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="0.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="48.6640625" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="48.6640625" style="3" customWidth="1"/>
     <col min="15" max="15" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2490,23 +2514,23 @@
       <c r="E1" t="s">
         <v>197</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2530,8 +2554,11 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2555,6 +2582,9 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2624,14 +2654,14 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
         <v>2</v>
       </c>
       <c r="D6">
@@ -2642,11 +2672,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
@@ -2683,7 +2716,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2707,15 +2740,18 @@
       <c r="G8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9">
@@ -2726,11 +2762,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2767,14 +2806,14 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>2</v>
       </c>
       <c r="D11">
@@ -2785,11 +2824,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="153" x14ac:dyDescent="0.2">
@@ -2826,14 +2868,14 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
         <v>2</v>
       </c>
       <c r="D13">
@@ -2844,21 +2886,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="J13" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
         <v>2</v>
       </c>
       <c r="D14">
@@ -2869,21 +2914,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="J14" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
         <v>2</v>
       </c>
       <c r="D15">
@@ -2894,21 +2942,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="J15" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16">
@@ -2919,21 +2970,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="J16" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
         <v>2</v>
       </c>
       <c r="D17">
@@ -2944,21 +2998,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="J17" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
         <v>2</v>
       </c>
       <c r="D18">
@@ -2969,21 +3026,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="J18" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
         <v>2</v>
       </c>
       <c r="D19">
@@ -2994,21 +3054,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="J19" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
         <v>2</v>
       </c>
       <c r="D20">
@@ -3019,21 +3082,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="J20" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
         <v>2</v>
       </c>
       <c r="D21">
@@ -3044,21 +3110,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="J21" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
         <v>2</v>
       </c>
       <c r="D22">
@@ -3069,21 +3138,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="J22" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B23" t="b">
-        <v>0</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
         <v>2</v>
       </c>
       <c r="D23">
@@ -3094,21 +3166,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="J23" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
         <v>2</v>
       </c>
       <c r="D24">
@@ -3119,14 +3194,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -3150,15 +3228,18 @@
       <c r="G25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
         <v>2</v>
       </c>
       <c r="D26">
@@ -3169,21 +3250,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="J26" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
         <v>2</v>
       </c>
       <c r="D27">
@@ -3194,21 +3278,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="J27" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="b">
-        <v>0</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
         <v>1</v>
       </c>
       <c r="D28">
@@ -3219,11 +3306,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="4" t="s">
         <v>72</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3260,7 +3350,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3284,6 +3374,9 @@
       <c r="G30" t="s">
         <v>78</v>
       </c>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
     </row>
     <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
@@ -3319,14 +3412,14 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
         <v>2</v>
       </c>
       <c r="D32">
@@ -3337,14 +3430,17 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -3368,15 +3464,18 @@
       <c r="G33" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B34" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
         <v>1</v>
       </c>
       <c r="D34">
@@ -3387,21 +3486,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="J34" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B35" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
         <v>2</v>
       </c>
       <c r="D35">
@@ -3412,21 +3514,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="J35" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8">
         <v>2</v>
       </c>
       <c r="D36">
@@ -3437,21 +3542,26 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B37" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8">
         <v>2</v>
       </c>
       <c r="D37">
@@ -3462,21 +3572,26 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38">
+      <c r="B38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
         <v>2</v>
       </c>
       <c r="D38">
@@ -3487,21 +3602,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="J38" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39">
+      <c r="B39" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
         <v>2</v>
       </c>
       <c r="D39">
@@ -3512,21 +3630,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="J39" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B40" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40">
+      <c r="B40" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
         <v>2</v>
       </c>
       <c r="D40">
@@ -3537,11 +3658,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="4" t="s">
         <v>104</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -3579,14 +3703,14 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
         <v>2</v>
       </c>
       <c r="D42">
@@ -3597,21 +3721,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="J42" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
         <v>2</v>
       </c>
       <c r="D43">
@@ -3622,21 +3749,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="J43" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B44" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
         <v>2</v>
       </c>
       <c r="D44">
@@ -3647,21 +3777,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="J44" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B45" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
         <v>2</v>
       </c>
       <c r="D45">
@@ -3672,21 +3805,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="J45" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B46" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
         <v>2</v>
       </c>
       <c r="D46">
@@ -3697,21 +3833,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="J46" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47">
+      <c r="B47" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
         <v>2</v>
       </c>
       <c r="D47">
@@ -3722,11 +3861,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="4" t="s">
         <v>122</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -3763,7 +3905,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3787,8 +3929,11 @@
       <c r="G49" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -3812,15 +3957,18 @@
       <c r="G50" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B51" t="b">
-        <v>0</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4">
         <v>1</v>
       </c>
       <c r="D51">
@@ -3831,11 +3979,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3907,14 +4058,14 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B54" t="b">
-        <v>0</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="4">
         <v>2</v>
       </c>
       <c r="D54">
@@ -3925,21 +4076,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="J54" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="b">
-        <v>0</v>
-      </c>
-      <c r="C55">
+      <c r="B55" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4">
         <v>2</v>
       </c>
       <c r="D55">
@@ -3950,21 +4104,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="J55" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B56" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56">
+      <c r="B56" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="4">
         <v>2</v>
       </c>
       <c r="D56">
@@ -3975,21 +4132,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="J56" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B57" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57">
+      <c r="B57" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
         <v>2</v>
       </c>
       <c r="D57">
@@ -4000,21 +4160,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="J57" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B58" t="b">
-        <v>0</v>
-      </c>
-      <c r="C58">
+      <c r="B58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4">
         <v>2</v>
       </c>
       <c r="D58">
@@ -4025,21 +4188,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="J58" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B59" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59">
+      <c r="B59" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
         <v>2</v>
       </c>
       <c r="D59">
@@ -4050,21 +4216,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="J59" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B60" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60">
+      <c r="B60" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" s="4">
         <v>2</v>
       </c>
       <c r="D60">
@@ -4075,21 +4244,24 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="J60" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B61" t="b">
-        <v>0</v>
-      </c>
-      <c r="C61">
+      <c r="B61" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="4">
         <v>2</v>
       </c>
       <c r="D61">
@@ -4100,11 +4272,14 @@
         <f>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</f>
         <v>do not hide</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="4" t="s">
         <v>157</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4175,7 +4350,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -4199,6 +4374,9 @@
       <c r="G64" s="1" t="s">
         <v>166</v>
       </c>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
     </row>
     <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
@@ -4269,12 +4447,12 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="4">
         <f>SUBTOTAL(103,CollectionsAndIIIFTable[example_page_link])</f>
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add typological fields to review file
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4D254-9651-D541-8597-565E1F42A403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5066CAAD-ACCC-CD45-9226-E9C20013DDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26880" yWindow="2580" windowWidth="23040" windowHeight="13900" activeTab="4" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-24820" yWindow="2460" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="532">
   <si>
     <t>collection</t>
   </si>
@@ -784,6 +784,867 @@
   </si>
   <si>
     <t>Redirects to home page of museum where there is no image to scrape. This link may help resolve the issue: https://stackoverflow.com/questions/110498/is-there-an-easy-way-to-request-a-url-in-python-and-not-follow-redirects</t>
+  </si>
+  <si>
+    <t>_date</t>
+  </si>
+  <si>
+    <t>19 BC</t>
+  </si>
+  <si>
+    <t>_date_range</t>
+  </si>
+  <si>
+    <t>25 BC - 23 BC</t>
+  </si>
+  <si>
+    <t>_denomination</t>
+  </si>
+  <si>
+    <t>Quinarius</t>
+  </si>
+  <si>
+    <t>_denomination2</t>
+  </si>
+  <si>
+    <t>AE1</t>
+  </si>
+  <si>
+    <t>_manufacture</t>
+  </si>
+  <si>
+    <t>Struck</t>
+  </si>
+  <si>
+    <t>_material</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>_material2</t>
+  </si>
+  <si>
+    <t>Bronze (uncertain)</t>
+  </si>
+  <si>
+    <t>_object_type</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>_object_type2</t>
+  </si>
+  <si>
+    <t>Medallion</t>
+  </si>
+  <si>
+    <t>authority_authority</t>
+  </si>
+  <si>
+    <t>Augustus</t>
+  </si>
+  <si>
+    <t>authority_authority2</t>
+  </si>
+  <si>
+    <t>Flavius Marcus</t>
+  </si>
+  <si>
+    <t>authority_issuer</t>
+  </si>
+  <si>
+    <t>P. Carisius</t>
+  </si>
+  <si>
+    <t>authority_issuer2</t>
+  </si>
+  <si>
+    <t>Galus</t>
+  </si>
+  <si>
+    <t>authority_issuer3</t>
+  </si>
+  <si>
+    <t>Messalla</t>
+  </si>
+  <si>
+    <t>authority_issuer4</t>
+  </si>
+  <si>
+    <t>Sisenna</t>
+  </si>
+  <si>
+    <t>authority_stated_authority</t>
+  </si>
+  <si>
+    <t>Priscus Attalus</t>
+  </si>
+  <si>
+    <t>date_on_object_date</t>
+  </si>
+  <si>
+    <t>AD 269</t>
+  </si>
+  <si>
+    <t>geographic_mint</t>
+  </si>
+  <si>
+    <t>Emerita</t>
+  </si>
+  <si>
+    <t>geographic_mint2</t>
+  </si>
+  <si>
+    <t>Ravenna</t>
+  </si>
+  <si>
+    <t>geographic_mint3</t>
+  </si>
+  <si>
+    <t>Aquileia</t>
+  </si>
+  <si>
+    <t>geographic_mint4</t>
+  </si>
+  <si>
+    <t>Antioch</t>
+  </si>
+  <si>
+    <t>geographic_mint5</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>geographic_region</t>
+  </si>
+  <si>
+    <t>Lusitania</t>
+  </si>
+  <si>
+    <t>geographic_region2</t>
+  </si>
+  <si>
+    <t>Gallia</t>
+  </si>
+  <si>
+    <t>geographic_region3</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>geographic_region4</t>
+  </si>
+  <si>
+    <t>Mysia</t>
+  </si>
+  <si>
+    <t>obverse_controlmark</t>
+  </si>
+  <si>
+    <t>• • •</t>
+  </si>
+  <si>
+    <t>obverse_deity</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>obverse_deity2</t>
+  </si>
+  <si>
+    <t>Alamannia</t>
+  </si>
+  <si>
+    <t>obverse_deity3</t>
+  </si>
+  <si>
+    <t>Juno</t>
+  </si>
+  <si>
+    <t>obverse_deity4</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>obverse_deity5</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>obverse_deity6</t>
+  </si>
+  <si>
+    <t>Minerva</t>
+  </si>
+  <si>
+    <t>obverse_legend</t>
+  </si>
+  <si>
+    <t>AVGVST</t>
+  </si>
+  <si>
+    <t>obverse_portrait</t>
+  </si>
+  <si>
+    <t>obverse_portrait2</t>
+  </si>
+  <si>
+    <t>obverse_state</t>
+  </si>
+  <si>
+    <t>Roman Republic</t>
+  </si>
+  <si>
+    <t>obverse_state2</t>
+  </si>
+  <si>
+    <t>obverse_type</t>
+  </si>
+  <si>
+    <t>Head of Augustus, bare, left</t>
+  </si>
+  <si>
+    <t>reverse_control_marks</t>
+  </si>
+  <si>
+    <t>A/-//-</t>
+  </si>
+  <si>
+    <t>reverse_deity</t>
+  </si>
+  <si>
+    <t>Victory</t>
+  </si>
+  <si>
+    <t>reverse_deity2</t>
+  </si>
+  <si>
+    <t>Genius</t>
+  </si>
+  <si>
+    <t>reverse_deity3</t>
+  </si>
+  <si>
+    <t>Constantinopolis</t>
+  </si>
+  <si>
+    <t>reverse_deity4</t>
+  </si>
+  <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>reverse_deity5</t>
+  </si>
+  <si>
+    <t>Remus</t>
+  </si>
+  <si>
+    <t>reverse_dynasty</t>
+  </si>
+  <si>
+    <t>Artaxiad Dynasty</t>
+  </si>
+  <si>
+    <t>reverse_legend</t>
+  </si>
+  <si>
+    <t>P CARISI LEG</t>
+  </si>
+  <si>
+    <t>reverse_mintmark</t>
+  </si>
+  <si>
+    <t>B/-//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark10</t>
+  </si>
+  <si>
+    <t>S/-//MLXXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark11</t>
+  </si>
+  <si>
+    <t>S/P//MLXXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark12</t>
+  </si>
+  <si>
+    <t>V/*//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark13</t>
+  </si>
+  <si>
+    <t>F/O//M(inv. L)</t>
+  </si>
+  <si>
+    <t>reverse_mintmark14</t>
+  </si>
+  <si>
+    <t>F/S//ML</t>
+  </si>
+  <si>
+    <t>reverse_mintmark15</t>
+  </si>
+  <si>
+    <t>L/-//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark16</t>
+  </si>
+  <si>
+    <t>-/L//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark17</t>
+  </si>
+  <si>
+    <t>L/-//ML</t>
+  </si>
+  <si>
+    <t>reverse_mintmark18</t>
+  </si>
+  <si>
+    <t>M/O//ML</t>
+  </si>
+  <si>
+    <t>reverse_mintmark19</t>
+  </si>
+  <si>
+    <t>O/F//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark2</t>
+  </si>
+  <si>
+    <t>-/-//SMNΓ</t>
+  </si>
+  <si>
+    <t>reverse_mintmark20</t>
+  </si>
+  <si>
+    <t>-/O//ML</t>
+  </si>
+  <si>
+    <t>reverse_mintmark21</t>
+  </si>
+  <si>
+    <t>S/P//MLXX</t>
+  </si>
+  <si>
+    <t>reverse_mintmark22</t>
+  </si>
+  <si>
+    <t>reverse_mintmark23</t>
+  </si>
+  <si>
+    <t>(crescent on Z)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark24</t>
+  </si>
+  <si>
+    <t>(crescent on H)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark25</t>
+  </si>
+  <si>
+    <t>(crescent on ∈Δ)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark26</t>
+  </si>
+  <si>
+    <t>(• on A)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark27</t>
+  </si>
+  <si>
+    <t>(• on B)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark28</t>
+  </si>
+  <si>
+    <t>(• on Γ)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark29</t>
+  </si>
+  <si>
+    <t>(• on Δ)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark3</t>
+  </si>
+  <si>
+    <t>-/-//SMNΓ•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark30</t>
+  </si>
+  <si>
+    <t>(• on ϵ)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark31</t>
+  </si>
+  <si>
+    <t>(• on ς)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark32</t>
+  </si>
+  <si>
+    <t>(• on Z)//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark33</t>
+  </si>
+  <si>
+    <t>A//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark34</t>
+  </si>
+  <si>
+    <t>B//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark35</t>
+  </si>
+  <si>
+    <t>Γ//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark36</t>
+  </si>
+  <si>
+    <t>Δ//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark37</t>
+  </si>
+  <si>
+    <t>ϵ//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark38</t>
+  </si>
+  <si>
+    <t>ς//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark39</t>
+  </si>
+  <si>
+    <t>Z//•XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark4</t>
+  </si>
+  <si>
+    <t>-/H//Δ</t>
+  </si>
+  <si>
+    <t>reverse_mintmark40</t>
+  </si>
+  <si>
+    <t>A//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark41</t>
+  </si>
+  <si>
+    <t>B//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark42</t>
+  </si>
+  <si>
+    <t>Γ//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark43</t>
+  </si>
+  <si>
+    <t>Δ//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark44</t>
+  </si>
+  <si>
+    <t>ϵ//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark45</t>
+  </si>
+  <si>
+    <t>ς//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark46</t>
+  </si>
+  <si>
+    <t>Z//XXI•</t>
+  </si>
+  <si>
+    <t>reverse_mintmark47</t>
+  </si>
+  <si>
+    <t>-/-//XXIT</t>
+  </si>
+  <si>
+    <t>reverse_mintmark48</t>
+  </si>
+  <si>
+    <t>-/-//XXIQ</t>
+  </si>
+  <si>
+    <t>reverse_mintmark49</t>
+  </si>
+  <si>
+    <t>-/-//XXIV</t>
+  </si>
+  <si>
+    <t>reverse_mintmark5</t>
+  </si>
+  <si>
+    <t>S/Γ//XXI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark50</t>
+  </si>
+  <si>
+    <t>-/-//XXIVI</t>
+  </si>
+  <si>
+    <t>reverse_mintmark6</t>
+  </si>
+  <si>
+    <t>ISI//XXIΓ</t>
+  </si>
+  <si>
+    <t>reverse_mintmark7</t>
+  </si>
+  <si>
+    <t>-/-//XXIΓS</t>
+  </si>
+  <si>
+    <t>reverse_mintmark8</t>
+  </si>
+  <si>
+    <t>L/*//-</t>
+  </si>
+  <si>
+    <t>reverse_mintmark9</t>
+  </si>
+  <si>
+    <t>reverse_monogram</t>
+  </si>
+  <si>
+    <t>Monogram 1 (Zeno)</t>
+  </si>
+  <si>
+    <t>reverse_officinamark</t>
+  </si>
+  <si>
+    <t>-/-//IIII</t>
+  </si>
+  <si>
+    <t>reverse_officinamark10</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>reverse_officinamark11</t>
+  </si>
+  <si>
+    <t>θ</t>
+  </si>
+  <si>
+    <t>reverse_officinamark12</t>
+  </si>
+  <si>
+    <t>reverse_officinamark13</t>
+  </si>
+  <si>
+    <t>ΓI</t>
+  </si>
+  <si>
+    <t>reverse_officinamark14</t>
+  </si>
+  <si>
+    <t>ΔI</t>
+  </si>
+  <si>
+    <t>reverse_officinamark15</t>
+  </si>
+  <si>
+    <t>∈I</t>
+  </si>
+  <si>
+    <t>reverse_officinamark2</t>
+  </si>
+  <si>
+    <t>Δ</t>
+  </si>
+  <si>
+    <t>reverse_officinamark3</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>reverse_officinamark4</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>reverse_officinamark5</t>
+  </si>
+  <si>
+    <t>∈</t>
+  </si>
+  <si>
+    <t>reverse_officinamark6</t>
+  </si>
+  <si>
+    <t>reverse_officinamark7</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>reverse_officinamark8</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>reverse_officinamark9</t>
+  </si>
+  <si>
+    <t>reverse_portrait</t>
+  </si>
+  <si>
+    <t>reverse_portrait2</t>
+  </si>
+  <si>
+    <t>Leo I</t>
+  </si>
+  <si>
+    <t>reverse_portrait3</t>
+  </si>
+  <si>
+    <t>Aelia Pulcheria</t>
+  </si>
+  <si>
+    <t>reverse_portrait4</t>
+  </si>
+  <si>
+    <t>Constantius II</t>
+  </si>
+  <si>
+    <t>reverse_portrait5</t>
+  </si>
+  <si>
+    <t>Dalmatius</t>
+  </si>
+  <si>
+    <t>reverse_state</t>
+  </si>
+  <si>
+    <t>reverse_state2</t>
+  </si>
+  <si>
+    <t>reverse_symbol</t>
+  </si>
+  <si>
+    <t>Monogram 1 (Theodosius II)</t>
+  </si>
+  <si>
+    <t>reverse_symbol2</t>
+  </si>
+  <si>
+    <t>Monogram 2 (Libius Severus) consists of C, E, V, R, and A</t>
+  </si>
+  <si>
+    <t>reverse_type</t>
+  </si>
+  <si>
+    <t>Victory standing right, placing wreath on trophy with dagger and sword at base</t>
+  </si>
+  <si>
+    <t>coin_id_example</t>
+  </si>
+  <si>
+    <t>example_value</t>
+  </si>
+  <si>
+    <t>example_uri</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.59</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.9.rom.42B</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.8.alex.92</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.2_3(2).hdn.2937</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.bas-mar_e.1034</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.464</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.visi.3701</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.mar.3</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.valt_iii_w.2074</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.cg.298</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.cg.266</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.aur.100</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.4.tr_d.48</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.251</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.6.tri.811</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).tib.67</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.2.tr.793</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.2.tr.811</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.4.ph_i.7</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.hon_w.1337</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.9.tri.99</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.4.ge.184</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.3.m_aur.736</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).gai.59</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.sala(2).1</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.cara.121</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.cara.101</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.7.nic.20</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.dio.323</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.7.nic.11</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.6.carth.26b</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.aur.244</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.jul_i.4</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.zeno(2)_e.958</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.5.fl.1</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.zeno(2)_e.936</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.zeno(2)_e.930</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.8.anch.194</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.visi.3775</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.valt_iii_w.2133</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.162A</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.anth_w.2899</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.marc_e.502</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.7.nic.89</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.7.cnp.89</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.1(2).aug.337</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.2.tr.797</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.theo_ii_e.462</t>
+  </si>
+  <si>
+    <t>http://numismatics.org/ocre/id/ric.10.lib_sev_w.2717</t>
   </si>
 </sst>
 </file>
@@ -976,6 +1837,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:D124" totalsRowShown="0">
+  <autoFilter ref="A1:D124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}" name="Table3" displayName="Table3" ref="A1:E9" totalsRowCount="1">
   <autoFilter ref="A1:E8" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}"/>
   <tableColumns count="5">
@@ -989,7 +1863,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:D57" totalsRowCount="1">
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
@@ -1004,7 +1878,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
@@ -1327,7 +2201,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,13 +2287,1761 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ECEDEA-565B-2645-A3E1-F668D8278F57}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <v>38964</v>
+      </c>
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8">
+        <v>37842</v>
+      </c>
+      <c r="C8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B10">
+        <v>7820</v>
+      </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12">
+        <v>40202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14">
+        <v>541</v>
+      </c>
+      <c r="C14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15">
+        <v>541</v>
+      </c>
+      <c r="C15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D15" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16">
+        <v>541</v>
+      </c>
+      <c r="C16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17">
+        <v>41163</v>
+      </c>
+      <c r="C17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18">
+        <v>24728</v>
+      </c>
+      <c r="C18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D18" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B20">
+        <v>40646</v>
+      </c>
+      <c r="C20" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21">
+        <v>21341</v>
+      </c>
+      <c r="C21" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>285</v>
+      </c>
+      <c r="B22">
+        <v>21306</v>
+      </c>
+      <c r="C22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D22" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B23">
+        <v>21306</v>
+      </c>
+      <c r="C23" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25">
+        <v>21527</v>
+      </c>
+      <c r="C25" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>293</v>
+      </c>
+      <c r="B26">
+        <v>21306</v>
+      </c>
+      <c r="C26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D26" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27">
+        <v>21306</v>
+      </c>
+      <c r="C27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D27" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28">
+        <v>18819</v>
+      </c>
+      <c r="C28" t="s">
+        <v>298</v>
+      </c>
+      <c r="D28" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>299</v>
+      </c>
+      <c r="B29">
+        <v>323</v>
+      </c>
+      <c r="C29" t="s">
+        <v>300</v>
+      </c>
+      <c r="D29" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>301</v>
+      </c>
+      <c r="B30">
+        <v>27853</v>
+      </c>
+      <c r="C30" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>303</v>
+      </c>
+      <c r="B31">
+        <v>696</v>
+      </c>
+      <c r="C31" t="s">
+        <v>304</v>
+      </c>
+      <c r="D31" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32">
+        <v>696</v>
+      </c>
+      <c r="C32" t="s">
+        <v>306</v>
+      </c>
+      <c r="D32" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B33">
+        <v>696</v>
+      </c>
+      <c r="C33" t="s">
+        <v>308</v>
+      </c>
+      <c r="D33" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>309</v>
+      </c>
+      <c r="B34">
+        <v>696</v>
+      </c>
+      <c r="C34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D34" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>311</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>312</v>
+      </c>
+      <c r="D35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>313</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37">
+        <v>40202</v>
+      </c>
+      <c r="C37" t="s">
+        <v>266</v>
+      </c>
+      <c r="D37" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38">
+        <v>6546</v>
+      </c>
+      <c r="C38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39">
+        <v>6564</v>
+      </c>
+      <c r="C39" t="s">
+        <v>316</v>
+      </c>
+      <c r="D39" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>318</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>320</v>
+      </c>
+      <c r="B41">
+        <v>18487</v>
+      </c>
+      <c r="C41" t="s">
+        <v>321</v>
+      </c>
+      <c r="D41" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>322</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>323</v>
+      </c>
+      <c r="D42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43">
+        <v>40418</v>
+      </c>
+      <c r="C43" t="s">
+        <v>325</v>
+      </c>
+      <c r="D43" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>326</v>
+      </c>
+      <c r="B44">
+        <v>39519</v>
+      </c>
+      <c r="C44" t="s">
+        <v>327</v>
+      </c>
+      <c r="D44" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>328</v>
+      </c>
+      <c r="B45">
+        <v>16073</v>
+      </c>
+      <c r="C45" t="s">
+        <v>329</v>
+      </c>
+      <c r="D45" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46">
+        <v>11115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>331</v>
+      </c>
+      <c r="D46" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>332</v>
+      </c>
+      <c r="B47">
+        <v>783</v>
+      </c>
+      <c r="C47" t="s">
+        <v>333</v>
+      </c>
+      <c r="D47" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>334</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>335</v>
+      </c>
+      <c r="D48" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>336</v>
+      </c>
+      <c r="B49">
+        <v>20948</v>
+      </c>
+      <c r="C49" t="s">
+        <v>337</v>
+      </c>
+      <c r="D49" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>338</v>
+      </c>
+      <c r="B50">
+        <v>25291</v>
+      </c>
+      <c r="C50" t="s">
+        <v>339</v>
+      </c>
+      <c r="D50" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>340</v>
+      </c>
+      <c r="B51">
+        <v>25291</v>
+      </c>
+      <c r="C51" t="s">
+        <v>341</v>
+      </c>
+      <c r="D51" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>342</v>
+      </c>
+      <c r="B52">
+        <v>25291</v>
+      </c>
+      <c r="C52" t="s">
+        <v>343</v>
+      </c>
+      <c r="D52" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B53">
+        <v>25271</v>
+      </c>
+      <c r="C53" t="s">
+        <v>345</v>
+      </c>
+      <c r="D53" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>346</v>
+      </c>
+      <c r="B54">
+        <v>25271</v>
+      </c>
+      <c r="C54" t="s">
+        <v>347</v>
+      </c>
+      <c r="D54" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>348</v>
+      </c>
+      <c r="B55">
+        <v>25271</v>
+      </c>
+      <c r="C55" t="s">
+        <v>349</v>
+      </c>
+      <c r="D55" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>350</v>
+      </c>
+      <c r="B56">
+        <v>25271</v>
+      </c>
+      <c r="C56" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>352</v>
+      </c>
+      <c r="B57">
+        <v>25271</v>
+      </c>
+      <c r="C57" t="s">
+        <v>353</v>
+      </c>
+      <c r="D57" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>354</v>
+      </c>
+      <c r="B58">
+        <v>25271</v>
+      </c>
+      <c r="C58" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>356</v>
+      </c>
+      <c r="B59">
+        <v>25271</v>
+      </c>
+      <c r="C59" t="s">
+        <v>357</v>
+      </c>
+      <c r="D59" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>358</v>
+      </c>
+      <c r="B60">
+        <v>34019</v>
+      </c>
+      <c r="C60" t="s">
+        <v>359</v>
+      </c>
+      <c r="D60" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>360</v>
+      </c>
+      <c r="B61">
+        <v>25271</v>
+      </c>
+      <c r="C61" t="s">
+        <v>361</v>
+      </c>
+      <c r="D61" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>362</v>
+      </c>
+      <c r="B62">
+        <v>25271</v>
+      </c>
+      <c r="C62" t="s">
+        <v>363</v>
+      </c>
+      <c r="D62" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>364</v>
+      </c>
+      <c r="B63">
+        <v>25271</v>
+      </c>
+      <c r="C63" t="s">
+        <v>341</v>
+      </c>
+      <c r="D63" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>365</v>
+      </c>
+      <c r="B64">
+        <v>23923</v>
+      </c>
+      <c r="C64" t="s">
+        <v>366</v>
+      </c>
+      <c r="D64" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>367</v>
+      </c>
+      <c r="B65">
+        <v>23923</v>
+      </c>
+      <c r="C65" t="s">
+        <v>368</v>
+      </c>
+      <c r="D65" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>369</v>
+      </c>
+      <c r="B66">
+        <v>23923</v>
+      </c>
+      <c r="C66" t="s">
+        <v>370</v>
+      </c>
+      <c r="D66" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>371</v>
+      </c>
+      <c r="B67">
+        <v>23923</v>
+      </c>
+      <c r="C67" t="s">
+        <v>372</v>
+      </c>
+      <c r="D67" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>373</v>
+      </c>
+      <c r="B68">
+        <v>23923</v>
+      </c>
+      <c r="C68" t="s">
+        <v>374</v>
+      </c>
+      <c r="D68" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>375</v>
+      </c>
+      <c r="B69">
+        <v>23923</v>
+      </c>
+      <c r="C69" t="s">
+        <v>376</v>
+      </c>
+      <c r="D69" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>377</v>
+      </c>
+      <c r="B70">
+        <v>23923</v>
+      </c>
+      <c r="C70" t="s">
+        <v>378</v>
+      </c>
+      <c r="D70" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>379</v>
+      </c>
+      <c r="B71">
+        <v>34010</v>
+      </c>
+      <c r="C71" t="s">
+        <v>380</v>
+      </c>
+      <c r="D71" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>381</v>
+      </c>
+      <c r="B72">
+        <v>23923</v>
+      </c>
+      <c r="C72" t="s">
+        <v>382</v>
+      </c>
+      <c r="D72" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>383</v>
+      </c>
+      <c r="B73">
+        <v>23923</v>
+      </c>
+      <c r="C73" t="s">
+        <v>384</v>
+      </c>
+      <c r="D73" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>385</v>
+      </c>
+      <c r="B74">
+        <v>23923</v>
+      </c>
+      <c r="C74" t="s">
+        <v>386</v>
+      </c>
+      <c r="D74" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>387</v>
+      </c>
+      <c r="B75">
+        <v>23923</v>
+      </c>
+      <c r="C75" t="s">
+        <v>388</v>
+      </c>
+      <c r="D75" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>389</v>
+      </c>
+      <c r="B76">
+        <v>23923</v>
+      </c>
+      <c r="C76" t="s">
+        <v>390</v>
+      </c>
+      <c r="D76" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>391</v>
+      </c>
+      <c r="B77">
+        <v>23923</v>
+      </c>
+      <c r="C77" t="s">
+        <v>392</v>
+      </c>
+      <c r="D77" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>393</v>
+      </c>
+      <c r="B78">
+        <v>23923</v>
+      </c>
+      <c r="C78" t="s">
+        <v>394</v>
+      </c>
+      <c r="D78" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>395</v>
+      </c>
+      <c r="B79">
+        <v>23923</v>
+      </c>
+      <c r="C79" t="s">
+        <v>396</v>
+      </c>
+      <c r="D79" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>397</v>
+      </c>
+      <c r="B80">
+        <v>23923</v>
+      </c>
+      <c r="C80" t="s">
+        <v>398</v>
+      </c>
+      <c r="D80" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>399</v>
+      </c>
+      <c r="B81">
+        <v>23923</v>
+      </c>
+      <c r="C81" t="s">
+        <v>400</v>
+      </c>
+      <c r="D81" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>401</v>
+      </c>
+      <c r="B82">
+        <v>29419</v>
+      </c>
+      <c r="C82" t="s">
+        <v>402</v>
+      </c>
+      <c r="D82" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>403</v>
+      </c>
+      <c r="B83">
+        <v>23923</v>
+      </c>
+      <c r="C83" t="s">
+        <v>404</v>
+      </c>
+      <c r="D83" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>405</v>
+      </c>
+      <c r="B84">
+        <v>23923</v>
+      </c>
+      <c r="C84" t="s">
+        <v>406</v>
+      </c>
+      <c r="D84" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>407</v>
+      </c>
+      <c r="B85">
+        <v>23923</v>
+      </c>
+      <c r="C85" t="s">
+        <v>408</v>
+      </c>
+      <c r="D85" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>409</v>
+      </c>
+      <c r="B86">
+        <v>23923</v>
+      </c>
+      <c r="C86" t="s">
+        <v>410</v>
+      </c>
+      <c r="D86" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>411</v>
+      </c>
+      <c r="B87">
+        <v>23923</v>
+      </c>
+      <c r="C87" t="s">
+        <v>412</v>
+      </c>
+      <c r="D87" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>413</v>
+      </c>
+      <c r="B88">
+        <v>23923</v>
+      </c>
+      <c r="C88" t="s">
+        <v>414</v>
+      </c>
+      <c r="D88" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>415</v>
+      </c>
+      <c r="B89">
+        <v>23923</v>
+      </c>
+      <c r="C89" t="s">
+        <v>416</v>
+      </c>
+      <c r="D89" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>417</v>
+      </c>
+      <c r="B90">
+        <v>21669</v>
+      </c>
+      <c r="C90" t="s">
+        <v>418</v>
+      </c>
+      <c r="D90" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>419</v>
+      </c>
+      <c r="B91">
+        <v>21669</v>
+      </c>
+      <c r="C91" t="s">
+        <v>420</v>
+      </c>
+      <c r="D91" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>421</v>
+      </c>
+      <c r="B92">
+        <v>21669</v>
+      </c>
+      <c r="C92" t="s">
+        <v>422</v>
+      </c>
+      <c r="D92" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>423</v>
+      </c>
+      <c r="B93">
+        <v>26506</v>
+      </c>
+      <c r="C93" t="s">
+        <v>424</v>
+      </c>
+      <c r="D93" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>425</v>
+      </c>
+      <c r="B94">
+        <v>21669</v>
+      </c>
+      <c r="C94" t="s">
+        <v>426</v>
+      </c>
+      <c r="D94" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>427</v>
+      </c>
+      <c r="B95">
+        <v>26506</v>
+      </c>
+      <c r="C95" t="s">
+        <v>428</v>
+      </c>
+      <c r="D95" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>429</v>
+      </c>
+      <c r="B96">
+        <v>26506</v>
+      </c>
+      <c r="C96" t="s">
+        <v>430</v>
+      </c>
+      <c r="D96" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>431</v>
+      </c>
+      <c r="B97">
+        <v>25291</v>
+      </c>
+      <c r="C97" t="s">
+        <v>432</v>
+      </c>
+      <c r="D97" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>433</v>
+      </c>
+      <c r="B98">
+        <v>25291</v>
+      </c>
+      <c r="C98" t="s">
+        <v>353</v>
+      </c>
+      <c r="D98" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>434</v>
+      </c>
+      <c r="B99">
+        <v>40260</v>
+      </c>
+      <c r="C99" t="s">
+        <v>435</v>
+      </c>
+      <c r="D99" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>436</v>
+      </c>
+      <c r="B100">
+        <v>22083</v>
+      </c>
+      <c r="C100" t="s">
+        <v>437</v>
+      </c>
+      <c r="D100" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>438</v>
+      </c>
+      <c r="B101">
+        <v>40236</v>
+      </c>
+      <c r="C101" t="s">
+        <v>439</v>
+      </c>
+      <c r="D101" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>440</v>
+      </c>
+      <c r="B102">
+        <v>40229</v>
+      </c>
+      <c r="C102" t="s">
+        <v>441</v>
+      </c>
+      <c r="D102" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>442</v>
+      </c>
+      <c r="B103">
+        <v>40229</v>
+      </c>
+      <c r="C103" t="s">
+        <v>439</v>
+      </c>
+      <c r="D103" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>443</v>
+      </c>
+      <c r="B104">
+        <v>37711</v>
+      </c>
+      <c r="C104" t="s">
+        <v>444</v>
+      </c>
+      <c r="D104" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>445</v>
+      </c>
+      <c r="B105">
+        <v>37711</v>
+      </c>
+      <c r="C105" t="s">
+        <v>446</v>
+      </c>
+      <c r="D105" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>447</v>
+      </c>
+      <c r="B106">
+        <v>37711</v>
+      </c>
+      <c r="C106" t="s">
+        <v>448</v>
+      </c>
+      <c r="D106" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>449</v>
+      </c>
+      <c r="B107">
+        <v>41237</v>
+      </c>
+      <c r="C107" t="s">
+        <v>450</v>
+      </c>
+      <c r="D107" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>451</v>
+      </c>
+      <c r="B108">
+        <v>41237</v>
+      </c>
+      <c r="C108" t="s">
+        <v>452</v>
+      </c>
+      <c r="D108" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>453</v>
+      </c>
+      <c r="B109">
+        <v>40705</v>
+      </c>
+      <c r="C109" t="s">
+        <v>454</v>
+      </c>
+      <c r="D109" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>455</v>
+      </c>
+      <c r="B110">
+        <v>40705</v>
+      </c>
+      <c r="C110" t="s">
+        <v>456</v>
+      </c>
+      <c r="D110" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>457</v>
+      </c>
+      <c r="B111">
+        <v>40236</v>
+      </c>
+      <c r="C111" t="s">
+        <v>452</v>
+      </c>
+      <c r="D111" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>458</v>
+      </c>
+      <c r="B112">
+        <v>40236</v>
+      </c>
+      <c r="C112" t="s">
+        <v>459</v>
+      </c>
+      <c r="D112" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>460</v>
+      </c>
+      <c r="B113">
+        <v>40236</v>
+      </c>
+      <c r="C113" t="s">
+        <v>461</v>
+      </c>
+      <c r="D113" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>462</v>
+      </c>
+      <c r="B114">
+        <v>40236</v>
+      </c>
+      <c r="C114" t="s">
+        <v>441</v>
+      </c>
+      <c r="D114" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>463</v>
+      </c>
+      <c r="B115">
+        <v>209</v>
+      </c>
+      <c r="C115" t="s">
+        <v>264</v>
+      </c>
+      <c r="D115" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>464</v>
+      </c>
+      <c r="B116">
+        <v>40976</v>
+      </c>
+      <c r="C116" t="s">
+        <v>465</v>
+      </c>
+      <c r="D116" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>466</v>
+      </c>
+      <c r="B117">
+        <v>39964</v>
+      </c>
+      <c r="C117" t="s">
+        <v>467</v>
+      </c>
+      <c r="D117" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>468</v>
+      </c>
+      <c r="B118">
+        <v>34088</v>
+      </c>
+      <c r="C118" t="s">
+        <v>469</v>
+      </c>
+      <c r="D118" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>470</v>
+      </c>
+      <c r="B119">
+        <v>33936</v>
+      </c>
+      <c r="C119" t="s">
+        <v>471</v>
+      </c>
+      <c r="D119" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>472</v>
+      </c>
+      <c r="B120">
+        <v>413</v>
+      </c>
+      <c r="C120" t="s">
+        <v>316</v>
+      </c>
+      <c r="D120" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>473</v>
+      </c>
+      <c r="B121">
+        <v>6550</v>
+      </c>
+      <c r="C121" t="s">
+        <v>316</v>
+      </c>
+      <c r="D121" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>474</v>
+      </c>
+      <c r="B122">
+        <v>39959</v>
+      </c>
+      <c r="C122" t="s">
+        <v>475</v>
+      </c>
+      <c r="D122" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>476</v>
+      </c>
+      <c r="B123">
+        <v>40865</v>
+      </c>
+      <c r="C123" t="s">
+        <v>477</v>
+      </c>
+      <c r="D123" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>478</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>479</v>
+      </c>
+      <c r="D124" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1596,7 +4218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0256B6-CC9F-DA43-B2FC-ADA39BBB9055}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -2476,7 +5098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
Start review of typological fields
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5066CAAD-ACCC-CD45-9226-E9C20013DDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F40C4-A100-C74F-9DC0-946FCC9C0B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24820" yWindow="2460" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="550">
   <si>
     <t>collection</t>
   </si>
@@ -1645,6 +1645,63 @@
   </si>
   <si>
     <t>http://numismatics.org/ocre/id/ric.10.lib_sev_w.2717</t>
+  </si>
+  <si>
+    <t>general_field_name</t>
+  </si>
+  <si>
+    <t>general_field_name_count</t>
+  </si>
+  <si>
+    <t>transformation</t>
+  </si>
+  <si>
+    <t>target_field_name</t>
+  </si>
+  <si>
+    <t>target_field_type</t>
+  </si>
+  <si>
+    <t>coin_date_range</t>
+  </si>
+  <si>
+    <t>denomination</t>
+  </si>
+  <si>
+    <t>VARCHAR[]</t>
+  </si>
+  <si>
+    <t>manufacture</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>object_type</t>
+  </si>
+  <si>
+    <t>if field in ("_date", "_date_range", "date_on_object_date"):
+   field = "coin_date_range"</t>
+  </si>
+  <si>
+    <t>if value.lower() == "medalian":
+   # do not add medalian object type to database
+   continue</t>
+  </si>
+  <si>
+    <t>authority_name</t>
+  </si>
+  <si>
+    <t>issuer_name</t>
+  </si>
+  <si>
+    <t>stated_authority_name</t>
+  </si>
+  <si>
+    <t>mint</t>
+  </si>
+  <si>
+    <t>region</t>
   </si>
 </sst>
 </file>
@@ -1720,7 +1777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1748,12 +1805,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1837,13 +1929,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:D124" totalsRowShown="0">
-  <autoFilter ref="A1:D124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="8">
+      <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="7">
+      <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1868,7 +1969,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="21">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -1879,23 +1980,23 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="20">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="18">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2287,1757 +2388,3277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ECEDEA-565B-2645-A3E1-F668D8278F57}">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>182</v>
       </c>
       <c r="B1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E1" t="s">
+        <v>535</v>
+      </c>
+      <c r="F1" t="s">
+        <v>536</v>
+      </c>
+      <c r="G1" t="s">
         <v>480</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>481</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_date</v>
+      </c>
+      <c r="C2" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="4">
         <v>84</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" s="4" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_date_range</v>
+      </c>
+      <c r="C3" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_denomination</v>
+      </c>
+      <c r="C4" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_denomination</v>
+      </c>
+      <c r="C5" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G5" s="4">
         <v>38964</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_manufacture</v>
+      </c>
+      <c r="C6" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="D6" t="s">
+      <c r="I6" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_material</v>
+      </c>
+      <c r="C7" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="D7" t="s">
+      <c r="I7" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_material</v>
+      </c>
+      <c r="C8" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G8" s="4">
         <v>37842</v>
       </c>
-      <c r="C8" t="s">
+      <c r="H8" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="D8" t="s">
+      <c r="I8" s="4" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_object_type</v>
+      </c>
+      <c r="C9" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="D9" t="s">
+      <c r="I9" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>_object_type</v>
+      </c>
+      <c r="C10" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G10" s="4">
         <v>7820</v>
       </c>
-      <c r="C10" t="s">
+      <c r="H10" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="D10" t="s">
+      <c r="I10" s="4" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_authority</v>
+      </c>
+      <c r="C11" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_authority</v>
+      </c>
+      <c r="C12" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G12" s="4">
         <v>40202</v>
       </c>
-      <c r="C12" t="s">
+      <c r="H12" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D12" t="s">
+      <c r="I12" s="4" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_issuer</v>
+      </c>
+      <c r="C13" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D13" t="s">
+      <c r="I13" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_issuer</v>
+      </c>
+      <c r="C14" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G14" s="4">
         <v>541</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D14" t="s">
+      <c r="I14" s="4" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_issuer</v>
+      </c>
+      <c r="C15" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G15" s="4">
         <v>541</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D15" t="s">
+      <c r="I15" s="4" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_issuer</v>
+      </c>
+      <c r="C16" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G16" s="4">
         <v>541</v>
       </c>
-      <c r="C16" t="s">
+      <c r="H16" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="D16" t="s">
+      <c r="I16" s="4" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_stated_authority</v>
+      </c>
+      <c r="C17" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="4">
         <v>41163</v>
       </c>
-      <c r="C17" t="s">
+      <c r="H17" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D17" t="s">
+      <c r="I17" s="4" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>date_on_object_date</v>
+      </c>
+      <c r="C18" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G18" s="4">
         <v>24728</v>
       </c>
-      <c r="C18" t="s">
+      <c r="H18" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D18" t="s">
+      <c r="I18" s="4" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_mint</v>
+      </c>
+      <c r="C19" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="D19" t="s">
+      <c r="I19" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_mint</v>
+      </c>
+      <c r="C20" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G20" s="4">
         <v>40646</v>
       </c>
-      <c r="C20" t="s">
+      <c r="H20" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D20" t="s">
+      <c r="I20" s="4" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_mint</v>
+      </c>
+      <c r="C21" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G21" s="4">
         <v>21341</v>
       </c>
-      <c r="C21" t="s">
+      <c r="H21" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D21" t="s">
+      <c r="I21" s="4" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_mint</v>
+      </c>
+      <c r="C22" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G22" s="4">
         <v>21306</v>
       </c>
-      <c r="C22" t="s">
+      <c r="H22" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="D22" t="s">
+      <c r="I22" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_mint</v>
+      </c>
+      <c r="C23" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G23" s="4">
         <v>21306</v>
       </c>
-      <c r="C23" t="s">
+      <c r="H23" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D23" t="s">
+      <c r="I23" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_region</v>
+      </c>
+      <c r="C24" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D24" t="s">
+      <c r="I24" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_region</v>
+      </c>
+      <c r="C25" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G25" s="4">
         <v>21527</v>
       </c>
-      <c r="C25" t="s">
+      <c r="H25" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="D25" t="s">
+      <c r="I25" s="4" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_region</v>
+      </c>
+      <c r="C26" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G26" s="4">
         <v>21306</v>
       </c>
-      <c r="C26" t="s">
+      <c r="H26" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="D26" t="s">
+      <c r="I26" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>geographic_region</v>
+      </c>
+      <c r="C27" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>4</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G27" s="4">
         <v>21306</v>
       </c>
-      <c r="C27" t="s">
+      <c r="H27" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="D27" t="s">
+      <c r="I27" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_controlmark</v>
+      </c>
+      <c r="C28" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_controlmark</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" s="4">
         <v>18819</v>
       </c>
-      <c r="C28" t="s">
+      <c r="H28" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="D28" t="s">
+      <c r="I28" s="4" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C29" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G29" s="4">
         <v>323</v>
       </c>
-      <c r="C29" t="s">
+      <c r="H29" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D29" t="s">
+      <c r="I29" s="4" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C30" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G30" s="4">
         <v>27853</v>
       </c>
-      <c r="C30" t="s">
+      <c r="H30" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D30" t="s">
+      <c r="I30" s="4" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C31" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G31" s="4">
         <v>696</v>
       </c>
-      <c r="C31" t="s">
+      <c r="H31" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D31" t="s">
+      <c r="I31" s="4" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C32" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G32" s="4">
         <v>696</v>
       </c>
-      <c r="C32" t="s">
+      <c r="H32" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="D32" t="s">
+      <c r="I32" s="4" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C33" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G33" s="4">
         <v>696</v>
       </c>
-      <c r="C33" t="s">
+      <c r="H33" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="D33" t="s">
+      <c r="I33" s="4" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_deity</v>
+      </c>
+      <c r="C34" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>6</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G34" s="4">
         <v>696</v>
       </c>
-      <c r="C34" t="s">
+      <c r="H34" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="D34" t="s">
+      <c r="I34" s="4" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_legend</v>
+      </c>
+      <c r="C35" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="D35" t="s">
+      <c r="I35" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_portrait</v>
+      </c>
+      <c r="C36" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D36" t="s">
+      <c r="I36" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_portrait</v>
+      </c>
+      <c r="C37" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4">
         <v>40202</v>
       </c>
-      <c r="C37" t="s">
+      <c r="H37" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D37" t="s">
+      <c r="I37" s="4" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_state</v>
+      </c>
+      <c r="C38" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4">
         <v>6546</v>
       </c>
-      <c r="C38" t="s">
+      <c r="H38" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D38" t="s">
+      <c r="I38" s="4" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_state</v>
+      </c>
+      <c r="C39" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4">
         <v>6564</v>
       </c>
-      <c r="C39" t="s">
+      <c r="H39" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D39" t="s">
+      <c r="I39" s="4" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>obverse_type</v>
+      </c>
+      <c r="C40" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="D40" t="s">
+      <c r="I40" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_control_marks</v>
+      </c>
+      <c r="C41" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4">
         <v>18487</v>
       </c>
-      <c r="C41" t="s">
+      <c r="H41" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D41" t="s">
+      <c r="I41" s="4" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_deity</v>
+      </c>
+      <c r="C42" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="D42" t="s">
+      <c r="I42" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_deity</v>
+      </c>
+      <c r="C43" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4">
         <v>40418</v>
       </c>
-      <c r="C43" t="s">
+      <c r="H43" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D43" t="s">
+      <c r="I43" s="4" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_deity</v>
+      </c>
+      <c r="C44" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4">
         <v>39519</v>
       </c>
-      <c r="C44" t="s">
+      <c r="H44" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D44" t="s">
+      <c r="I44" s="4" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_deity</v>
+      </c>
+      <c r="C45" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4">
         <v>16073</v>
       </c>
-      <c r="C45" t="s">
+      <c r="H45" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="D45" t="s">
+      <c r="I45" s="4" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_deity</v>
+      </c>
+      <c r="C46" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4">
         <v>11115</v>
       </c>
-      <c r="C46" t="s">
+      <c r="H46" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D46" t="s">
+      <c r="I46" s="4" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_dynasty</v>
+      </c>
+      <c r="C47" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4">
         <v>783</v>
       </c>
-      <c r="C47" t="s">
+      <c r="H47" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D47" t="s">
+      <c r="I47" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B48" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_legend</v>
+      </c>
+      <c r="C48" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D48" t="s">
+      <c r="I48" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C49" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4">
         <v>20948</v>
       </c>
-      <c r="C49" t="s">
+      <c r="H49" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D49" t="s">
+      <c r="I49" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C50" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4">
         <v>25291</v>
       </c>
-      <c r="C50" t="s">
+      <c r="H50" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="D50" t="s">
+      <c r="I50" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C51" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4">
         <v>25291</v>
       </c>
-      <c r="C51" t="s">
+      <c r="H51" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D51" t="s">
+      <c r="I51" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C52" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4">
         <v>25291</v>
       </c>
-      <c r="C52" t="s">
+      <c r="H52" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="D52" t="s">
+      <c r="I52" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C53" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4">
         <v>25271</v>
       </c>
-      <c r="C53" t="s">
+      <c r="H53" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="D53" t="s">
+      <c r="I53" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C54" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4">
         <v>25271</v>
       </c>
-      <c r="C54" t="s">
+      <c r="H54" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D54" t="s">
+      <c r="I54" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C55" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4">
         <v>25271</v>
       </c>
-      <c r="C55" t="s">
+      <c r="H55" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="D55" t="s">
+      <c r="I55" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C56" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4">
         <v>25271</v>
       </c>
-      <c r="C56" t="s">
+      <c r="H56" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="D56" t="s">
+      <c r="I56" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C57" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4">
         <v>25271</v>
       </c>
-      <c r="C57" t="s">
+      <c r="H57" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D57" t="s">
+      <c r="I57" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C58" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4">
         <v>25271</v>
       </c>
-      <c r="C58" t="s">
+      <c r="H58" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="D58" t="s">
+      <c r="I58" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C59" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4">
         <v>25271</v>
       </c>
-      <c r="C59" t="s">
+      <c r="H59" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="D59" t="s">
+      <c r="I59" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C60" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4">
         <v>34019</v>
       </c>
-      <c r="C60" t="s">
+      <c r="H60" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="D60" t="s">
+      <c r="I60" s="4" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C61" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4">
         <v>25271</v>
       </c>
-      <c r="C61" t="s">
+      <c r="H61" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="D61" t="s">
+      <c r="I61" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C62" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4">
         <v>25271</v>
       </c>
-      <c r="C62" t="s">
+      <c r="H62" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D62" t="s">
+      <c r="I62" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C63" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4">
         <v>25271</v>
       </c>
-      <c r="C63" t="s">
+      <c r="H63" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D63" t="s">
+      <c r="I63" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C64" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4">
         <v>23923</v>
       </c>
-      <c r="C64" t="s">
+      <c r="H64" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="D64" t="s">
+      <c r="I64" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C65" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4">
         <v>23923</v>
       </c>
-      <c r="C65" t="s">
+      <c r="H65" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="D65" t="s">
+      <c r="I65" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C66" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4">
         <v>23923</v>
       </c>
-      <c r="C66" t="s">
+      <c r="H66" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="D66" t="s">
+      <c r="I66" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C67" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4">
         <v>23923</v>
       </c>
-      <c r="C67" t="s">
+      <c r="H67" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D67" t="s">
+      <c r="I67" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C68" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4">
         <v>23923</v>
       </c>
-      <c r="C68" t="s">
+      <c r="H68" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="D68" t="s">
+      <c r="I68" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C69" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4">
         <v>23923</v>
       </c>
-      <c r="C69" t="s">
+      <c r="H69" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D69" t="s">
+      <c r="I69" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C70" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4">
         <v>23923</v>
       </c>
-      <c r="C70" t="s">
+      <c r="H70" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D70" t="s">
+      <c r="I70" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C71" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4">
         <v>34010</v>
       </c>
-      <c r="C71" t="s">
+      <c r="H71" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="D71" t="s">
+      <c r="I71" s="4" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C72" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4">
         <v>23923</v>
       </c>
-      <c r="C72" t="s">
+      <c r="H72" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="D72" t="s">
+      <c r="I72" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C73" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4">
         <v>23923</v>
       </c>
-      <c r="C73" t="s">
+      <c r="H73" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="D73" t="s">
+      <c r="I73" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C74" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4">
         <v>23923</v>
       </c>
-      <c r="C74" t="s">
+      <c r="H74" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="D74" t="s">
+      <c r="I74" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C75" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4">
         <v>23923</v>
       </c>
-      <c r="C75" t="s">
+      <c r="H75" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="D75" t="s">
+      <c r="I75" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C76" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4">
         <v>23923</v>
       </c>
-      <c r="C76" t="s">
+      <c r="H76" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="D76" t="s">
+      <c r="I76" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C77" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4">
         <v>23923</v>
       </c>
-      <c r="C77" t="s">
+      <c r="H77" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="D77" t="s">
+      <c r="I77" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C78" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4">
         <v>23923</v>
       </c>
-      <c r="C78" t="s">
+      <c r="H78" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="D78" t="s">
+      <c r="I78" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C79" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4">
         <v>23923</v>
       </c>
-      <c r="C79" t="s">
+      <c r="H79" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="D79" t="s">
+      <c r="I79" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C80" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4">
         <v>23923</v>
       </c>
-      <c r="C80" t="s">
+      <c r="H80" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="D80" t="s">
+      <c r="I80" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C81" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4">
         <v>23923</v>
       </c>
-      <c r="C81" t="s">
+      <c r="H81" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="D81" t="s">
+      <c r="I81" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C82" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4">
         <v>29419</v>
       </c>
-      <c r="C82" t="s">
+      <c r="H82" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="D82" t="s">
+      <c r="I82" s="4" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C83" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4">
         <v>23923</v>
       </c>
-      <c r="C83" t="s">
+      <c r="H83" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="D83" t="s">
+      <c r="I83" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C84" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4">
         <v>23923</v>
       </c>
-      <c r="C84" t="s">
+      <c r="H84" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="D84" t="s">
+      <c r="I84" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C85" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4">
         <v>23923</v>
       </c>
-      <c r="C85" t="s">
+      <c r="H85" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="D85" t="s">
+      <c r="I85" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C86" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4">
         <v>23923</v>
       </c>
-      <c r="C86" t="s">
+      <c r="H86" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="D86" t="s">
+      <c r="I86" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C87" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4">
         <v>23923</v>
       </c>
-      <c r="C87" t="s">
+      <c r="H87" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="D87" t="s">
+      <c r="I87" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C88" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4">
         <v>23923</v>
       </c>
-      <c r="C88" t="s">
+      <c r="H88" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D88" t="s">
+      <c r="I88" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C89" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4">
         <v>23923</v>
       </c>
-      <c r="C89" t="s">
+      <c r="H89" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="D89" t="s">
+      <c r="I89" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C90" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4">
         <v>21669</v>
       </c>
-      <c r="C90" t="s">
+      <c r="H90" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="D90" t="s">
+      <c r="I90" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C91" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4">
         <v>21669</v>
       </c>
-      <c r="C91" t="s">
+      <c r="H91" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="D91" t="s">
+      <c r="I91" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C92" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4">
         <v>21669</v>
       </c>
-      <c r="C92" t="s">
+      <c r="H92" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="D92" t="s">
+      <c r="I92" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C93" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4">
         <v>26506</v>
       </c>
-      <c r="C93" t="s">
+      <c r="H93" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="D93" t="s">
+      <c r="I93" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C94" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4">
         <v>21669</v>
       </c>
-      <c r="C94" t="s">
+      <c r="H94" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="D94" t="s">
+      <c r="I94" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C95" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4">
         <v>26506</v>
       </c>
-      <c r="C95" t="s">
+      <c r="H95" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="D95" t="s">
+      <c r="I95" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C96" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4">
         <v>26506</v>
       </c>
-      <c r="C96" t="s">
+      <c r="H96" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="D96" t="s">
+      <c r="I96" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C97" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4">
         <v>25291</v>
       </c>
-      <c r="C97" t="s">
+      <c r="H97" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="D97" t="s">
+      <c r="I97" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_mintmark</v>
+      </c>
+      <c r="C98" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>50</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4">
         <v>25291</v>
       </c>
-      <c r="C98" t="s">
+      <c r="H98" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D98" t="s">
+      <c r="I98" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_monogram</v>
+      </c>
+      <c r="C99" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4">
         <v>40260</v>
       </c>
-      <c r="C99" t="s">
+      <c r="H99" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="D99" t="s">
+      <c r="I99" s="4" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C100" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4">
         <v>22083</v>
       </c>
-      <c r="C100" t="s">
+      <c r="H100" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="D100" t="s">
+      <c r="I100" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C101" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4">
         <v>40236</v>
       </c>
-      <c r="C101" t="s">
+      <c r="H101" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="D101" t="s">
+      <c r="I101" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C102" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4">
         <v>40229</v>
       </c>
-      <c r="C102" t="s">
+      <c r="H102" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="D102" t="s">
+      <c r="I102" s="4" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C103" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4">
         <v>40229</v>
       </c>
-      <c r="C103" t="s">
+      <c r="H103" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="D103" t="s">
+      <c r="I103" s="4" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C104" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4">
         <v>37711</v>
       </c>
-      <c r="C104" t="s">
+      <c r="H104" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="D104" t="s">
+      <c r="I104" s="4" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C105" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4">
         <v>37711</v>
       </c>
-      <c r="C105" t="s">
+      <c r="H105" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="D105" t="s">
+      <c r="I105" s="4" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C106" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4">
         <v>37711</v>
       </c>
-      <c r="C106" t="s">
+      <c r="H106" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="D106" t="s">
+      <c r="I106" s="4" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C107" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4">
         <v>41237</v>
       </c>
-      <c r="C107" t="s">
+      <c r="H107" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="D107" t="s">
+      <c r="I107" s="4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C108" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4">
         <v>41237</v>
       </c>
-      <c r="C108" t="s">
+      <c r="H108" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="D108" t="s">
+      <c r="I108" s="4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C109" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4">
         <v>40705</v>
       </c>
-      <c r="C109" t="s">
+      <c r="H109" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="D109" t="s">
+      <c r="I109" s="4" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C110" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4">
         <v>40705</v>
       </c>
-      <c r="C110" t="s">
+      <c r="H110" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="D110" t="s">
+      <c r="I110" s="4" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C111" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4">
         <v>40236</v>
       </c>
-      <c r="C111" t="s">
+      <c r="H111" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="D111" t="s">
+      <c r="I111" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C112" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4">
         <v>40236</v>
       </c>
-      <c r="C112" t="s">
+      <c r="H112" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="D112" t="s">
+      <c r="I112" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C113" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4">
         <v>40236</v>
       </c>
-      <c r="C113" t="s">
+      <c r="H113" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="D113" t="s">
+      <c r="I113" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_officinamark</v>
+      </c>
+      <c r="C114" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>15</v>
+      </c>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4">
         <v>40236</v>
       </c>
-      <c r="C114" t="s">
+      <c r="H114" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="D114" t="s">
+      <c r="I114" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_portrait</v>
+      </c>
+      <c r="C115" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4">
         <v>209</v>
       </c>
-      <c r="C115" t="s">
+      <c r="H115" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D115" t="s">
+      <c r="I115" s="4" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_portrait</v>
+      </c>
+      <c r="C116" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4">
         <v>40976</v>
       </c>
-      <c r="C116" t="s">
+      <c r="H116" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D116" t="s">
+      <c r="I116" s="4" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_portrait</v>
+      </c>
+      <c r="C117" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4">
         <v>39964</v>
       </c>
-      <c r="C117" t="s">
+      <c r="H117" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D117" t="s">
+      <c r="I117" s="4" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_portrait</v>
+      </c>
+      <c r="C118" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4">
         <v>34088</v>
       </c>
-      <c r="C118" t="s">
+      <c r="H118" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="D118" t="s">
+      <c r="I118" s="4" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_portrait</v>
+      </c>
+      <c r="C119" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>5</v>
+      </c>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4">
         <v>33936</v>
       </c>
-      <c r="C119" t="s">
+      <c r="H119" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="D119" t="s">
+      <c r="I119" s="4" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_state</v>
+      </c>
+      <c r="C120" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4">
         <v>413</v>
       </c>
-      <c r="C120" t="s">
+      <c r="H120" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D120" t="s">
+      <c r="I120" s="4" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_state</v>
+      </c>
+      <c r="C121" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4">
         <v>6550</v>
       </c>
-      <c r="C121" t="s">
+      <c r="H121" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D121" t="s">
+      <c r="I121" s="4" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_symbol</v>
+      </c>
+      <c r="C122" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4">
         <v>39959</v>
       </c>
-      <c r="C122" t="s">
+      <c r="H122" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D122" t="s">
+      <c r="I122" s="4" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_symbol</v>
+      </c>
+      <c r="C123" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>2</v>
+      </c>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4">
         <v>40865</v>
       </c>
-      <c r="C123" t="s">
+      <c r="H123" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D123" t="s">
+      <c r="I123" s="4" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="B124">
-        <v>1</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="B124" s="4" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>reverse_type</v>
+      </c>
+      <c r="C124" s="4">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4">
+        <v>1</v>
+      </c>
+      <c r="H124" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="D124" t="s">
+      <c r="I124" s="4" t="s">
         <v>192</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Finish review of typological fields
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F40C4-A100-C74F-9DC0-946FCC9C0B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9D50F-7532-5E46-B15B-D4D4E6A79E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-25160" yWindow="1480" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -40,8 +40,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={86CF3DBB-3F7B-394B-AE87-6F3ACE1106E1}</author>
+    <author>tc={E5C103C6-CA70-6D4A-B5CA-9DB44C052FDF}</author>
+    <author>tc={4804A6C7-DC03-A14D-9A76-EC3E30F27E82}</author>
+    <author>tc={3B86C5CF-579A-9B44-92B9-DE570572C285}</author>
+  </authors>
+  <commentList>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{86CF3DBB-3F7B-394B-AE87-6F3ACE1106E1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="1" shapeId="0" xr:uid="{E5C103C6-CA70-6D4A-B5CA-9DB44C052FDF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="F48" authorId="2" shapeId="0" xr:uid="{4804A6C7-DC03-A14D-9A76-EC3E30F27E82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="F124" authorId="3" shapeId="0" xr:uid="{3B86C5CF-579A-9B44-92B9-DE570572C285}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="551">
   <si>
     <t>collection</t>
   </si>
@@ -1703,12 +1748,15 @@
   <si>
     <t>region</t>
   </si>
+  <si>
+    <t>TEXT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1737,6 +1785,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1833,6 +1887,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1840,7 +1895,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1862,7 +1916,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1871,10 +1928,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1915,6 +1969,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jamal Hamadeh" id="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" userId="a925bebb50509816" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B83FD7C4-BC5E-964C-B461-DC52D3B69E7A}" name="Table4" displayName="Table4" ref="A1:D5" totalsRowCount="1">
   <autoFilter ref="A1:D4" xr:uid="{B83FD7C4-BC5E-964C-B461-DC52D3B69E7A}"/>
@@ -1929,22 +1989,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="7">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="6">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1983,13 +2043,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="20">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="16">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="15">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="14"/>
@@ -2297,6 +2357,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F35" dT="2023-07-19T02:59:44.18" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{86CF3DBB-3F7B-394B-AE87-6F3ACE1106E1}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="F40" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{E5C103C6-CA70-6D4A-B5CA-9DB44C052FDF}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="F48" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{4804A6C7-DC03-A14D-9A76-EC3E30F27E82}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="F124" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{3B86C5CF-579A-9B44-92B9-DE570572C285}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDD5D45-1DCC-E44B-8D59-8507F8236A7D}">
   <dimension ref="A1:D5"/>
@@ -2387,14 +2464,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ECEDEA-565B-2645-A3E1-F668D8278F57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ECEDEA-565B-2645-A3E1-F668D8278F57}">
   <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3408,27 +3485,31 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B35" s="4" t="str">
+      <c r="B35" s="8" t="str">
         <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
         <v>obverse_legend</v>
       </c>
-      <c r="C35" s="4">
-        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4" t="s">
+      <c r="C35" s="8">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="8" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3445,8 +3526,12 @@
         <v>2</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G36" s="4">
         <v>1</v>
       </c>
@@ -3470,8 +3555,12 @@
         <v>2</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G37" s="4">
         <v>40202</v>
       </c>
@@ -3495,8 +3584,12 @@
         <v>2</v>
       </c>
       <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G38" s="4">
         <v>6546</v>
       </c>
@@ -3520,8 +3613,12 @@
         <v>2</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G39" s="4">
         <v>6564</v>
       </c>
@@ -3533,27 +3630,31 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="B40" s="4" t="str">
+      <c r="B40" s="8" t="str">
         <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
         <v>obverse_type</v>
       </c>
-      <c r="C40" s="4">
-        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
-        <v>1</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4" t="s">
+      <c r="C40" s="8">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G40" s="8">
+        <v>1</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="8" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3570,8 +3671,12 @@
         <v>1</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G41" s="4">
         <v>18487</v>
       </c>
@@ -3595,8 +3700,12 @@
         <v>5</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G42" s="4">
         <v>1</v>
       </c>
@@ -3620,8 +3729,12 @@
         <v>5</v>
       </c>
       <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G43" s="4">
         <v>40418</v>
       </c>
@@ -3645,8 +3758,12 @@
         <v>5</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G44" s="4">
         <v>39519</v>
       </c>
@@ -3670,8 +3787,12 @@
         <v>5</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G45" s="4">
         <v>16073</v>
       </c>
@@ -3695,8 +3816,12 @@
         <v>5</v>
       </c>
       <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G46" s="4">
         <v>11115</v>
       </c>
@@ -3720,8 +3845,12 @@
         <v>1</v>
       </c>
       <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G47" s="4">
         <v>783</v>
       </c>
@@ -3733,27 +3862,31 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="B48" s="4" t="str">
+      <c r="B48" s="8" t="str">
         <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
         <v>reverse_legend</v>
       </c>
-      <c r="C48" s="4">
-        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
-        <v>1</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4" t="s">
+      <c r="C48" s="8">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G48" s="8">
+        <v>1</v>
+      </c>
+      <c r="H48" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" s="8" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3770,8 +3903,12 @@
         <v>50</v>
       </c>
       <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G49" s="4">
         <v>20948</v>
       </c>
@@ -3795,8 +3932,12 @@
         <v>50</v>
       </c>
       <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G50" s="4">
         <v>25291</v>
       </c>
@@ -3820,8 +3961,12 @@
         <v>50</v>
       </c>
       <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G51" s="4">
         <v>25291</v>
       </c>
@@ -3845,8 +3990,12 @@
         <v>50</v>
       </c>
       <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G52" s="4">
         <v>25291</v>
       </c>
@@ -3870,8 +4019,12 @@
         <v>50</v>
       </c>
       <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G53" s="4">
         <v>25271</v>
       </c>
@@ -3895,8 +4048,12 @@
         <v>50</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G54" s="4">
         <v>25271</v>
       </c>
@@ -3920,8 +4077,12 @@
         <v>50</v>
       </c>
       <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G55" s="4">
         <v>25271</v>
       </c>
@@ -3945,8 +4106,12 @@
         <v>50</v>
       </c>
       <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G56" s="4">
         <v>25271</v>
       </c>
@@ -3970,8 +4135,12 @@
         <v>50</v>
       </c>
       <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G57" s="4">
         <v>25271</v>
       </c>
@@ -3995,8 +4164,12 @@
         <v>50</v>
       </c>
       <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G58" s="4">
         <v>25271</v>
       </c>
@@ -4020,8 +4193,12 @@
         <v>50</v>
       </c>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G59" s="4">
         <v>25271</v>
       </c>
@@ -4045,8 +4222,12 @@
         <v>50</v>
       </c>
       <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
+      <c r="E60" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G60" s="4">
         <v>34019</v>
       </c>
@@ -4070,8 +4251,12 @@
         <v>50</v>
       </c>
       <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
+      <c r="E61" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G61" s="4">
         <v>25271</v>
       </c>
@@ -4095,8 +4280,12 @@
         <v>50</v>
       </c>
       <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G62" s="4">
         <v>25271</v>
       </c>
@@ -4120,8 +4309,12 @@
         <v>50</v>
       </c>
       <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G63" s="4">
         <v>25271</v>
       </c>
@@ -4145,8 +4338,12 @@
         <v>50</v>
       </c>
       <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G64" s="4">
         <v>23923</v>
       </c>
@@ -4170,8 +4367,12 @@
         <v>50</v>
       </c>
       <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G65" s="4">
         <v>23923</v>
       </c>
@@ -4195,8 +4396,12 @@
         <v>50</v>
       </c>
       <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G66" s="4">
         <v>23923</v>
       </c>
@@ -4220,8 +4425,12 @@
         <v>50</v>
       </c>
       <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G67" s="4">
         <v>23923</v>
       </c>
@@ -4245,8 +4454,12 @@
         <v>50</v>
       </c>
       <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G68" s="4">
         <v>23923</v>
       </c>
@@ -4270,8 +4483,12 @@
         <v>50</v>
       </c>
       <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
+      <c r="E69" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G69" s="4">
         <v>23923</v>
       </c>
@@ -4295,8 +4512,12 @@
         <v>50</v>
       </c>
       <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G70" s="4">
         <v>23923</v>
       </c>
@@ -4320,8 +4541,12 @@
         <v>50</v>
       </c>
       <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G71" s="4">
         <v>34010</v>
       </c>
@@ -4345,8 +4570,12 @@
         <v>50</v>
       </c>
       <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+      <c r="E72" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G72" s="4">
         <v>23923</v>
       </c>
@@ -4370,8 +4599,12 @@
         <v>50</v>
       </c>
       <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G73" s="4">
         <v>23923</v>
       </c>
@@ -4395,8 +4628,12 @@
         <v>50</v>
       </c>
       <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G74" s="4">
         <v>23923</v>
       </c>
@@ -4420,8 +4657,12 @@
         <v>50</v>
       </c>
       <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G75" s="4">
         <v>23923</v>
       </c>
@@ -4445,8 +4686,12 @@
         <v>50</v>
       </c>
       <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G76" s="4">
         <v>23923</v>
       </c>
@@ -4470,8 +4715,12 @@
         <v>50</v>
       </c>
       <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G77" s="4">
         <v>23923</v>
       </c>
@@ -4495,8 +4744,12 @@
         <v>50</v>
       </c>
       <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G78" s="4">
         <v>23923</v>
       </c>
@@ -4520,8 +4773,12 @@
         <v>50</v>
       </c>
       <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G79" s="4">
         <v>23923</v>
       </c>
@@ -4545,8 +4802,12 @@
         <v>50</v>
       </c>
       <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G80" s="4">
         <v>23923</v>
       </c>
@@ -4570,8 +4831,12 @@
         <v>50</v>
       </c>
       <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
+      <c r="E81" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G81" s="4">
         <v>23923</v>
       </c>
@@ -4595,8 +4860,12 @@
         <v>50</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
+      <c r="E82" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G82" s="4">
         <v>29419</v>
       </c>
@@ -4620,8 +4889,12 @@
         <v>50</v>
       </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G83" s="4">
         <v>23923</v>
       </c>
@@ -4645,8 +4918,12 @@
         <v>50</v>
       </c>
       <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
+      <c r="E84" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G84" s="4">
         <v>23923</v>
       </c>
@@ -4670,8 +4947,12 @@
         <v>50</v>
       </c>
       <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
+      <c r="E85" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G85" s="4">
         <v>23923</v>
       </c>
@@ -4695,8 +4976,12 @@
         <v>50</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G86" s="4">
         <v>23923</v>
       </c>
@@ -4720,8 +5005,12 @@
         <v>50</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G87" s="4">
         <v>23923</v>
       </c>
@@ -4745,8 +5034,12 @@
         <v>50</v>
       </c>
       <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
+      <c r="E88" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G88" s="4">
         <v>23923</v>
       </c>
@@ -4770,8 +5063,12 @@
         <v>50</v>
       </c>
       <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G89" s="4">
         <v>23923</v>
       </c>
@@ -4795,8 +5092,12 @@
         <v>50</v>
       </c>
       <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
+      <c r="E90" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G90" s="4">
         <v>21669</v>
       </c>
@@ -4820,8 +5121,12 @@
         <v>50</v>
       </c>
       <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
+      <c r="E91" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G91" s="4">
         <v>21669</v>
       </c>
@@ -4845,8 +5150,12 @@
         <v>50</v>
       </c>
       <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
+      <c r="E92" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G92" s="4">
         <v>21669</v>
       </c>
@@ -4870,8 +5179,12 @@
         <v>50</v>
       </c>
       <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
+      <c r="E93" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G93" s="4">
         <v>26506</v>
       </c>
@@ -4895,8 +5208,12 @@
         <v>50</v>
       </c>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G94" s="4">
         <v>21669</v>
       </c>
@@ -4920,8 +5237,12 @@
         <v>50</v>
       </c>
       <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
+      <c r="E95" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G95" s="4">
         <v>26506</v>
       </c>
@@ -4945,8 +5266,12 @@
         <v>50</v>
       </c>
       <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
+      <c r="E96" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G96" s="4">
         <v>26506</v>
       </c>
@@ -4970,8 +5295,12 @@
         <v>50</v>
       </c>
       <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G97" s="4">
         <v>25291</v>
       </c>
@@ -4995,8 +5324,12 @@
         <v>50</v>
       </c>
       <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G98" s="4">
         <v>25291</v>
       </c>
@@ -5020,8 +5353,12 @@
         <v>1</v>
       </c>
       <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
+      <c r="E99" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="G99" s="4">
         <v>40260</v>
       </c>
@@ -5045,8 +5382,12 @@
         <v>15</v>
       </c>
       <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
+      <c r="E100" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G100" s="4">
         <v>22083</v>
       </c>
@@ -5070,8 +5411,12 @@
         <v>15</v>
       </c>
       <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
+      <c r="E101" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G101" s="4">
         <v>40236</v>
       </c>
@@ -5095,8 +5440,12 @@
         <v>15</v>
       </c>
       <c r="D102" s="4"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
+      <c r="E102" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G102" s="4">
         <v>40229</v>
       </c>
@@ -5120,8 +5469,12 @@
         <v>15</v>
       </c>
       <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
+      <c r="E103" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G103" s="4">
         <v>40229</v>
       </c>
@@ -5145,8 +5498,12 @@
         <v>15</v>
       </c>
       <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
+      <c r="E104" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G104" s="4">
         <v>37711</v>
       </c>
@@ -5170,8 +5527,12 @@
         <v>15</v>
       </c>
       <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
+      <c r="E105" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G105" s="4">
         <v>37711</v>
       </c>
@@ -5195,8 +5556,12 @@
         <v>15</v>
       </c>
       <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
+      <c r="E106" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G106" s="4">
         <v>37711</v>
       </c>
@@ -5220,8 +5585,12 @@
         <v>15</v>
       </c>
       <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G107" s="4">
         <v>41237</v>
       </c>
@@ -5245,8 +5614,12 @@
         <v>15</v>
       </c>
       <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
+      <c r="E108" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G108" s="4">
         <v>41237</v>
       </c>
@@ -5270,8 +5643,12 @@
         <v>15</v>
       </c>
       <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
+      <c r="E109" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G109" s="4">
         <v>40705</v>
       </c>
@@ -5295,8 +5672,12 @@
         <v>15</v>
       </c>
       <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G110" s="4">
         <v>40705</v>
       </c>
@@ -5320,8 +5701,12 @@
         <v>15</v>
       </c>
       <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G111" s="4">
         <v>40236</v>
       </c>
@@ -5345,8 +5730,12 @@
         <v>15</v>
       </c>
       <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
+      <c r="E112" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G112" s="4">
         <v>40236</v>
       </c>
@@ -5370,8 +5759,12 @@
         <v>15</v>
       </c>
       <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
+      <c r="E113" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G113" s="4">
         <v>40236</v>
       </c>
@@ -5395,8 +5788,12 @@
         <v>15</v>
       </c>
       <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
+      <c r="E114" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G114" s="4">
         <v>40236</v>
       </c>
@@ -5420,8 +5817,12 @@
         <v>5</v>
       </c>
       <c r="D115" s="4"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G115" s="4">
         <v>209</v>
       </c>
@@ -5445,8 +5846,12 @@
         <v>5</v>
       </c>
       <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
+      <c r="E116" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G116" s="4">
         <v>40976</v>
       </c>
@@ -5470,8 +5875,12 @@
         <v>5</v>
       </c>
       <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
+      <c r="E117" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G117" s="4">
         <v>39964</v>
       </c>
@@ -5495,8 +5904,12 @@
         <v>5</v>
       </c>
       <c r="D118" s="4"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
+      <c r="E118" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G118" s="4">
         <v>34088</v>
       </c>
@@ -5520,8 +5933,12 @@
         <v>5</v>
       </c>
       <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G119" s="4">
         <v>33936</v>
       </c>
@@ -5545,8 +5962,12 @@
         <v>2</v>
       </c>
       <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
+      <c r="E120" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G120" s="4">
         <v>413</v>
       </c>
@@ -5570,8 +5991,12 @@
         <v>2</v>
       </c>
       <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
+      <c r="E121" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G121" s="4">
         <v>6550</v>
       </c>
@@ -5595,8 +6020,12 @@
         <v>2</v>
       </c>
       <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
+      <c r="E122" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G122" s="4">
         <v>39959</v>
       </c>
@@ -5620,8 +6049,12 @@
         <v>2</v>
       </c>
       <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
+      <c r="E123" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="G123" s="4">
         <v>40865</v>
       </c>
@@ -5633,35 +6066,40 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="8" t="s">
         <v>478</v>
       </c>
-      <c r="B124" s="4" t="str">
+      <c r="B124" s="8" t="str">
         <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
         <v>reverse_type</v>
       </c>
-      <c r="C124" s="4">
-        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
-        <v>1</v>
-      </c>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4">
-        <v>1</v>
-      </c>
-      <c r="H124" s="4" t="s">
+      <c r="C124" s="8">
+        <f>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</f>
+        <v>1</v>
+      </c>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G124" s="8">
+        <v>1</v>
+      </c>
+      <c r="H124" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="I124" s="4" t="s">
+      <c r="I124" s="8" t="s">
         <v>192</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add WSs for additional database tables
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9D50F-7532-5E46-B15B-D4D4E6A79E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC307C-FBAE-474B-B1F3-2DC0D0D3BEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25160" yWindow="1480" windowWidth="23040" windowHeight="13900" activeTab="1" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23940" yWindow="720" windowWidth="23040" windowHeight="13900" activeTab="2" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
     <sheet name="TypologicalFields" sheetId="2" r:id="rId2"/>
-    <sheet name="ExamplesFields" sheetId="3" r:id="rId3"/>
-    <sheet name="Collections" sheetId="4" r:id="rId4"/>
-    <sheet name="CollectionsAndIIIF" sheetId="5" r:id="rId5"/>
-    <sheet name="CollectionsAndIIIFSummary" sheetId="6" r:id="rId6"/>
+    <sheet name="UniqueTypologicalFields" sheetId="9" r:id="rId3"/>
+    <sheet name="ExamplesFields" sheetId="3" r:id="rId4"/>
+    <sheet name="Collections" sheetId="4" r:id="rId5"/>
+    <sheet name="CollectionsAndIIIF" sheetId="5" r:id="rId6"/>
+    <sheet name="CollectionsAndIIIFSummary" sheetId="6" r:id="rId7"/>
+    <sheet name="stg_coins" sheetId="7" r:id="rId8"/>
+    <sheet name="stg_examples" sheetId="8" r:id="rId9"/>
+    <sheet name="stg_uri_pages" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,8 +89,53 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D4DC02ED-B345-BA4C-B034-520BBE5D6F8A}</author>
+    <author>tc={35A60B14-E187-3C46-BBDF-ABF000849503}</author>
+    <author>tc={6A10D586-80FD-C24E-A78C-BCC37B4E9B19}</author>
+    <author>tc={E0DA0131-AF0F-9A40-95B9-9F167B4A0F25}</author>
+  </authors>
+  <commentList>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{D4DC02ED-B345-BA4C-B034-520BBE5D6F8A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{35A60B14-E187-3C46-BBDF-ABF000849503}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="2" shapeId="0" xr:uid="{6A10D586-80FD-C24E-A78C-BCC37B4E9B19}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="3" shapeId="0" xr:uid="{E0DA0131-AF0F-9A40-95B9-9F167B4A0F25}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Try as TEXT and then change if this type is too large.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="551">
   <si>
     <t>collection</t>
   </si>
@@ -1831,7 +1880,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1862,44 +1911,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1951,6 +1969,38 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1989,28 +2039,39 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="19">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="18">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6CEF1CA9-0DCC-394B-BA91-CFDE8748A8EE}" name="Table6" displayName="Table6" ref="A1:B28" totalsRowShown="0">
+  <autoFilter ref="A1:B28" xr:uid="{6CEF1CA9-0DCC-394B-BA91-CFDE8748A8EE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{7B2A3A3E-1226-BD44-8B03-BE553B4DA31B}" name="field_name"/>
+    <tableColumn id="2" xr3:uid="{6F19C2CB-8D01-F04F-B578-E92F145FCC28}" name="data_type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}" name="Table3" displayName="Table3" ref="A1:E9" totalsRowCount="1">
   <autoFilter ref="A1:E8" xr:uid="{1A78B450-1655-3D49-827D-DF076DEDEF05}"/>
   <tableColumns count="5">
@@ -2024,12 +2085,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}" name="CollectionsTable" displayName="CollectionsTable" ref="A1:D57" totalsRowCount="1">
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="11">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2039,24 +2100,24 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="20">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="6">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="5">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2374,6 +2435,23 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B14" dT="2023-07-19T02:59:44.18" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{D4DC02ED-B345-BA4C-B034-520BBE5D6F8A}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="B17" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{35A60B14-E187-3C46-BBDF-ABF000849503}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="B21" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{6A10D586-80FD-C24E-A78C-BCC37B4E9B19}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+  <threadedComment ref="B28" dT="2023-07-19T03:00:05.99" personId="{0B902D7C-F8F7-7A4D-8BD7-A8C355A718B7}" id="{E0DA0131-AF0F-9A40-95B9-9F167B4A0F25}">
+    <text>Try as TEXT and then change if this type is too large.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDD5D45-1DCC-E44B-8D59-8507F8236A7D}">
   <dimension ref="A1:D5"/>
@@ -2463,15 +2541,27 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ECEDEA-565B-2645-A3E1-F668D8278F57}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F124" sqref="F124"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6105,6 +6195,254 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9732F9C-CA6E-C74C-B92D-16543E5A2491}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>546</v>
+      </c>
+      <c r="B8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>547</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>548</v>
+      </c>
+      <c r="B10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>549</v>
+      </c>
+      <c r="B11" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
+        <v>authority_authority</v>
+      </c>
+      <c r="B12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>320</v>
+      </c>
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>434</v>
+      </c>
+      <c r="B23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>436</v>
+      </c>
+      <c r="B24" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>463</v>
+      </c>
+      <c r="B25" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>472</v>
+      </c>
+      <c r="B26" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>474</v>
+      </c>
+      <c r="B27" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE1820D-22EF-E748-B98F-E9ADAA6A4092}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -6273,7 +6611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0256B6-CC9F-DA43-B2FC-ADA39BBB9055}">
   <dimension ref="A1:D57"/>
   <sheetViews>
@@ -7153,7 +7491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
   <dimension ref="A1:P67"/>
   <sheetViews>
@@ -9168,7 +9506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE74E1F-321C-FE4E-8C79-1D622E514933}">
   <dimension ref="A1:E44"/>
   <sheetViews>
@@ -9457,4 +9795,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Define schema for stg_coins table
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC307C-FBAE-474B-B1F3-2DC0D0D3BEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44956E15-18D2-B341-9FF8-DB7C80BFF556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23940" yWindow="720" windowWidth="23040" windowHeight="13900" activeTab="2" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="1" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="565">
   <si>
     <t>collection</t>
   </si>
@@ -1799,6 +1799,48 @@
   </si>
   <si>
     <t>TEXT</t>
+  </si>
+  <si>
+    <t>table_name</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>stg_coins</t>
+  </si>
+  <si>
+    <t>coin_id</t>
+  </si>
+  <si>
+    <t>primary_key</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>raw_uri_pages table</t>
+  </si>
+  <si>
+    <t>has_examples</t>
+  </si>
+  <si>
+    <t>has_examples_pagination</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>Scraping URI page</t>
+  </si>
+  <si>
+    <t>ts</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>Database generated</t>
   </si>
 </sst>
 </file>
@@ -2118,6 +2160,20 @@
     <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
     <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
     <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:E35" totalsRowShown="0">
+  <autoFilter ref="A1:E35" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6117DFE2-6236-1848-B40F-CB876F761A46}" name="table_name"/>
+    <tableColumn id="2" xr3:uid="{828DEEED-8A27-DA45-942B-678BAE403B37}" name="field_name"/>
+    <tableColumn id="3" xr3:uid="{F356DD31-BF0B-D941-A415-2020AD7CD0F2}" name="data_type"/>
+    <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
+    <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6198,8 +6254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9732F9C-CA6E-C74C-B92D-16543E5A2491}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9799,13 +9855,620 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" t="s">
+        <v>558</v>
+      </c>
+      <c r="C3" t="s">
+        <v>560</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>553</v>
+      </c>
+      <c r="B4" t="s">
+        <v>559</v>
+      </c>
+      <c r="C4" t="s">
+        <v>560</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>553</v>
+      </c>
+      <c r="B5" t="s">
+        <v>537</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B6" t="s">
+        <v>538</v>
+      </c>
+      <c r="C6" t="s">
+        <v>539</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B7" t="s">
+        <v>540</v>
+      </c>
+      <c r="C7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>553</v>
+      </c>
+      <c r="B8" t="s">
+        <v>541</v>
+      </c>
+      <c r="C8" t="s">
+        <v>539</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>553</v>
+      </c>
+      <c r="B9" t="s">
+        <v>542</v>
+      </c>
+      <c r="C9" t="s">
+        <v>539</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>553</v>
+      </c>
+      <c r="B10" t="s">
+        <v>545</v>
+      </c>
+      <c r="C10" t="s">
+        <v>539</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>553</v>
+      </c>
+      <c r="B11" t="s">
+        <v>546</v>
+      </c>
+      <c r="C11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>553</v>
+      </c>
+      <c r="B12" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>553</v>
+      </c>
+      <c r="B13" t="s">
+        <v>548</v>
+      </c>
+      <c r="C13" t="s">
+        <v>539</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>553</v>
+      </c>
+      <c r="B14" t="s">
+        <v>549</v>
+      </c>
+      <c r="C14" t="s">
+        <v>539</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>553</v>
+      </c>
+      <c r="B16" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" t="s">
+        <v>539</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>553</v>
+      </c>
+      <c r="B17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>553</v>
+      </c>
+      <c r="B18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" t="s">
+        <v>539</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>553</v>
+      </c>
+      <c r="B19" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" t="s">
+        <v>539</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>553</v>
+      </c>
+      <c r="B20" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" t="s">
+        <v>550</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>553</v>
+      </c>
+      <c r="B21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>553</v>
+      </c>
+      <c r="B22" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>553</v>
+      </c>
+      <c r="B23" t="s">
+        <v>332</v>
+      </c>
+      <c r="C23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>553</v>
+      </c>
+      <c r="B24" t="s">
+        <v>334</v>
+      </c>
+      <c r="C24" t="s">
+        <v>550</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>553</v>
+      </c>
+      <c r="B25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>553</v>
+      </c>
+      <c r="B26" t="s">
+        <v>434</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>553</v>
+      </c>
+      <c r="B27" t="s">
+        <v>436</v>
+      </c>
+      <c r="C27" t="s">
+        <v>539</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>553</v>
+      </c>
+      <c r="B28" t="s">
+        <v>463</v>
+      </c>
+      <c r="C28" t="s">
+        <v>539</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>553</v>
+      </c>
+      <c r="B29" t="s">
+        <v>472</v>
+      </c>
+      <c r="C29" t="s">
+        <v>539</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30" t="s">
+        <v>474</v>
+      </c>
+      <c r="C30" t="s">
+        <v>539</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>553</v>
+      </c>
+      <c r="B31" t="s">
+        <v>478</v>
+      </c>
+      <c r="C31" t="s">
+        <v>550</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>553</v>
+      </c>
+      <c r="B32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>553</v>
+      </c>
+      <c r="B33" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>553</v>
+      </c>
+      <c r="B34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>553</v>
+      </c>
+      <c r="B35" t="s">
+        <v>562</v>
+      </c>
+      <c r="C35" t="s">
+        <v>563</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>564</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add stg_examples table schema
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44956E15-18D2-B341-9FF8-DB7C80BFF556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD83A0-930E-B344-8623-A1615047F49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="1" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="570">
   <si>
     <t>collection</t>
   </si>
@@ -1841,6 +1841,21 @@
   </si>
   <si>
     <t>Database generated</t>
+  </si>
+  <si>
+    <t>stg_examples</t>
+  </si>
+  <si>
+    <t>examples_id</t>
+  </si>
+  <si>
+    <t>SERIAL</t>
+  </si>
+  <si>
+    <t>Database generated. (This is the table ID)</t>
+  </si>
+  <si>
+    <t>uri_examples_id</t>
   </si>
 </sst>
 </file>
@@ -2174,6 +2189,34 @@
     <tableColumn id="3" xr3:uid="{F356DD31-BF0B-D941-A415-2020AD7CD0F2}" name="data_type"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}" name="Table8" displayName="Table8" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F7340B1E-35F9-5648-82E2-8460E781DD0B}" name="table_name"/>
+    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name"/>
+    <tableColumn id="3" xr3:uid="{4CC7DC79-F70D-2A4E-B93F-ACBBB84B801F}" name="data_type"/>
+    <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
+    <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A7ACFD44-D83B-AD40-B1C7-4B033D49056A}" name="table_name"/>
+    <tableColumn id="2" xr3:uid="{EED50E56-653F-F44B-A5A2-06A8BAD5110E}" name="field_name"/>
+    <tableColumn id="3" xr3:uid="{41814122-2E6B-A940-894C-98B36AE88A63}" name="data_type"/>
+    <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
+    <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2599,13 +2642,43 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -9857,8 +9930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10474,12 +10547,228 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" t="s">
+        <v>554</v>
+      </c>
+      <c r="C3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>565</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>565</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>565</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>565</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>565</v>
+      </c>
+      <c r="B11" t="s">
+        <v>569</v>
+      </c>
+      <c r="C11" t="s">
+        <v>556</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>565</v>
+      </c>
+      <c r="B12" t="s">
+        <v>562</v>
+      </c>
+      <c r="C12" t="s">
+        <v>563</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>564</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add stg_examples_images table schema
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD83A0-930E-B344-8623-A1615047F49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770C36CB-EAAE-314D-B6E3-E58B6ADEAE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="9" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="CollectionsAndIIIFSummary" sheetId="6" r:id="rId7"/>
     <sheet name="stg_coins" sheetId="7" r:id="rId8"/>
     <sheet name="stg_examples" sheetId="8" r:id="rId9"/>
-    <sheet name="stg_uri_pages" sheetId="10" r:id="rId10"/>
+    <sheet name="stg_examples_images" sheetId="11" r:id="rId10"/>
+    <sheet name="stg_uri_pages" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -135,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="578">
   <si>
     <t>collection</t>
   </si>
@@ -1856,6 +1857,30 @@
   </si>
   <si>
     <t>uri_examples_id</t>
+  </si>
+  <si>
+    <t>stg_examples_images</t>
+  </si>
+  <si>
+    <t>examples_images_id</t>
+  </si>
+  <si>
+    <t>stg_examples_id</t>
+  </si>
+  <si>
+    <t>image_type</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Scraping URI page. (This is from URI page)</t>
+  </si>
+  <si>
+    <t>table: stg_examples, field: examples_id</t>
+  </si>
+  <si>
+    <t>One of: obverse, reverse, both sides, unknown</t>
   </si>
 </sst>
 </file>
@@ -2095,6 +2120,20 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A7ACFD44-D83B-AD40-B1C7-4B033D49056A}" name="table_name"/>
+    <tableColumn id="2" xr3:uid="{EED50E56-653F-F44B-A5A2-06A8BAD5110E}" name="field_name"/>
+    <tableColumn id="3" xr3:uid="{41814122-2E6B-A940-894C-98B36AE88A63}" name="data_type"/>
+    <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
+    <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
@@ -2209,14 +2248,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}" name="Table10" displayName="Table10" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A7ACFD44-D83B-AD40-B1C7-4B033D49056A}" name="table_name"/>
-    <tableColumn id="2" xr3:uid="{EED50E56-653F-F44B-A5A2-06A8BAD5110E}" name="field_name"/>
-    <tableColumn id="3" xr3:uid="{41814122-2E6B-A940-894C-98B36AE88A63}" name="data_type"/>
-    <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
-    <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
+    <tableColumn id="1" xr3:uid="{07A88E05-541C-0849-B472-33E52C37EEA1}" name="table_name"/>
+    <tableColumn id="2" xr3:uid="{803A1D07-1C0D-F549-BF92-C19C63999FD7}" name="field_name"/>
+    <tableColumn id="3" xr3:uid="{5C665CF7-3EEB-5349-960F-B35A05BA2840}" name="data_type"/>
+    <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
+    <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2641,20 +2680,145 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA434118-7673-B544-AD54-0753231E47ED}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" t="s">
+        <v>572</v>
+      </c>
+      <c r="C3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B4" t="s">
+        <v>573</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>570</v>
+      </c>
+      <c r="B5" t="s">
+        <v>574</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -9930,8 +10094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10549,16 +10713,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -10745,7 +10909,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add stg_uri_pages table schema
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770C36CB-EAAE-314D-B6E3-E58B6ADEAE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB36BC4B-6B19-774E-9E26-55A277291157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="9" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="10" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="588">
   <si>
     <t>collection</t>
   </si>
@@ -1881,6 +1881,36 @@
   </si>
   <si>
     <t>One of: obverse, reverse, both sides, unknown</t>
+  </si>
+  <si>
+    <t>stg_uri_pages</t>
+  </si>
+  <si>
+    <t>uri_page_id</t>
+  </si>
+  <si>
+    <t>table: raw_uri_pages, field: raw_uri_id</t>
+  </si>
+  <si>
+    <t>examples_pagination_id</t>
+  </si>
+  <si>
+    <t>examples_total_pagination</t>
+  </si>
+  <si>
+    <t>examples_start_id</t>
+  </si>
+  <si>
+    <t>examples_end_id</t>
+  </si>
+  <si>
+    <t>examples_max_id</t>
+  </si>
+  <si>
+    <t>uri_link</t>
+  </si>
+  <si>
+    <t>raw_uri_pages</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2151,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A7ACFD44-D83B-AD40-B1C7-4B033D49056A}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{EED50E56-653F-F44B-A5A2-06A8BAD5110E}" name="field_name"/>
@@ -2683,7 +2713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA434118-7673-B544-AD54-0753231E47ED}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2807,10 +2837,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2836,6 +2866,159 @@
       </c>
       <c r="E1" t="s">
         <v>552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>578</v>
+      </c>
+      <c r="B3" t="s">
+        <v>554</v>
+      </c>
+      <c r="C3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C4" t="s">
+        <v>556</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>578</v>
+      </c>
+      <c r="B5" t="s">
+        <v>582</v>
+      </c>
+      <c r="C5" t="s">
+        <v>556</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>578</v>
+      </c>
+      <c r="B7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C7" t="s">
+        <v>556</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>578</v>
+      </c>
+      <c r="B8" t="s">
+        <v>585</v>
+      </c>
+      <c r="C8" t="s">
+        <v>556</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>578</v>
+      </c>
+      <c r="B9" t="s">
+        <v>586</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>578</v>
+      </c>
+      <c r="B10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C10" t="s">
+        <v>563</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fields to stg_coins
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB36BC4B-6B19-774E-9E26-55A277291157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02542D4A-79A5-534A-A003-321AA576CE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="10" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="591">
   <si>
     <t>collection</t>
   </si>
@@ -1912,12 +1912,21 @@
   <si>
     <t>raw_uri_pages</t>
   </si>
+  <si>
+    <t>has_typological</t>
+  </si>
+  <si>
+    <t>Always TRUE/scraping</t>
+  </si>
+  <si>
+    <t>has_analysis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1946,12 +1955,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2250,8 +2253,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:E35" totalsRowShown="0">
-  <autoFilter ref="A1:E35" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:E37" totalsRowShown="0">
+  <autoFilter ref="A1:E37" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6117DFE2-6236-1848-B40F-CB876F761A46}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{828DEEED-8A27-DA45-942B-678BAE403B37}" name="field_name"/>
@@ -2839,7 +2842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -10275,10 +10278,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10328,7 +10331,7 @@
         <v>553</v>
       </c>
       <c r="B3" t="s">
-        <v>558</v>
+        <v>588</v>
       </c>
       <c r="C3" t="s">
         <v>560</v>
@@ -10337,7 +10340,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>557</v>
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -10345,7 +10348,7 @@
         <v>553</v>
       </c>
       <c r="B4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C4" t="s">
         <v>560</v>
@@ -10362,16 +10365,16 @@
         <v>553</v>
       </c>
       <c r="B5" t="s">
-        <v>537</v>
+        <v>559</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>560</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -10379,10 +10382,10 @@
         <v>553</v>
       </c>
       <c r="B6" t="s">
-        <v>538</v>
+        <v>590</v>
       </c>
       <c r="C6" t="s">
-        <v>539</v>
+        <v>560</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -10396,7 +10399,7 @@
         <v>553</v>
       </c>
       <c r="B7" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C7" t="s">
         <v>188</v>
@@ -10413,7 +10416,7 @@
         <v>553</v>
       </c>
       <c r="B8" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C8" t="s">
         <v>539</v>
@@ -10430,10 +10433,10 @@
         <v>553</v>
       </c>
       <c r="B9" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C9" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -10447,7 +10450,7 @@
         <v>553</v>
       </c>
       <c r="B10" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C10" t="s">
         <v>539</v>
@@ -10464,7 +10467,7 @@
         <v>553</v>
       </c>
       <c r="B11" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C11" t="s">
         <v>539</v>
@@ -10481,10 +10484,10 @@
         <v>553</v>
       </c>
       <c r="B12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -10498,7 +10501,7 @@
         <v>553</v>
       </c>
       <c r="B13" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C13" t="s">
         <v>539</v>
@@ -10515,10 +10518,10 @@
         <v>553</v>
       </c>
       <c r="B14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C14" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -10532,10 +10535,10 @@
         <v>553</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>548</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -10549,7 +10552,7 @@
         <v>553</v>
       </c>
       <c r="B16" t="s">
-        <v>299</v>
+        <v>549</v>
       </c>
       <c r="C16" t="s">
         <v>539</v>
@@ -10566,10 +10569,10 @@
         <v>553</v>
       </c>
       <c r="B17" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
-        <v>550</v>
+        <v>188</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -10583,7 +10586,7 @@
         <v>553</v>
       </c>
       <c r="B18" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="C18" t="s">
         <v>539</v>
@@ -10600,10 +10603,10 @@
         <v>553</v>
       </c>
       <c r="B19" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C19" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -10617,10 +10620,10 @@
         <v>553</v>
       </c>
       <c r="B20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C20" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -10634,10 +10637,10 @@
         <v>553</v>
       </c>
       <c r="B21" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C21" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -10651,10 +10654,10 @@
         <v>553</v>
       </c>
       <c r="B22" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C22" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -10668,7 +10671,7 @@
         <v>553</v>
       </c>
       <c r="B23" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C23" t="s">
         <v>188</v>
@@ -10685,10 +10688,10 @@
         <v>553</v>
       </c>
       <c r="B24" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C24" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -10702,7 +10705,7 @@
         <v>553</v>
       </c>
       <c r="B25" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C25" t="s">
         <v>188</v>
@@ -10719,10 +10722,10 @@
         <v>553</v>
       </c>
       <c r="B26" t="s">
-        <v>434</v>
+        <v>334</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>550</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -10736,10 +10739,10 @@
         <v>553</v>
       </c>
       <c r="B27" t="s">
-        <v>436</v>
+        <v>336</v>
       </c>
       <c r="C27" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -10753,10 +10756,10 @@
         <v>553</v>
       </c>
       <c r="B28" t="s">
-        <v>463</v>
+        <v>434</v>
       </c>
       <c r="C28" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -10770,7 +10773,7 @@
         <v>553</v>
       </c>
       <c r="B29" t="s">
-        <v>472</v>
+        <v>436</v>
       </c>
       <c r="C29" t="s">
         <v>539</v>
@@ -10787,7 +10790,7 @@
         <v>553</v>
       </c>
       <c r="B30" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="C30" t="s">
         <v>539</v>
@@ -10804,10 +10807,10 @@
         <v>553</v>
       </c>
       <c r="B31" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C31" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -10821,10 +10824,10 @@
         <v>553</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>474</v>
       </c>
       <c r="C32" t="s">
-        <v>187</v>
+        <v>539</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -10838,10 +10841,10 @@
         <v>553</v>
       </c>
       <c r="B33" t="s">
-        <v>193</v>
+        <v>478</v>
       </c>
       <c r="C33" t="s">
-        <v>187</v>
+        <v>550</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -10855,7 +10858,7 @@
         <v>553</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C34" t="s">
         <v>187</v>
@@ -10872,15 +10875,49 @@
         <v>553</v>
       </c>
       <c r="B35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>553</v>
+      </c>
+      <c r="B36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>553</v>
+      </c>
+      <c r="B37" t="s">
         <v>562</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>563</v>
       </c>
-      <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
         <v>564</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix stg_coins field, add columns to schema, and auto-generate code
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02542D4A-79A5-534A-A003-321AA576CE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ABFD47-2300-D441-A6BC-BF4BB1D52A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-24060" yWindow="1380" windowWidth="23040" windowHeight="13900" firstSheet="1" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="597">
   <si>
     <t>collection</t>
   </si>
@@ -1920,6 +1920,24 @@
   </si>
   <si>
     <t>has_analysis</t>
+  </si>
+  <si>
+    <t>is_null</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>sql_code</t>
   </si>
 </sst>
 </file>
@@ -2032,7 +2050,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2168,22 +2189,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="22">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="20">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2219,7 +2240,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="12">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2230,37 +2251,42 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="11">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="7">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="6">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:E37" totalsRowShown="0">
-  <autoFilter ref="A1:E37" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:H37" totalsRowShown="0">
+  <autoFilter ref="A1:H37" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6117DFE2-6236-1848-B40F-CB876F761A46}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{828DEEED-8A27-DA45-942B-678BAE403B37}" name="field_name"/>
     <tableColumn id="3" xr3:uid="{F356DD31-BF0B-D941-A415-2020AD7CD0F2}" name="data_type"/>
+    <tableColumn id="6" xr3:uid="{A5EC5CEA-3010-7E45-98F0-5956CCC323D8}" name="is_null"/>
+    <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3037,10 +3063,10 @@
   <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6678,7 +6704,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B28"/>
+      <selection activeCell="A18" sqref="A18:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6776,9 +6802,8 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <f>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</f>
-        <v>authority_authority</v>
+      <c r="A12" t="s">
+        <v>297</v>
       </c>
       <c r="B12" t="s">
         <v>188</v>
@@ -10278,10 +10303,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10289,10 +10314,13 @@
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>551</v>
       </c>
@@ -10303,13 +10331,22 @@
         <v>186</v>
       </c>
       <c r="D1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E1" t="s">
+        <v>594</v>
+      </c>
+      <c r="F1" t="s">
         <v>555</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>553</v>
       </c>
@@ -10319,14 +10356,21 @@
       <c r="C2" t="s">
         <v>556</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" t="s">
+        <v>592</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>coin_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>553</v>
       </c>
@@ -10336,14 +10380,21 @@
       <c r="C3" t="s">
         <v>560</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
+        <v>592</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>has_typological BOOLEAN NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>553</v>
       </c>
@@ -10353,14 +10404,21 @@
       <c r="C4" t="s">
         <v>560</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
+        <v>592</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>has_examples BOOLEAN NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>553</v>
       </c>
@@ -10370,14 +10428,21 @@
       <c r="C5" t="s">
         <v>560</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
+        <v>592</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>has_examples_pagination BOOLEAN NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>553</v>
       </c>
@@ -10387,14 +10452,21 @@
       <c r="C6" t="s">
         <v>560</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
+        <v>592</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>has_analysis BOOLEAN NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>553</v>
       </c>
@@ -10404,14 +10476,21 @@
       <c r="C7" t="s">
         <v>188</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
+        <v>593</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>coin_date_range VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>553</v>
       </c>
@@ -10421,14 +10500,21 @@
       <c r="C8" t="s">
         <v>539</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
+        <v>593</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>denomination VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>553</v>
       </c>
@@ -10438,14 +10524,21 @@
       <c r="C9" t="s">
         <v>188</v>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
+        <v>593</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H9" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>manufacture VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>553</v>
       </c>
@@ -10455,14 +10548,21 @@
       <c r="C10" t="s">
         <v>539</v>
       </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H10" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>material VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>553</v>
       </c>
@@ -10472,14 +10572,21 @@
       <c r="C11" t="s">
         <v>539</v>
       </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" t="s">
+        <v>593</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H11" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>object_type VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>553</v>
       </c>
@@ -10489,14 +10596,21 @@
       <c r="C12" t="s">
         <v>539</v>
       </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
+        <v>593</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>authority_name VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>553</v>
       </c>
@@ -10506,14 +10620,21 @@
       <c r="C13" t="s">
         <v>539</v>
       </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
+        <v>593</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H13" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>issuer_name VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>553</v>
       </c>
@@ -10523,14 +10644,21 @@
       <c r="C14" t="s">
         <v>188</v>
       </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
+        <v>593</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H14" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>stated_authority_name VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>553</v>
       </c>
@@ -10540,14 +10668,21 @@
       <c r="C15" t="s">
         <v>539</v>
       </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
+        <v>593</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H15" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>mint VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>553</v>
       </c>
@@ -10557,31 +10692,45 @@
       <c r="C16" t="s">
         <v>539</v>
       </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H16" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>region VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>553</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
       <c r="C17" t="s">
         <v>188</v>
       </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
+        <v>593</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H17" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_controlmark VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>553</v>
       </c>
@@ -10591,14 +10740,21 @@
       <c r="C18" t="s">
         <v>539</v>
       </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s">
+        <v>593</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H18" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_deity VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>553</v>
       </c>
@@ -10608,14 +10764,21 @@
       <c r="C19" t="s">
         <v>550</v>
       </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
+        <v>593</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H19" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_legend TEXT NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>553</v>
       </c>
@@ -10625,14 +10788,21 @@
       <c r="C20" t="s">
         <v>539</v>
       </c>
-      <c r="D20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H20" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_portrait VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>553</v>
       </c>
@@ -10642,14 +10812,21 @@
       <c r="C21" t="s">
         <v>539</v>
       </c>
-      <c r="D21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" t="s">
+        <v>593</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H21" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_state VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>553</v>
       </c>
@@ -10659,14 +10836,21 @@
       <c r="C22" t="s">
         <v>550</v>
       </c>
-      <c r="D22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
+        <v>593</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H22" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>obverse_type TEXT NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>553</v>
       </c>
@@ -10676,14 +10860,21 @@
       <c r="C23" t="s">
         <v>188</v>
       </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
+        <v>593</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H23" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_control_marks VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>553</v>
       </c>
@@ -10693,14 +10884,21 @@
       <c r="C24" t="s">
         <v>539</v>
       </c>
-      <c r="D24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
+        <v>593</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H24" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_deity VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>553</v>
       </c>
@@ -10710,14 +10908,21 @@
       <c r="C25" t="s">
         <v>188</v>
       </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
+        <v>593</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H25" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_dynasty VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>553</v>
       </c>
@@ -10727,14 +10932,21 @@
       <c r="C26" t="s">
         <v>550</v>
       </c>
-      <c r="D26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
+        <v>593</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H26" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_legend TEXT NULL,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>553</v>
       </c>
@@ -10744,14 +10956,21 @@
       <c r="C27" t="s">
         <v>188</v>
       </c>
-      <c r="D27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
+        <v>593</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H27" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_mintmark VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>553</v>
       </c>
@@ -10761,14 +10980,21 @@
       <c r="C28" t="s">
         <v>188</v>
       </c>
-      <c r="D28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s">
+        <v>593</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H28" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_monogram VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>553</v>
       </c>
@@ -10778,14 +11004,21 @@
       <c r="C29" t="s">
         <v>539</v>
       </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" t="s">
+        <v>593</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H29" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_officinamark VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>553</v>
       </c>
@@ -10795,14 +11028,21 @@
       <c r="C30" t="s">
         <v>539</v>
       </c>
-      <c r="D30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" t="s">
+        <v>593</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H30" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_portrait VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>553</v>
       </c>
@@ -10812,14 +11052,21 @@
       <c r="C31" t="s">
         <v>539</v>
       </c>
-      <c r="D31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" t="s">
+        <v>593</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H31" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_state VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>553</v>
       </c>
@@ -10829,14 +11076,21 @@
       <c r="C32" t="s">
         <v>539</v>
       </c>
-      <c r="D32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" t="s">
+        <v>593</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H32" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_symbol VARCHAR[] NULL,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>553</v>
       </c>
@@ -10846,14 +11100,21 @@
       <c r="C33" t="s">
         <v>550</v>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D33" t="s">
+        <v>593</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H33" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>reverse_type TEXT NULL,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>553</v>
       </c>
@@ -10863,14 +11124,21 @@
       <c r="C34" t="s">
         <v>187</v>
       </c>
-      <c r="D34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D34" t="s">
+        <v>593</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H34" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>average_axis NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>553</v>
       </c>
@@ -10880,14 +11148,21 @@
       <c r="C35" t="s">
         <v>187</v>
       </c>
-      <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" t="s">
+        <v>593</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H35" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>average_diameter NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>553</v>
       </c>
@@ -10897,14 +11172,21 @@
       <c r="C36" t="s">
         <v>187</v>
       </c>
-      <c r="D36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" t="s">
+        <v>593</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H36" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>average_weight NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>553</v>
       </c>
@@ -10914,15 +11196,26 @@
       <c r="C37" t="s">
         <v>563</v>
       </c>
-      <c r="D37" t="b">
-        <v>0</v>
+      <c r="D37" t="s">
+        <v>592</v>
       </c>
       <c r="E37" t="s">
+        <v>595</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
         <v>564</v>
+      </c>
+      <c r="H37" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Add create stg_examples script and update schema in spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ABFD47-2300-D441-A6BC-BF4BB1D52A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CAA4E4-249F-B44D-B46B-EC6ACE4D73D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24060" yWindow="1380" windowWidth="23040" windowHeight="13900" firstSheet="1" activeTab="7" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-24080" yWindow="1380" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="600">
   <si>
     <t>collection</t>
   </si>
@@ -1856,9 +1856,6 @@
     <t>Database generated. (This is the table ID)</t>
   </si>
   <si>
-    <t>uri_examples_id</t>
-  </si>
-  <si>
     <t>stg_examples_images</t>
   </si>
   <si>
@@ -1938,6 +1935,18 @@
   </si>
   <si>
     <t>sql_code</t>
+  </si>
+  <si>
+    <t>uri_page_examples_id</t>
+  </si>
+  <si>
+    <t>coin_axis</t>
+  </si>
+  <si>
+    <t>coin_diameter</t>
+  </si>
+  <si>
+    <t>coin_weight</t>
   </si>
 </sst>
 </file>
@@ -2050,7 +2059,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2189,22 +2201,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="21">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2240,7 +2252,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="13">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2251,23 +2263,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="12">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="8">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="7">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2284,7 +2296,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2293,14 +2305,19 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}" name="Table8" displayName="Table8" ref="A1:E12" totalsRowShown="0">
-  <autoFilter ref="A1:E12" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}" name="Table8" displayName="Table8" ref="A1:H12" totalsRowShown="0">
+  <autoFilter ref="A1:H12" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F7340B1E-35F9-5648-82E2-8460E781DD0B}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name"/>
     <tableColumn id="3" xr3:uid="{4CC7DC79-F70D-2A4E-B93F-ACBBB84B801F}" name="data_type"/>
+    <tableColumn id="6" xr3:uid="{CCD0FDAB-579C-0A4E-B073-6A0596D1E8DB}" name="is_null"/>
+    <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2773,10 +2790,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B2" t="s">
         <v>570</v>
-      </c>
-      <c r="B2" t="s">
-        <v>571</v>
       </c>
       <c r="C2" t="s">
         <v>567</v>
@@ -2790,10 +2807,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C3" t="s">
         <v>556</v>
@@ -2802,15 +2819,15 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C4" t="s">
         <v>188</v>
@@ -2819,15 +2836,15 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C5" t="s">
         <v>188</v>
@@ -2841,7 +2858,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B6" t="s">
         <v>562</v>
@@ -2899,10 +2916,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" t="s">
         <v>578</v>
-      </c>
-      <c r="B2" t="s">
-        <v>579</v>
       </c>
       <c r="C2" t="s">
         <v>556</v>
@@ -2911,12 +2928,12 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B3" t="s">
         <v>554</v>
@@ -2928,15 +2945,15 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C4" t="s">
         <v>556</v>
@@ -2945,15 +2962,15 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C5" t="s">
         <v>556</v>
@@ -2962,15 +2979,15 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C6" t="s">
         <v>556</v>
@@ -2979,15 +2996,15 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C7" t="s">
         <v>556</v>
@@ -2996,15 +3013,15 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C8" t="s">
         <v>556</v>
@@ -3013,15 +3030,15 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C9" t="s">
         <v>188</v>
@@ -3030,12 +3047,12 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B10" t="s">
         <v>562</v>
@@ -10305,8 +10322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10317,7 +10334,7 @@
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -10331,10 +10348,10 @@
         <v>186</v>
       </c>
       <c r="D1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F1" t="s">
         <v>555</v>
@@ -10343,7 +10360,7 @@
         <v>552</v>
       </c>
       <c r="H1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -10357,7 +10374,7 @@
         <v>556</v>
       </c>
       <c r="D2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -10375,19 +10392,19 @@
         <v>553</v>
       </c>
       <c r="B3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C3" t="s">
         <v>560</v>
       </c>
       <c r="D3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H3" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
@@ -10405,7 +10422,7 @@
         <v>560</v>
       </c>
       <c r="D4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -10429,7 +10446,7 @@
         <v>560</v>
       </c>
       <c r="D5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -10447,13 +10464,13 @@
         <v>553</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C6" t="s">
         <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -10477,7 +10494,7 @@
         <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -10501,7 +10518,7 @@
         <v>539</v>
       </c>
       <c r="D8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -10525,7 +10542,7 @@
         <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -10549,7 +10566,7 @@
         <v>539</v>
       </c>
       <c r="D10" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -10573,7 +10590,7 @@
         <v>539</v>
       </c>
       <c r="D11" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -10597,7 +10614,7 @@
         <v>539</v>
       </c>
       <c r="D12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -10621,7 +10638,7 @@
         <v>539</v>
       </c>
       <c r="D13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -10645,7 +10662,7 @@
         <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -10669,7 +10686,7 @@
         <v>539</v>
       </c>
       <c r="D15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -10693,7 +10710,7 @@
         <v>539</v>
       </c>
       <c r="D16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -10717,7 +10734,7 @@
         <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -10741,7 +10758,7 @@
         <v>539</v>
       </c>
       <c r="D18" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -10765,7 +10782,7 @@
         <v>550</v>
       </c>
       <c r="D19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -10789,7 +10806,7 @@
         <v>539</v>
       </c>
       <c r="D20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -10813,7 +10830,7 @@
         <v>539</v>
       </c>
       <c r="D21" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -10837,7 +10854,7 @@
         <v>550</v>
       </c>
       <c r="D22" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -10861,7 +10878,7 @@
         <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -10885,7 +10902,7 @@
         <v>539</v>
       </c>
       <c r="D24" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -10909,7 +10926,7 @@
         <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -10933,7 +10950,7 @@
         <v>550</v>
       </c>
       <c r="D26" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -10957,7 +10974,7 @@
         <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -10981,7 +10998,7 @@
         <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -11005,7 +11022,7 @@
         <v>539</v>
       </c>
       <c r="D29" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -11029,7 +11046,7 @@
         <v>539</v>
       </c>
       <c r="D30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -11053,7 +11070,7 @@
         <v>539</v>
       </c>
       <c r="D31" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -11077,7 +11094,7 @@
         <v>539</v>
       </c>
       <c r="D32" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -11101,7 +11118,7 @@
         <v>550</v>
       </c>
       <c r="D33" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -11125,7 +11142,7 @@
         <v>187</v>
       </c>
       <c r="D34" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -11149,7 +11166,7 @@
         <v>187</v>
       </c>
       <c r="D35" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -11173,7 +11190,7 @@
         <v>187</v>
       </c>
       <c r="D36" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -11197,10 +11214,10 @@
         <v>563</v>
       </c>
       <c r="D37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -11224,21 +11241,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="3" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>551</v>
       </c>
@@ -11249,13 +11267,22 @@
         <v>186</v>
       </c>
       <c r="D1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" t="s">
         <v>555</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>565</v>
       </c>
@@ -11265,14 +11292,21 @@
       <c r="C2" t="s">
         <v>567</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>examples_id SERIAL NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>565</v>
       </c>
@@ -11282,150 +11316,213 @@
       <c r="C3" t="s">
         <v>556</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>coin_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>565</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>596</v>
       </c>
       <c r="C4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>556</v>
+      </c>
+      <c r="D4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>574</v>
+      </c>
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>uri_page_examples_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>565</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>597</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>592</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>coin_axis NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>565</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>592</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>collection_name VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>565</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>598</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="s">
+        <v>592</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>coin_diameter NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>565</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>188</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
+        <v>592</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>findspot VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>565</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
         <v>188</v>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
+        <v>592</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H9" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>hoard VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>565</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" t="s">
+        <v>592</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H10" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>identifier VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>565</v>
       </c>
       <c r="B11" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
       <c r="C11" t="s">
-        <v>556</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+      <c r="D11" t="s">
+        <v>592</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>561</v>
+      </c>
+      <c r="H11" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>coin_weight NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>565</v>
       </c>
@@ -11435,15 +11532,27 @@
       <c r="C12" t="s">
         <v>563</v>
       </c>
-      <c r="D12" t="b">
-        <v>0</v>
+      <c r="D12" t="s">
+        <v>591</v>
       </c>
       <c r="E12" t="s">
+        <v>594</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
         <v>564</v>
       </c>
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Add create stg_examples_images script and schema in spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CAA4E4-249F-B44D-B46B-EC6ACE4D73D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BBDC88-ECA4-4548-AE18-17F17AD09E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24080" yWindow="1380" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23920" yWindow="920" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="9" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="600">
   <si>
     <t>collection</t>
   </si>
@@ -2059,7 +2059,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2201,22 +2204,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="22">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="21">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2252,7 +2255,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="14">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2263,23 +2266,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="13">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="9">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="8">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2296,7 +2299,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2315,7 +2318,7 @@
     <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
-    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,14 +2327,19 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}" name="Table10" displayName="Table10" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}" name="Table10" displayName="Table10" ref="A2:H7" totalsRowShown="0">
+  <autoFilter ref="A2:H7" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{07A88E05-541C-0849-B472-33E52C37EEA1}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{803A1D07-1C0D-F549-BF92-C19C63999FD7}" name="field_name"/>
     <tableColumn id="3" xr3:uid="{5C665CF7-3EEB-5349-960F-B35A05BA2840}" name="data_type"/>
+    <tableColumn id="6" xr3:uid="{ECA370F4-87A2-9447-B408-063DCBF950CD}" name="is_null"/>
+    <tableColumn id="7" xr3:uid="{C3D521DA-8B4C-DE40-B393-07D69A13443B}" name="default"/>
     <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
+    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2757,21 +2765,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA434118-7673-B544-AD54-0753231E47ED}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="3" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>551</v>
       </c>
@@ -2782,99 +2791,174 @@
         <v>186</v>
       </c>
       <c r="D1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" t="s">
         <v>555</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="B2" t="s">
-        <v>570</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>567</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>590</v>
       </c>
       <c r="E2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>593</v>
+      </c>
+      <c r="F2" t="s">
+        <v>555</v>
+      </c>
+      <c r="G2" t="s">
+        <v>552</v>
+      </c>
+      <c r="H2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>569</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C3" t="s">
-        <v>556</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>567</v>
+      </c>
+      <c r="D3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>564</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>examples_images_id SERIAL NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>569</v>
       </c>
       <c r="B4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" t="b">
+        <v>556</v>
+      </c>
+      <c r="D4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>stg_examples_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>569</v>
       </c>
       <c r="B5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C5" t="s">
         <v>188</v>
       </c>
-      <c r="D5" t="b">
+      <c r="D5" t="s">
+        <v>591</v>
+      </c>
+      <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>576</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>image_type VARCHAR NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>569</v>
       </c>
       <c r="B6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>591</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>561</v>
+      </c>
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>link VARCHAR NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>569</v>
+      </c>
+      <c r="B7" t="s">
         <v>562</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>563</v>
       </c>
-      <c r="D6" t="b">
+      <c r="D7" t="s">
+        <v>591</v>
+      </c>
+      <c r="E7" t="s">
+        <v>594</v>
+      </c>
+      <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G7" t="s">
         <v>564</v>
       </c>
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -11243,8 +11327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add create stg_uri_pages script and update schema in spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BBDC88-ECA4-4548-AE18-17F17AD09E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C857C3-FB7A-154C-87A5-2280A7BFC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23920" yWindow="920" windowWidth="23040" windowHeight="13900" firstSheet="3" activeTab="9" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23920" yWindow="920" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="10" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="600">
   <si>
     <t>collection</t>
   </si>
@@ -2059,7 +2059,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2190,36 +2193,41 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:E10" totalsRowShown="0">
-  <autoFilter ref="A1:E10" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}" name="Table9" displayName="Table9" ref="A1:H10" totalsRowShown="0">
+  <autoFilter ref="A1:H10" xr:uid="{A383A2EC-64EB-314E-A4B5-652AA0105B14}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A7ACFD44-D83B-AD40-B1C7-4B033D49056A}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{EED50E56-653F-F44B-A5A2-06A8BAD5110E}" name="field_name"/>
     <tableColumn id="3" xr3:uid="{41814122-2E6B-A940-894C-98B36AE88A63}" name="data_type"/>
+    <tableColumn id="6" xr3:uid="{BCB552EE-EEAD-1649-8763-5305E442772E}" name="is_null"/>
+    <tableColumn id="7" xr3:uid="{13B45FA7-B2BD-6744-81EC-7C7DA0F79F53}" name="default"/>
     <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
+    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="25">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="23">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="22">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2255,7 +2263,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="15">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2266,23 +2274,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="14">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="10">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="9">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,7 +2307,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2318,7 +2326,7 @@
     <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
-    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2327,8 +2335,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}" name="Table10" displayName="Table10" ref="A2:H7" totalsRowShown="0">
-  <autoFilter ref="A2:H7" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}" name="Table10" displayName="Table10" ref="A1:H6" totalsRowShown="0">
+  <autoFilter ref="A1:H6" xr:uid="{6C7B0E7D-BAF9-2F40-B1EF-C01F7EF13DD4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{07A88E05-541C-0849-B472-33E52C37EEA1}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{803A1D07-1C0D-F549-BF92-C19C63999FD7}" name="field_name"/>
@@ -2337,7 +2345,7 @@
     <tableColumn id="7" xr3:uid="{C3D521DA-8B4C-DE40-B393-07D69A13443B}" name="default"/>
     <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
-    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2765,10 +2773,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA434118-7673-B544-AD54-0753231E47ED}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2808,28 +2816,26 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>570</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>567</v>
       </c>
       <c r="D2" t="s">
-        <v>590</v>
-      </c>
-      <c r="E2" t="s">
-        <v>593</v>
-      </c>
-      <c r="F2" t="s">
-        <v>555</v>
+        <v>591</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H2" t="s">
-        <v>595</v>
+        <v>564</v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
+        <v>examples_images_id SERIAL NOT NULL,</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2837,23 +2843,23 @@
         <v>569</v>
       </c>
       <c r="B3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C3" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
         <v>591</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="H3" t="str">
         <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
-        <v>examples_images_id SERIAL NOT NULL,</v>
+        <v>stg_examples_id INTEGER NOT NULL,</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2861,10 +2867,10 @@
         <v>569</v>
       </c>
       <c r="B4" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C4" t="s">
-        <v>556</v>
+        <v>188</v>
       </c>
       <c r="D4" t="s">
         <v>591</v>
@@ -2873,11 +2879,11 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H4" t="str">
         <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
-        <v>stg_examples_id INTEGER NOT NULL,</v>
+        <v>image_type VARCHAR NOT NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2885,7 +2891,7 @@
         <v>569</v>
       </c>
       <c r="B5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C5" t="s">
         <v>188</v>
@@ -2897,11 +2903,11 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="H5" t="str">
         <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
-        <v>image_type VARCHAR NOT NULL,</v>
+        <v>link VARCHAR NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2909,48 +2915,24 @@
         <v>569</v>
       </c>
       <c r="B6" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>563</v>
       </c>
       <c r="D6" t="s">
         <v>591</v>
       </c>
+      <c r="E6" t="s">
+        <v>594</v>
+      </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="H6" t="str">
-        <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
-        <v>link VARCHAR NOT NULL,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>569</v>
-      </c>
-      <c r="B7" t="s">
-        <v>562</v>
-      </c>
-      <c r="C7" t="s">
-        <v>563</v>
-      </c>
-      <c r="D7" t="s">
-        <v>591</v>
-      </c>
-      <c r="E7" t="s">
-        <v>594</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>564</v>
-      </c>
-      <c r="H7" t="str">
         <f>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</f>
         <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
       </c>
@@ -2967,21 +2949,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="3" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>551</v>
       </c>
@@ -2992,13 +2975,22 @@
         <v>186</v>
       </c>
       <c r="D1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" t="s">
         <v>555</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>577</v>
       </c>
@@ -3008,14 +3000,21 @@
       <c r="C2" t="s">
         <v>556</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>uri_page_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>577</v>
       </c>
@@ -3025,14 +3024,21 @@
       <c r="C3" t="s">
         <v>556</v>
       </c>
-      <c r="D3" t="b">
+      <c r="D3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>coin_id INTEGER NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>577</v>
       </c>
@@ -3042,14 +3048,21 @@
       <c r="C4" t="s">
         <v>556</v>
       </c>
-      <c r="D4" t="b">
+      <c r="D4" t="s">
+        <v>592</v>
+      </c>
+      <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>examples_pagination_id INTEGER NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>577</v>
       </c>
@@ -3059,14 +3072,21 @@
       <c r="C5" t="s">
         <v>556</v>
       </c>
-      <c r="D5" t="b">
+      <c r="D5" t="s">
+        <v>592</v>
+      </c>
+      <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>examples_total_pagination INTEGER NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>577</v>
       </c>
@@ -3076,14 +3096,21 @@
       <c r="C6" t="s">
         <v>556</v>
       </c>
-      <c r="D6" t="b">
+      <c r="D6" t="s">
+        <v>592</v>
+      </c>
+      <c r="F6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>examples_start_id INTEGER NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>577</v>
       </c>
@@ -3093,14 +3120,21 @@
       <c r="C7" t="s">
         <v>556</v>
       </c>
-      <c r="D7" t="b">
+      <c r="D7" t="s">
+        <v>592</v>
+      </c>
+      <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>examples_end_id INTEGER NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>577</v>
       </c>
@@ -3110,14 +3144,21 @@
       <c r="C8" t="s">
         <v>556</v>
       </c>
-      <c r="D8" t="b">
+      <c r="D8" t="s">
+        <v>592</v>
+      </c>
+      <c r="F8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>examples_max_id INTEGER NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>577</v>
       </c>
@@ -3127,14 +3168,21 @@
       <c r="C9" t="s">
         <v>188</v>
       </c>
-      <c r="D9" t="b">
+      <c r="D9" t="s">
+        <v>591</v>
+      </c>
+      <c r="F9" t="b">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H9" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>uri_link VARCHAR NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>577</v>
       </c>
@@ -3144,15 +3192,27 @@
       <c r="C10" t="s">
         <v>563</v>
       </c>
-      <c r="D10" t="b">
+      <c r="D10" t="s">
+        <v>591</v>
+      </c>
+      <c r="E10" t="s">
+        <v>594</v>
+      </c>
+      <c r="F10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>564</v>
       </c>
+      <c r="H10" t="str">
+        <f>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</f>
+        <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Update schemas on spreadsheets
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C857C3-FB7A-154C-87A5-2280A7BFC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33A8AF4-4FE2-694B-9C60-2BAF69EC7874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23920" yWindow="920" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="10" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23380" yWindow="540" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="603">
   <si>
     <t>collection</t>
   </si>
@@ -1947,6 +1947,15 @@
   </si>
   <si>
     <t>coin_weight</t>
+  </si>
+  <si>
+    <t>coin_name</t>
+  </si>
+  <si>
+    <t>has_fields_section</t>
+  </si>
+  <si>
+    <t>has_links_section</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1993,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1994,6 +2003,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFD78"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2022,7 +2037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2054,12 +2069,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2203,7 +2229,7 @@
     <tableColumn id="7" xr3:uid="{13B45FA7-B2BD-6744-81EC-7C7DA0F79F53}" name="default"/>
     <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
-    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2212,22 +2238,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}" name="Table5" displayName="Table5" ref="A1:I124" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A1:I124" xr:uid="{90515A87-CE83-5343-ADCB-FFD7A2FC5A42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{E2A2C69C-F4CD-FA43-A6B3-9DAA3AA1D9DA}" name="field_name" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{F89AE2AE-3995-C44F-A7AD-0F78964959F5}" name="general_field_name" dataDxfId="24">
       <calculatedColumnFormula>IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],1)))=TRUE, Table5[[#This Row],[field_name]], IF(ISERR(VALUE(RIGHT(Table5[[#This Row],[field_name]],2)))=TRUE, LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-1), LEFT(Table5[[#This Row],[field_name]], LEN(Table5[[#This Row],[field_name]])-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{0045F9B6-683C-AB4F-B547-FF9F35C6A3D6}" name="general_field_name_count" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(Table5[general_field_name], "="&amp;Table5[[#This Row],[general_field_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{173FD3D7-1FE1-BF4E-B7A7-C30A1C5E3D06}" name="transformation" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{584F8E33-BCEF-EA4C-A64B-34767D4E4824}" name="target_field_name" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{FBA044CD-3E8A-4043-AFA4-B674DE31001D}" name="target_field_type" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{5F109D57-9F02-8045-99AD-1CE38D2A051F}" name="coin_id_example" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{B27689A2-559D-CA4F-BD31-5526793FB68E}" name="example_value" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{6A804817-99E9-7744-ACA4-8F20BD7ABBE2}" name="example_uri" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2263,7 +2289,7 @@
   <autoFilter ref="A1:D56" xr:uid="{A0148D89-BF01-B94F-9B30-7515455D042E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{264B7C6E-4682-D443-93C0-45C8CDD842E1}" name="collection_name" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{17CCFCF0-CDE8-C942-BE41-D823A6D6A4CD}" name="max_length" totalsRowFunction="max" dataDxfId="16">
       <calculatedColumnFormula>LEN(CollectionsTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{78452DC5-1520-C343-AE70-0A729CB15809}" name="first_example_coin"/>
@@ -2274,31 +2300,31 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="15">
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="10">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:H37" totalsRowShown="0">
-  <autoFilter ref="A1:H37" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}" name="Table7" displayName="Table7" ref="A1:H38" totalsRowShown="0">
+  <autoFilter ref="A1:H38" xr:uid="{838C36CA-F85B-1146-AAEF-9D6864969FB4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6117DFE2-6236-1848-B40F-CB876F761A46}" name="table_name"/>
     <tableColumn id="2" xr3:uid="{828DEEED-8A27-DA45-942B-678BAE403B37}" name="field_name"/>
@@ -2307,7 +2333,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2316,17 +2342,17 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}" name="Table8" displayName="Table8" ref="A1:H12" totalsRowShown="0">
-  <autoFilter ref="A1:H12" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}" name="Table8" displayName="Table8" ref="A1:H15" totalsRowShown="0">
+  <autoFilter ref="A1:H15" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F7340B1E-35F9-5648-82E2-8460E781DD0B}" name="table_name"/>
-    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name"/>
+    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{4CC7DC79-F70D-2A4E-B93F-ACBBB84B801F}" name="data_type"/>
     <tableColumn id="6" xr3:uid="{CCD0FDAB-579C-0A4E-B073-6A0596D1E8DB}" name="is_null"/>
     <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
-    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2345,7 +2371,7 @@
     <tableColumn id="7" xr3:uid="{C3D521DA-8B4C-DE40-B393-07D69A13443B}" name="default"/>
     <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
-    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2775,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA434118-7673-B544-AD54-0753231E47ED}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2818,7 +2844,7 @@
       <c r="A2" t="s">
         <v>569</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>570</v>
       </c>
       <c r="C2" t="s">
@@ -2842,7 +2868,7 @@
       <c r="A3" t="s">
         <v>569</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>571</v>
       </c>
       <c r="C3" t="s">
@@ -2914,7 +2940,7 @@
       <c r="A6" t="s">
         <v>569</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>562</v>
       </c>
       <c r="C6" t="s">
@@ -2951,7 +2977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6401C34-37B7-4248-926A-F31126A9BB24}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3224,10 +3250,10 @@
   <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:F124"/>
+      <selection pane="bottomRight" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6865,7 +6891,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7100,6 +7126,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -7112,7 +7139,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7270,6 +7297,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -10464,10 +10492,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2A06A9-74E3-D943-A3A2-B73F58CDB53A}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10536,10 +10564,10 @@
         <v>553</v>
       </c>
       <c r="B3" t="s">
-        <v>587</v>
+        <v>600</v>
       </c>
       <c r="C3" t="s">
-        <v>560</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
         <v>591</v>
@@ -10548,11 +10576,11 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>588</v>
+        <v>561</v>
       </c>
       <c r="H3" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>has_typological BOOLEAN NOT NULL,</v>
+        <v>coin_name VARCHAR NOT NULL,</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -10560,7 +10588,7 @@
         <v>553</v>
       </c>
       <c r="B4" t="s">
-        <v>558</v>
+        <v>587</v>
       </c>
       <c r="C4" t="s">
         <v>560</v>
@@ -10572,11 +10600,11 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>557</v>
+        <v>588</v>
       </c>
       <c r="H4" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>has_examples BOOLEAN NOT NULL,</v>
+        <v>has_typological BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -10584,7 +10612,7 @@
         <v>553</v>
       </c>
       <c r="B5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C5" t="s">
         <v>560</v>
@@ -10600,7 +10628,7 @@
       </c>
       <c r="H5" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>has_examples_pagination BOOLEAN NOT NULL,</v>
+        <v>has_examples BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -10608,7 +10636,7 @@
         <v>553</v>
       </c>
       <c r="B6" t="s">
-        <v>589</v>
+        <v>559</v>
       </c>
       <c r="C6" t="s">
         <v>560</v>
@@ -10620,11 +10648,11 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H6" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>has_analysis BOOLEAN NOT NULL,</v>
+        <v>has_examples_pagination BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -10632,13 +10660,13 @@
         <v>553</v>
       </c>
       <c r="B7" t="s">
-        <v>537</v>
+        <v>589</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>560</v>
       </c>
       <c r="D7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -10648,7 +10676,7 @@
       </c>
       <c r="H7" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>coin_date_range VARCHAR NULL,</v>
+        <v>has_analysis BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -10656,10 +10684,10 @@
         <v>553</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C8" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
         <v>592</v>
@@ -10672,7 +10700,7 @@
       </c>
       <c r="H8" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>denomination VARCHAR[] NULL,</v>
+        <v>coin_date_range VARCHAR NULL,</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -10680,10 +10708,10 @@
         <v>553</v>
       </c>
       <c r="B9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D9" t="s">
         <v>592</v>
@@ -10696,7 +10724,7 @@
       </c>
       <c r="H9" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>manufacture VARCHAR NULL,</v>
+        <v>denomination VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -10704,10 +10732,10 @@
         <v>553</v>
       </c>
       <c r="B10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C10" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
         <v>592</v>
@@ -10720,7 +10748,7 @@
       </c>
       <c r="H10" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>material VARCHAR[] NULL,</v>
+        <v>manufacture VARCHAR NULL,</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -10728,7 +10756,7 @@
         <v>553</v>
       </c>
       <c r="B11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C11" t="s">
         <v>539</v>
@@ -10744,7 +10772,7 @@
       </c>
       <c r="H11" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>object_type VARCHAR[] NULL,</v>
+        <v>material VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -10752,7 +10780,7 @@
         <v>553</v>
       </c>
       <c r="B12" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C12" t="s">
         <v>539</v>
@@ -10768,7 +10796,7 @@
       </c>
       <c r="H12" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>authority_name VARCHAR[] NULL,</v>
+        <v>object_type VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -10776,7 +10804,7 @@
         <v>553</v>
       </c>
       <c r="B13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C13" t="s">
         <v>539</v>
@@ -10792,7 +10820,7 @@
       </c>
       <c r="H13" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>issuer_name VARCHAR[] NULL,</v>
+        <v>authority_name VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -10800,10 +10828,10 @@
         <v>553</v>
       </c>
       <c r="B14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D14" t="s">
         <v>592</v>
@@ -10816,7 +10844,7 @@
       </c>
       <c r="H14" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>stated_authority_name VARCHAR NULL,</v>
+        <v>issuer_name VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -10824,10 +10852,10 @@
         <v>553</v>
       </c>
       <c r="B15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C15" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D15" t="s">
         <v>592</v>
@@ -10840,7 +10868,7 @@
       </c>
       <c r="H15" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>mint VARCHAR[] NULL,</v>
+        <v>stated_authority_name VARCHAR NULL,</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -10848,7 +10876,7 @@
         <v>553</v>
       </c>
       <c r="B16" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C16" t="s">
         <v>539</v>
@@ -10864,7 +10892,7 @@
       </c>
       <c r="H16" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>region VARCHAR[] NULL,</v>
+        <v>mint VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -10872,10 +10900,10 @@
         <v>553</v>
       </c>
       <c r="B17" t="s">
-        <v>297</v>
+        <v>549</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D17" t="s">
         <v>592</v>
@@ -10888,7 +10916,7 @@
       </c>
       <c r="H17" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_controlmark VARCHAR NULL,</v>
+        <v>region VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -10896,10 +10924,10 @@
         <v>553</v>
       </c>
       <c r="B18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C18" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
         <v>592</v>
@@ -10912,7 +10940,7 @@
       </c>
       <c r="H18" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_deity VARCHAR[] NULL,</v>
+        <v>obverse_controlmark VARCHAR NULL,</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -10920,10 +10948,10 @@
         <v>553</v>
       </c>
       <c r="B19" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C19" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D19" t="s">
         <v>592</v>
@@ -10936,7 +10964,7 @@
       </c>
       <c r="H19" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_legend TEXT NULL,</v>
+        <v>obverse_deity VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -10944,10 +10972,10 @@
         <v>553</v>
       </c>
       <c r="B20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C20" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="D20" t="s">
         <v>592</v>
@@ -10960,7 +10988,7 @@
       </c>
       <c r="H20" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_portrait VARCHAR[] NULL,</v>
+        <v>obverse_legend TEXT NULL,</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -10968,7 +10996,7 @@
         <v>553</v>
       </c>
       <c r="B21" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C21" t="s">
         <v>539</v>
@@ -10984,7 +11012,7 @@
       </c>
       <c r="H21" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_state VARCHAR[] NULL,</v>
+        <v>obverse_portrait VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -10992,10 +11020,10 @@
         <v>553</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C22" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D22" t="s">
         <v>592</v>
@@ -11008,7 +11036,7 @@
       </c>
       <c r="H22" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>obverse_type TEXT NULL,</v>
+        <v>obverse_state VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -11016,10 +11044,10 @@
         <v>553</v>
       </c>
       <c r="B23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>550</v>
       </c>
       <c r="D23" t="s">
         <v>592</v>
@@ -11032,7 +11060,7 @@
       </c>
       <c r="H23" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_control_marks VARCHAR NULL,</v>
+        <v>obverse_type TEXT NULL,</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -11040,10 +11068,10 @@
         <v>553</v>
       </c>
       <c r="B24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C24" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
         <v>592</v>
@@ -11056,7 +11084,7 @@
       </c>
       <c r="H24" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_deity VARCHAR[] NULL,</v>
+        <v>reverse_control_marks VARCHAR NULL,</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -11064,10 +11092,10 @@
         <v>553</v>
       </c>
       <c r="B25" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C25" t="s">
-        <v>188</v>
+        <v>539</v>
       </c>
       <c r="D25" t="s">
         <v>592</v>
@@ -11080,7 +11108,7 @@
       </c>
       <c r="H25" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_dynasty VARCHAR NULL,</v>
+        <v>reverse_deity VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -11088,10 +11116,10 @@
         <v>553</v>
       </c>
       <c r="B26" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C26" t="s">
-        <v>550</v>
+        <v>188</v>
       </c>
       <c r="D26" t="s">
         <v>592</v>
@@ -11104,7 +11132,7 @@
       </c>
       <c r="H26" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_legend TEXT NULL,</v>
+        <v>reverse_dynasty VARCHAR NULL,</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -11112,10 +11140,10 @@
         <v>553</v>
       </c>
       <c r="B27" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>550</v>
       </c>
       <c r="D27" t="s">
         <v>592</v>
@@ -11128,7 +11156,7 @@
       </c>
       <c r="H27" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_mintmark VARCHAR NULL,</v>
+        <v>reverse_legend TEXT NULL,</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -11136,7 +11164,7 @@
         <v>553</v>
       </c>
       <c r="B28" t="s">
-        <v>434</v>
+        <v>336</v>
       </c>
       <c r="C28" t="s">
         <v>188</v>
@@ -11152,7 +11180,7 @@
       </c>
       <c r="H28" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_monogram VARCHAR NULL,</v>
+        <v>reverse_mintmark VARCHAR NULL,</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -11160,10 +11188,10 @@
         <v>553</v>
       </c>
       <c r="B29" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C29" t="s">
-        <v>539</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
         <v>592</v>
@@ -11176,7 +11204,7 @@
       </c>
       <c r="H29" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_officinamark VARCHAR[] NULL,</v>
+        <v>reverse_monogram VARCHAR NULL,</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -11184,7 +11212,7 @@
         <v>553</v>
       </c>
       <c r="B30" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="C30" t="s">
         <v>539</v>
@@ -11200,7 +11228,7 @@
       </c>
       <c r="H30" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_portrait VARCHAR[] NULL,</v>
+        <v>reverse_officinamark VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -11208,7 +11236,7 @@
         <v>553</v>
       </c>
       <c r="B31" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="C31" t="s">
         <v>539</v>
@@ -11224,7 +11252,7 @@
       </c>
       <c r="H31" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_state VARCHAR[] NULL,</v>
+        <v>reverse_portrait VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -11232,7 +11260,7 @@
         <v>553</v>
       </c>
       <c r="B32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C32" t="s">
         <v>539</v>
@@ -11248,7 +11276,7 @@
       </c>
       <c r="H32" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_symbol VARCHAR[] NULL,</v>
+        <v>reverse_state VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -11256,10 +11284,10 @@
         <v>553</v>
       </c>
       <c r="B33" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C33" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D33" t="s">
         <v>592</v>
@@ -11272,7 +11300,7 @@
       </c>
       <c r="H33" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>reverse_type TEXT NULL,</v>
+        <v>reverse_symbol VARCHAR[] NULL,</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -11280,10 +11308,10 @@
         <v>553</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>478</v>
       </c>
       <c r="C34" t="s">
-        <v>187</v>
+        <v>550</v>
       </c>
       <c r="D34" t="s">
         <v>592</v>
@@ -11296,7 +11324,7 @@
       </c>
       <c r="H34" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>average_axis NUMERIC NULL,</v>
+        <v>reverse_type TEXT NULL,</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -11304,7 +11332,7 @@
         <v>553</v>
       </c>
       <c r="B35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C35" t="s">
         <v>187</v>
@@ -11320,7 +11348,7 @@
       </c>
       <c r="H35" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>average_diameter NUMERIC NULL,</v>
+        <v>average_axis NUMERIC NULL,</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -11328,7 +11356,7 @@
         <v>553</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" t="s">
         <v>187</v>
@@ -11344,7 +11372,7 @@
       </c>
       <c r="H36" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
-        <v>average_weight NUMERIC NULL,</v>
+        <v>average_diameter NUMERIC NULL,</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -11352,24 +11380,48 @@
         <v>553</v>
       </c>
       <c r="B37" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" t="s">
+        <v>592</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>561</v>
+      </c>
+      <c r="H37" t="str">
+        <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
+        <v>average_weight NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>553</v>
+      </c>
+      <c r="B38" t="s">
         <v>562</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>563</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>591</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>594</v>
       </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
         <v>564</v>
       </c>
-      <c r="H37" t="str">
+      <c r="H38" t="str">
         <f>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</f>
         <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
       </c>
@@ -11385,10 +11437,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11430,7 +11482,7 @@
       <c r="A2" t="s">
         <v>565</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="14" t="s">
         <v>566</v>
       </c>
       <c r="C2" t="s">
@@ -11454,7 +11506,7 @@
       <c r="A3" t="s">
         <v>565</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>554</v>
       </c>
       <c r="C3" t="s">
@@ -11478,7 +11530,7 @@
       <c r="A4" t="s">
         <v>565</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>596</v>
       </c>
       <c r="C4" t="s">
@@ -11502,14 +11554,14 @@
       <c r="A5" t="s">
         <v>565</v>
       </c>
-      <c r="B5" t="s">
-        <v>597</v>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -11519,21 +11571,21 @@
       </c>
       <c r="H5" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>coin_axis NUMERIC NULL,</v>
+        <v>example_name VARCHAR NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>565</v>
       </c>
-      <c r="B6" t="s">
-        <v>170</v>
+      <c r="B6" s="14" t="s">
+        <v>601</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -11541,23 +11593,23 @@
       <c r="G6" t="s">
         <v>561</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H6" s="15" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>collection_name VARCHAR NULL,</v>
+        <v>has_fields_section BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>565</v>
       </c>
-      <c r="B7" t="s">
-        <v>598</v>
+      <c r="B7" s="14" t="s">
+        <v>602</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>560</v>
       </c>
       <c r="D7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -11565,20 +11617,20 @@
       <c r="G7" t="s">
         <v>561</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7" s="15" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>coin_diameter NUMERIC NULL,</v>
+        <v>has_links_section BOOLEAN NOT NULL,</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>565</v>
       </c>
-      <c r="B8" t="s">
-        <v>175</v>
+      <c r="B8" s="14" t="s">
+        <v>597</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
         <v>592</v>
@@ -11591,15 +11643,15 @@
       </c>
       <c r="H8" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>findspot VARCHAR NULL,</v>
+        <v>coin_axis NUMERIC NULL,</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>565</v>
       </c>
-      <c r="B9" t="s">
-        <v>177</v>
+      <c r="B9" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="C9" t="s">
         <v>188</v>
@@ -11615,18 +11667,18 @@
       </c>
       <c r="H9" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>hoard VARCHAR NULL,</v>
+        <v>collection_name VARCHAR NULL,</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>565</v>
       </c>
-      <c r="B10" t="s">
-        <v>179</v>
+      <c r="B10" s="14" t="s">
+        <v>598</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
         <v>592</v>
@@ -11639,18 +11691,18 @@
       </c>
       <c r="H10" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>identifier VARCHAR NULL,</v>
+        <v>coin_diameter NUMERIC NULL,</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>565</v>
       </c>
-      <c r="B11" t="s">
-        <v>599</v>
+      <c r="B11" s="14" t="s">
+        <v>175</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
         <v>592</v>
@@ -11663,32 +11715,104 @@
       </c>
       <c r="H11" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
-        <v>coin_weight NUMERIC NULL,</v>
+        <v>findspot VARCHAR NULL,</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>565</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" t="s">
+        <v>592</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>561</v>
+      </c>
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>hoard VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>565</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>592</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>561</v>
+      </c>
+      <c r="H13" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>identifier VARCHAR NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>565</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" t="s">
+        <v>592</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>561</v>
+      </c>
+      <c r="H14" t="str">
+        <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
+        <v>coin_weight NUMERIC NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>565</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>562</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>563</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>591</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>594</v>
       </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
         <v>564</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H15" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
         <v>ts TIMESTAMP NOT NULL DEFAULT CURRENT_TIMESTAMP,</v>
       </c>

</xml_diff>

<commit_message>
Update schemas in spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33A8AF4-4FE2-694B-9C60-2BAF69EC7874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DDE93-4199-3342-BD8F-41F884CBCE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23380" yWindow="540" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="8" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-23380" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="5" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -2037,7 +2037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2070,8 +2070,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2079,27 +2077,16 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2120,13 +2107,24 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2229,7 +2227,7 @@
     <tableColumn id="7" xr3:uid="{13B45FA7-B2BD-6744-81EC-7C7DA0F79F53}" name="default"/>
     <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
-    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2301,22 +2299,28 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}" name="CollectionsAndIIIFTable" displayName="CollectionsAndIIIFTable" ref="A1:J67" totalsRowCount="1" headerRowDxfId="15">
-  <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}"/>
+  <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="14">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="13">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2333,7 +2337,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2346,13 +2350,13 @@
   <autoFilter ref="A1:H15" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F7340B1E-35F9-5648-82E2-8460E781DD0B}" name="table_name"/>
-    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{4CC7DC79-F70D-2A4E-B93F-ACBBB84B801F}" name="data_type"/>
     <tableColumn id="6" xr3:uid="{CCD0FDAB-579C-0A4E-B073-6A0596D1E8DB}" name="is_null"/>
     <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
-    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2371,7 +2375,7 @@
     <tableColumn id="7" xr3:uid="{C3D521DA-8B4C-DE40-B393-07D69A13443B}" name="default"/>
     <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
-    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="9">
       <calculatedColumnFormula>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2802,7 +2806,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7308,7 +7312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0256B6-CC9F-DA43-B2FC-ADA39BBB9055}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -8188,18 +8192,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA16E2E-DB77-5147-BA8D-767530543406}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9" style="4" customWidth="1"/>
-    <col min="3" max="3" width="4.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="0.5" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="30.6640625" style="4" customWidth="1"/>
@@ -8298,7 +8302,7 @@
       <c r="I3"/>
       <c r="J3"/>
     </row>
-    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -8332,7 +8336,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -8394,7 +8398,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -8484,7 +8488,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -8546,7 +8550,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -9028,7 +9032,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>73</v>
       </c>
@@ -9090,7 +9094,7 @@
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
@@ -9380,7 +9384,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>105</v>
       </c>
@@ -9583,7 +9587,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>123</v>
       </c>
@@ -9701,7 +9705,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -9735,7 +9739,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>136</v>
       </c>
@@ -9994,7 +9998,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>158</v>
       </c>
@@ -10028,7 +10032,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>161</v>
       </c>
@@ -10090,7 +10094,7 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -10124,7 +10128,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>164</v>
       </c>
@@ -10164,7 +10168,7 @@
       </c>
       <c r="G67" s="4">
         <f>SUBTOTAL(103,CollectionsAndIIIFTable[example_page_link])</f>
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -10193,6 +10197,7 @@
     <hyperlink ref="I66" r:id="rId21" xr:uid="{223800AA-A6C1-2D42-8154-61CFBA8142F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId22"/>
   </tableParts>
@@ -10204,7 +10209,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10487,6 +10492,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -11439,7 +11445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D35B23E-547B-A747-9CE7-23FE29E4880F}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -11482,7 +11488,7 @@
       <c r="A2" t="s">
         <v>565</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>566</v>
       </c>
       <c r="C2" t="s">
@@ -11506,7 +11512,7 @@
       <c r="A3" t="s">
         <v>565</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" t="s">
         <v>554</v>
       </c>
       <c r="C3" t="s">
@@ -11530,7 +11536,7 @@
       <c r="A4" t="s">
         <v>565</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" t="s">
         <v>596</v>
       </c>
       <c r="C4" t="s">
@@ -11554,7 +11560,7 @@
       <c r="A5" t="s">
         <v>565</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -11578,7 +11584,7 @@
       <c r="A6" t="s">
         <v>565</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" t="s">
         <v>601</v>
       </c>
       <c r="C6" t="s">
@@ -11593,7 +11599,7 @@
       <c r="G6" t="s">
         <v>561</v>
       </c>
-      <c r="H6" s="15" t="str">
+      <c r="H6" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
         <v>has_fields_section BOOLEAN NOT NULL,</v>
       </c>
@@ -11602,7 +11608,7 @@
       <c r="A7" t="s">
         <v>565</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" t="s">
         <v>602</v>
       </c>
       <c r="C7" t="s">
@@ -11617,7 +11623,7 @@
       <c r="G7" t="s">
         <v>561</v>
       </c>
-      <c r="H7" s="15" t="str">
+      <c r="H7" t="str">
         <f>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</f>
         <v>has_links_section BOOLEAN NOT NULL,</v>
       </c>
@@ -11626,7 +11632,7 @@
       <c r="A8" t="s">
         <v>565</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" t="s">
         <v>597</v>
       </c>
       <c r="C8" t="s">
@@ -11650,7 +11656,7 @@
       <c r="A9" t="s">
         <v>565</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" t="s">
         <v>170</v>
       </c>
       <c r="C9" t="s">
@@ -11674,7 +11680,7 @@
       <c r="A10" t="s">
         <v>565</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" t="s">
         <v>598</v>
       </c>
       <c r="C10" t="s">
@@ -11698,7 +11704,7 @@
       <c r="A11" t="s">
         <v>565</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" t="s">
         <v>175</v>
       </c>
       <c r="C11" t="s">
@@ -11722,7 +11728,7 @@
       <c r="A12" t="s">
         <v>565</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" t="s">
         <v>177</v>
       </c>
       <c r="C12" t="s">
@@ -11746,7 +11752,7 @@
       <c r="A13" t="s">
         <v>565</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" t="s">
         <v>179</v>
       </c>
       <c r="C13" t="s">
@@ -11770,7 +11776,7 @@
       <c r="A14" t="s">
         <v>565</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" t="s">
         <v>599</v>
       </c>
       <c r="C14" t="s">
@@ -11794,7 +11800,7 @@
       <c r="A15" t="s">
         <v>565</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" t="s">
         <v>562</v>
       </c>
       <c r="C15" t="s">

</xml_diff>

<commit_message>
Update schema in spreadsheet
</commit_message>
<xml_diff>
--- a/data/uri_field_and_value_review.xlsx
+++ b/data/uri_field_and_value_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamal/Workspace/ocre-database-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DDE93-4199-3342-BD8F-41F884CBCE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2502398A-D782-444B-8D27-33828D110D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23380" yWindow="500" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="5" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
+    <workbookView xWindow="-26460" yWindow="3480" windowWidth="23040" windowHeight="13900" firstSheet="4" activeTab="5" xr2:uid="{BC58D712-1FB2-5F43-B3AE-5DF2BFDC2690}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalysisFields" sheetId="1" r:id="rId1"/>
@@ -2077,16 +2077,27 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2107,24 +2118,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2227,7 +2227,7 @@
     <tableColumn id="7" xr3:uid="{13B45FA7-B2BD-6744-81EC-7C7DA0F79F53}" name="default"/>
     <tableColumn id="4" xr3:uid="{A6FF6C8C-94E8-D24D-B06A-BDF4CB4A8D7B}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{B747C877-A78C-B146-BB89-189A5186D2A2}" name="source"/>
-    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{1958E9D1-3F5A-144C-BFD4-44A03427DEFD}" name="sql_code" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(Table9[[#This Row],[field_name]], " ", Table9[[#This Row],[data_type]], " ", Table9[[#This Row],[is_null]], IF(LEN(Table9[[#This Row],[default]])=0,""," DEFAULT "&amp;Table9[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2302,25 +2302,25 @@
   <autoFilter ref="A1:J66" xr:uid="{D4CAB645-43A3-F94D-A136-B4FC47F37204}">
     <filterColumn colId="1">
       <filters>
-        <filter val="FALSE"/>
+        <filter val="TRUE"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{19263661-A7BA-A745-8CCD-3503DF7E2A7F}" name="collection_name" totalsRowLabel="Total" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1AF04E96-5527-3942-BCD9-80CA0B112B98}" name="uses_iiif" totalsRowDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C8B5C049-69A4-5E4A-8E00-A84CEB5929C7}" name="num_links" totalsRowDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{EF50508F-F805-0A4E-9E02-FF082912F63D}" name="collection_count" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(CollectionsAndIIIFTable[collection_name], "="&amp;CollectionsAndIIIFTable[[#This Row],[collection_name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{FD8825E0-E9B1-284E-BCB6-FBADE703726B}" name="Column1" dataDxfId="10">
       <calculatedColumnFormula>IF(AND(CollectionsAndIIIFTable[[#This Row],[num_links]]=0,CollectionsAndIIIFTable[[#This Row],[collection_count]]&gt;1)=TRUE, "hide", "do not hide")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4FC16E6A-1BBC-764D-877A-93FEBC2C3087}" name="example_name" totalsRowDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{5CFBDB0A-1F4C-B146-920B-E045FA650F2C}" name="example_page_link" totalsRowFunction="count" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EF6735BE-833E-B248-B9B3-1F0F3A93E74D}" name="link_to_image" totalsRowDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{6112D607-B997-6742-B7AD-8C900694CF2E}" name="link_from_scraping" totalsRowDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{C00533FC-4213-CA4A-A903-7EC6B6D1937A}" name="Notes" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2337,7 +2337,7 @@
     <tableColumn id="7" xr3:uid="{5B71E517-87C5-6845-AF72-8F8EDB6CF2DF}" name="default"/>
     <tableColumn id="5" xr3:uid="{9496267A-32A2-164A-AC1F-2A663EB3D3CA}" name="primary_key"/>
     <tableColumn id="4" xr3:uid="{E3AD2819-1B8A-A846-A599-4171D76077EF}" name="source"/>
-    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="12">
+    <tableColumn id="8" xr3:uid="{C908F267-5260-8344-9A3B-B8E80D8B8D8C}" name="sql_code" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT(Table7[[#This Row],[field_name]], " ", Table7[[#This Row],[data_type]], " ", Table7[[#This Row],[is_null]], IF(LEN(Table7[[#This Row],[default]])=0,""," DEFAULT "&amp;Table7[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2350,13 +2350,13 @@
   <autoFilter ref="A1:H15" xr:uid="{A83EC273-4D5F-5144-969C-1A5DD79AC914}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F7340B1E-35F9-5648-82E2-8460E781DD0B}" name="table_name"/>
-    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{46C5BF6A-FB8B-E44E-B393-884C14343218}" name="field_name" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{4CC7DC79-F70D-2A4E-B93F-ACBBB84B801F}" name="data_type"/>
     <tableColumn id="6" xr3:uid="{CCD0FDAB-579C-0A4E-B073-6A0596D1E8DB}" name="is_null"/>
     <tableColumn id="7" xr3:uid="{F98C71D5-533C-044D-ACD4-9BAAB7DC5757}" name="default"/>
     <tableColumn id="4" xr3:uid="{5A32623C-0F48-3340-8BF2-A80B158C7972}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{E793E59B-2D60-3046-937B-B6880B0896B6}" name="source"/>
-    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{7FEFCCE3-E09F-0B43-B86F-E86D6C5BC6BD}" name="sql_code" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[field_name]], " ", Table8[[#This Row],[data_type]], " ", Table8[[#This Row],[is_null]], IF(LEN(Table8[[#This Row],[default]])=0,""," DEFAULT "&amp;Table8[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2375,7 +2375,7 @@
     <tableColumn id="7" xr3:uid="{C3D521DA-8B4C-DE40-B393-07D69A13443B}" name="default"/>
     <tableColumn id="4" xr3:uid="{E38B7632-4CC6-6D40-B3B4-59FD1D96C855}" name="primary_key"/>
     <tableColumn id="5" xr3:uid="{7399CB2D-1A2A-C749-8E13-4EC162C3677F}" name="source"/>
-    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="9">
+    <tableColumn id="8" xr3:uid="{2C65647B-F349-D441-9A57-04E6CF10B256}" name="sql_code" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table10[[#This Row],[field_name]], " ", Table10[[#This Row],[data_type]], " ", Table10[[#This Row],[is_null]], IF(LEN(Table10[[#This Row],[default]])=0,""," DEFAULT "&amp;Table10[[#This Row],[default]]), ",")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8193,10 +8193,10 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8246,7 +8246,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -8274,7 +8274,7 @@
       <c r="I2"/>
       <c r="J2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -8302,7 +8302,7 @@
       <c r="I3"/>
       <c r="J3"/>
     </row>
-    <row r="4" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -8460,7 +8460,7 @@
       <c r="I8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="153" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -8668,7 +8668,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -8948,7 +8948,7 @@
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>67</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>73</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -9094,7 +9094,7 @@
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
@@ -9128,7 +9128,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>81</v>
       </c>
@@ -9156,7 +9156,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -9184,7 +9184,7 @@
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>84</v>
       </c>
@@ -9212,7 +9212,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>84</v>
       </c>
@@ -9240,7 +9240,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>91</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>94</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>97</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>100</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>102</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>105</v>
       </c>
@@ -9419,7 +9419,7 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>108</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>111</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>113</v>
       </c>
@@ -9503,7 +9503,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>114</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>117</v>
       </c>
@@ -9559,7 +9559,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>120</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>123</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -9649,7 +9649,7 @@
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -9677,7 +9677,7 @@
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>129</v>
       </c>
@@ -9705,7 +9705,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>136</v>
       </c>
@@ -9774,7 +9774,7 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>138</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>141</v>
       </c>
@@ -9830,7 +9830,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>144</v>
       </c>
@@ -9858,7 +9858,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
@@ -9886,7 +9886,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>147</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>149</v>
       </c>
@@ -9942,7 +9942,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>152</v>
       </c>
@@ -9970,7 +9970,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>155</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>158</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>161</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -10094,7 +10094,7 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>164</v>
       </c>
@@ -10168,7 +10168,7 @@
       </c>
       <c r="G67" s="4">
         <f>SUBTOTAL(103,CollectionsAndIIIFTable[example_page_link])</f>
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>